<commit_message>
added plots to retrain pipeline
</commit_message>
<xml_diff>
--- a/immowelt_price_guide/data/retrain_train_data.xlsx
+++ b/immowelt_price_guide/data/retrain_train_data.xlsx
@@ -496,7 +496,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
+          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -506,12 +506,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
+          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>532.19</t>
+          <t>1183.37</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -521,12 +521,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>56.02</t>
+          <t>81.32</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -536,39 +536,39 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>["Personenaufzug"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
+          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
+          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -578,12 +578,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Bestlage mit Festungsblick"</t>
+          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>610</t>
+          <t>554.99</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,54 +593,54 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>58.42</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
+          <t>["Personenaufzug", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
+          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
+          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -650,12 +650,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
+          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>950</t>
+          <t>532.19</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -665,54 +665,54 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>56.02</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1911</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
+          <t>["Personenaufzug"]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
+          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
+          <t>"https://www.immowelt.de/expose/2arkq5m"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -722,12 +722,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
+          <t>"Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>474.53</t>
+          <t>2175</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -737,54 +737,54 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>49.95</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>["Personenaufzug"]</t>
+          <t>["WANNE", "DUSCHE", "FENSTER", "Personenaufzug", "FERNE", "renoviert", "FERN", "Fu\u00dfbodenheizung", "Zentralheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Speisekammer", "Balkon", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "\u20ac 6.525,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 2175, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 450, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2625, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
+          <t>["https://ms.immowelt.org/1e8dcfd3-4788-4f09-a3c0-28d3414e57a3/5c7e81c2-8706-4ef4-8899-cfd4e8a5a029"]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>{"companyName": "Werner Fleischhacker Immobilien GmbH &amp;a; Co. KG", "address": {"city": "W\u00fcrzburg", "zipCode": "97072", "street": "Valentin-Becker-Stra\u00dfe 8"}, "salutation": "Herr", "firstName": "Werner", "lastName": "Fleischhacker", "phone": "0931/2706700"}</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City", "basicObjectPricEur": 2175, "basicLivingSpace": 150, "basicRooms": 5.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2arkq5m", "basicContactPhone": "0931/2706700"}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
+          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -794,12 +794,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1165</t>
+          <t>420</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -809,12 +809,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -824,22 +824,22 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["GAS"]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
+          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -938,12 +938,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
+          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>554.99</t>
+          <t>1165</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>58.42</t>
+          <t>77</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -963,44 +963,44 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Stellplatz"]</t>
+          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
+          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2arkq5m"</t>
+          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1010,12 +1010,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City"</t>
+          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2175</t>
+          <t>566.96</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1025,54 +1025,54 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>59.68</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>["WANNE", "DUSCHE", "FENSTER", "Personenaufzug", "FERNE", "renoviert", "FERN", "Fu\u00dfbodenheizung", "Zentralheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Speisekammer", "Balkon", "Kunststofffenster"]</t>
+          <t>["Stellplatz"]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "\u20ac 6.525,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 2175, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 450, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2625, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/1e8dcfd3-4788-4f09-a3c0-28d3414e57a3/5c7e81c2-8706-4ef4-8899-cfd4e8a5a029"]</t>
+          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>{"companyName": "Werner Fleischhacker Immobilien GmbH &amp;a; Co. KG", "address": {"city": "W\u00fcrzburg", "zipCode": "97072", "street": "Valentin-Becker-Stra\u00dfe 8"}, "salutation": "Herr", "firstName": "Werner", "lastName": "Fleischhacker", "phone": "0931/2706700"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City", "basicObjectPricEur": 2175, "basicLivingSpace": 150, "basicRooms": 5.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2arkq5m", "basicContactPhone": "0931/2706700"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
+          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1082,12 +1082,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
+          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>566.96</t>
+          <t>750</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1097,54 +1097,54 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>59.68</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1960</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>["Stellplatz"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
+          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
+          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1154,12 +1154,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
+          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1183.37</t>
+          <t>2880</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1169,54 +1169,54 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>81.32</t>
+          <t>195</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
+          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2awv45u"</t>
+          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1226,12 +1226,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
+          <t>"Bestlage mit Festungsblick"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1720</t>
+          <t>610</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1241,54 +1241,54 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>123.36</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
+          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
+          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>{"companyName": "Gute Bude Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 3c"}, "salutation": "Frau", "firstName": "Nelly", "lastName": "Gronau"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
+          <t>"https://www.immowelt.de/expose/2awv45u"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
+          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1313,54 +1313,54 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>123.36</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
+          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "Gute Bude Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 3c"}, "salutation": "Frau", "firstName": "Nelly", "lastName": "Gronau"}</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a8sz5p"</t>
+          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Gro\u00dfz\u00fcgige Zwei-Zimmer-Altbauwohnung, gut geeignet f\u00fcr einen 2-Personen-Haushalt"</t>
+          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1250</t>
+          <t>474.53</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>101.95</t>
+          <t>49.95</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1395,37 +1395,37 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1930</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "FENSTER", "Kelleranteil", "FERN", "Zentralheizung", "Einbauk\u00fcche", "Haustiere erlaubt", "Balkon"]</t>
+          <t>["Personenaufzug"]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Daimlerstra\u00dfe 17", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3750", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 1250, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 250, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1500, "Unit": "EUR"}, {"NumberValue": 35, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/cfccaab0-62e1-4e1a-9e82-41708e65355b/e5e0177f-3834-4a31-8a0e-7671d9334eaf", "https://ms.immowelt.org/9b865496-04ab-438a-8006-6cb1376458e3/1b35b733-4d27-4925-b322-cf95707fbd71", "https://ms.immowelt.org/954393bd-e85f-456d-b5ff-ed0308b4613c/b8b3587d-e932-46dd-877a-158b564af85f", "https://ms.immowelt.org/de1e5690-69cf-4922-9cfc-0a3ebb638fcd/82bf1fe1-319a-4ead-9d30-e94a41f2de6c", "https://ms.immowelt.org/c975b3d5-dce8-452b-9e87-b2012e7d8a17/94f5006d-ee5b-4cc0-892a-9c3022a48a43", "https://ms.immowelt.org/08221e0f-f8f8-4a3d-8e53-e3692122fe80/36c03dd6-03ca-436b-97af-7a11358edddc", "https://ms.immowelt.org/d17bc972-106a-4728-97e8-0ad06cfdcf97/ec216fc9-1977-4a3a-a6d0-7eb75b44c951", "https://ms.immowelt.org/cae6a3d4-4522-4d55-81ca-fb4250c0ea03/ac9fd403-a785-4ce0-836a-37253c1361e8", "https://ms.immowelt.org/3754b522-8579-4e99-98ed-88ad806ef135/0f09df4d-a2de-45e1-8691-7c114c1d1dc6", "https://ms.immowelt.org/82d0fcad-d38d-42ee-b917-0a48f0c441e1/29fda676-34cf-4710-a47c-f401e9d2dde7", "https://ms.immowelt.org/2eb6260e-1b97-4bb1-a6a8-1ffdfa9f1a91/ae1a36f9-5917-46fb-a025-7418cf42b4cc", "https://ms.immowelt.org/7e159185-d839-4d06-9cbb-a2ab09b461ae/d6f5253e-5dad-412a-9324-c447e9cd46a7", "https://ms.immowelt.org/39dbf15c-7f65-40dc-bd54-8fe566989602/f37b7c55-ee2c-48e6-906e-d0587570c550", "https://ms.immowelt.org/bdaffbe4-d997-41e5-a70f-79e4afa1eae5/17734c1e-5a32-44e3-b540-09380622a1d5", "https://ms.immowelt.org/42d9e46b-1986-460f-b622-720fd89441b8/98c7eaa9-1985-4905-b2f5-416e4431f0f6", "https://ms.immowelt.org/8a4c2605-e151-4b34-b58d-17158f1869ea/7759073e-5676-4f9e-a39d-74e152750dc6"]</t>
+          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfz\u00fcgige Zwei-Zimmer-Altbauwohnung, gut geeignet f\u00fcr einen 2-Personen-Haushalt", "basicObjectPricEur": 1250, "basicLivingSpace": 101.95, "basicRooms": 2, "basicConstructionYear": 1930, "basicCity": "W\u00fcrzburg", "basicStreet": "Daimlerstra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2a8sz5p", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
         </is>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
+          <t>"https://www.immowelt.de/expose/2asr65p"</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1514,12 +1514,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld "</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>1100</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1529,54 +1529,54 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>103</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1984</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>["GAS"]</t>
+          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "renoviert", "GAS", "Etagenheizung", "gartennutzung", "Einbauk\u00fcche", "wg_geeignet", "Balkon"]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "Street": "Unterer Kirchbergweg 37", "LocationId": 496013, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2200,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1400, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["https://ms.immowelt.org/bbd4dcbf-c64e-4c60-9789-afc66db53a3f/7fc04ce4-7f84-4ce5-8111-31fcc917306c", "https://ms.immowelt.org/315ff83e-d234-453a-ad52-c4b99bef7055/a979f182-320d-49d1-8002-bcde353d36ee", "https://ms.immowelt.org/6137c704-6a29-47ae-a5a3-88abd0a2fde0/d535204c-f43a-4229-8152-507fc644a211", "https://ms.immowelt.org/1981c2ad-23cb-41f4-825a-77d67f5fbbe7/e968ecc9-ea46-4188-a2c4-968720f069c0", "https://ms.immowelt.org/a4965ee1-de2b-4d90-8333-b793f90a7406/867d9997-6f27-48da-ade0-9096bf31cf3e", "https://ms.immowelt.org/aed0a388-445d-4f8f-9afd-4a146b35d962/3bc7e507-92a3-446a-a3f1-5799c1df7338", "https://ms.immowelt.org/f9d8ba2e-fb1a-4cdd-98ea-ba6ba4973c25/fde9d74e-bd14-4413-a148-81aad236c43f", "https://ms.immowelt.org/e0fbe89c-ecbb-41e9-9ecd-61c2762b9189/3784b2d8-f66d-4f7f-a893-cb9c7b3e982c", "https://ms.immowelt.org/16af38b3-f1c4-4d16-ba17-2685efc0dbe6/b5361690-0608-4e15-8167-e5ab29ac41e7", "https://ms.immowelt.org/fb842589-0c99-45bb-b567-5d04f811adf5/729e7fb7-c4eb-47db-936a-8a406b3efda8", "https://ms.immowelt.org/2f97e2d2-4fcd-40db-bee9-5d4161812bb0/a57df980-0cf8-4352-8cf0-5e867376c343", "https://ms.immowelt.org/79cf67c5-73a5-4097-8b85-e20df2ab786e/363fc58b-d0d5-4f6e-afda-b1d880cf8747", "https://ms.immowelt.org/d9ae7b88-e98c-4d7f-8096-8ede0076f326/e28b854c-9b59-46d6-84a5-28d2595f9ff2", "https://ms.immowelt.org/dffe6319-03a2-4071-98a5-e0f1e3954460/de63d734-7d33-492b-acbf-be5ca5b61e49", "https://ms.immowelt.org/8af5caf8-2627-4044-83b1-a3824003abcd/a9a95b7e-658f-4e56-989c-5a564997561b", "https://ms.immowelt.org/de373ea2-fa91-495b-aa05-ffa24233b025/ff4e0de7-6c79-411b-bec2-3f5b973c460c", "https://ms.immowelt.org/1db3601f-db1c-4e6f-8b1d-e2f17c88804b/e84274ae-8668-49f0-8327-447ff8511752", "https://ms.immowelt.org/6bc525ad-0769-42c3-aaff-a169a251a660/789b8d1b-633d-4989-a0e8-50949ea51d51"]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"salutation": "Herr", "firstName": "Arnold", "lastName": "Hammer", "mobile": "017683299994", "phone": "0931/60565"}</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld ", "basicObjectPricEur": 1100, "basicLivingSpace": 103, "basicRooms": 4, "basicConstructionYear": 1984, "basicCity": "W\u00fcrzburg", "basicStreet": "Unterer Kirchbergweg 37", "basicUrl": "https://www.immowelt.de/expose/2asr65p", "basicContactPhone": "0931/60565", "basicContactMobile": "017683299994"}</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2gr494f"</t>
+          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"Sch\u00f6ne 3-Zimmer Wohnung - Zell am Main  Hauptstra\u00dfe"</t>
+          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>715</t>
+          <t>950</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>82.2</t>
+          <t>79</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1611,27 +1611,27 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1900</t>
+          <t>1911</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Erdgeschoss", "GAS", "Etagenheizung", "DSL", "KUNSTSTOFF", "Sat", "Kunststofffenster"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Zell a. Main", "ZipCode": "97299", "Street": "Hauptstra\u00dfe", "LocationId": 12631, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2145", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Zell a. Main", "Link": "https://www.immowelt.de/immobilienpreise/zell-a-main/mietspiegel"}}, "DataTable": [{"NumberValue": 715, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 110, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 125, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/843e2d49-84f6-4e47-b77d-63d29ab1066e/26140dff-55d6-4812-bc01-0d9e6c646fa0", "https://ms.immowelt.org/41f37c51-8639-4424-8ee1-7a2fefff4273/d88e819f-e564-4c41-bbac-99323793838a", "https://ms.immowelt.org/662f3397-8654-43ec-b435-d79bacab8763/2fc81c17-dad7-4a2f-a9bb-77e7f8fa27dc", "https://ms.immowelt.org/f8805103-18da-476d-9f24-d04169f73813/a5cf5830-f53c-4a5e-9f1b-78a790ec5d0a", "https://ms.immowelt.org/460515a3-d738-48d8-9c73-c7c11596d325/5bbddf00-b1c1-4704-9731-886ba0a1b78a", "https://ms.immowelt.org/525c5aa4-226e-4419-bb47-0d14c2e5bd62/73fae45a-7a74-4082-b2ad-c3876b95942d", "https://ms.immowelt.org/863f8610-efdb-47dd-9cc5-249b10b8d350/fc44d80c-bb9d-44f0-afb1-dbe1a240157a"]</t>
+          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1641,14 +1641,14 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Sch\u00f6ne 3-Zimmer Wohnung - Zell am Main  Hauptstra\u00dfe", "basicObjectPricEur": 715, "basicLivingSpace": 82.2, "basicRooms": 3, "basicConstructionYear": 1900, "basicCity": "Zell a. Main", "basicStreet": "Hauptstra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2gr494f", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
+          <t>"https://www.immowelt.de/expose/2gr494f"</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1658,12 +1658,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
+          <t>"Sch\u00f6ne 3-Zimmer Wohnung - Zell am Main  Hauptstra\u00dfe"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>715</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1673,54 +1673,54 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>82.2</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1900</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>["WANNE"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Erdgeschoss", "GAS", "Etagenheizung", "DSL", "KUNSTSTOFF", "Sat", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "Zell a. Main", "ZipCode": "97299", "Street": "Hauptstra\u00dfe", "LocationId": 12631, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2145", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Zell a. Main", "Link": "https://www.immowelt.de/immobilienpreise/zell-a-main/mietspiegel"}}, "DataTable": [{"NumberValue": 715, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 110, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 125, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
+          <t>["https://ms.immowelt.org/843e2d49-84f6-4e47-b77d-63d29ab1066e/26140dff-55d6-4812-bc01-0d9e6c646fa0", "https://ms.immowelt.org/41f37c51-8639-4424-8ee1-7a2fefff4273/d88e819f-e564-4c41-bbac-99323793838a", "https://ms.immowelt.org/662f3397-8654-43ec-b435-d79bacab8763/2fc81c17-dad7-4a2f-a9bb-77e7f8fa27dc", "https://ms.immowelt.org/f8805103-18da-476d-9f24-d04169f73813/a5cf5830-f53c-4a5e-9f1b-78a790ec5d0a", "https://ms.immowelt.org/460515a3-d738-48d8-9c73-c7c11596d325/5bbddf00-b1c1-4704-9731-886ba0a1b78a", "https://ms.immowelt.org/525c5aa4-226e-4419-bb47-0d14c2e5bd62/73fae45a-7a74-4082-b2ad-c3876b95942d", "https://ms.immowelt.org/863f8610-efdb-47dd-9cc5-249b10b8d350/fc44d80c-bb9d-44f0-afb1-dbe1a240157a"]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Sch\u00f6ne 3-Zimmer Wohnung - Zell am Main  Hauptstra\u00dfe", "basicObjectPricEur": 715, "basicLivingSpace": 82.2, "basicRooms": 3, "basicConstructionYear": 1900, "basicCity": "Zell a. Main", "basicStreet": "Hauptstra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2gr494f", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
+          <t>"https://www.immowelt.de/expose/2almm5r"</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1730,12 +1730,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
+          <t>"TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2880</t>
+          <t>1700</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1745,54 +1745,54 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>153.3</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
+          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "GAS", "Zentralheizung", "teilweise m\u00f6bliert", "TEPPICH", "PARKETT", "FLIESEN", "Einbauk\u00fcche", "offene K\u00fcche", "Stellplatz", "Tiefgarage", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Gartenstra\u00dfe 9", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5.400,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 1700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 240, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten", "Comments": ["in Warmmiete enthalten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2340, "Unit": "EUR"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
+          <t>["https://ms.immowelt.org/338d1cbc-cb3f-423f-8523-42cc120d72f9/e4b563bc-671f-4dea-a726-71d7b9386009", "https://ms.immowelt.org/4da068e4-1a27-465c-b0e7-ffb77b79880b/908c43fa-aa39-4e85-97c8-98295a3c363c", "https://ms.immowelt.org/cab19ffc-0f4a-42a9-89e9-7189e9dafd92/2a5e6769-ad31-4185-a454-e8d753be9cdb", "https://ms.immowelt.org/f6511334-9f04-476c-9659-9f19a5df115f/ff04d8f5-f770-493d-9394-6ac1a456d4ef", "https://ms.immowelt.org/733f5f85-bc20-4e60-ba25-388eeb6563cf/4094751f-b73c-432d-b6b4-6d68ba45d6d9", "https://ms.immowelt.org/05e1b42e-75a4-4206-aaad-48ffa57f162d/a3aafbff-20b6-4c17-a8a1-b916eb14b8aa", "https://ms.immowelt.org/1233e75d-2ab4-4291-8b67-e87c5a4898f1/6153dd66-9325-4066-80d3-ed8642487cd8", "https://ms.immowelt.org/99f6825d-9789-4ae1-9a78-4e6acb5853a7/f727c1c7-69a0-420d-adf8-9119f5849a16", "https://ms.immowelt.org/19d94014-cd12-4f9a-81a5-8f9745f63b90/48988be8-85bb-4980-a25a-276af2606ac6", "https://ms.immowelt.org/f351ce35-7e50-4939-b806-4f6dc375cc86/84c997d9-1332-4173-9248-fb7b75a10943", "https://ms.immowelt.org/cdd250a7-47f6-4535-ac59-6ea51157c95e/bed7b410-ef26-42d6-a562-595eafba5999", "https://ms.immowelt.org/644f0235-e6ba-482b-bb26-2fea622cd4a1/6d2746f3-ea97-4996-8617-e82aeced34e0", "https://ms.immowelt.org/0174f587-e7b3-4c39-8603-c1d8465305ec/508d427a-f8c5-4d05-bd55-06ee858889be", "https://ms.immowelt.org/e3dbe0a9-b856-43a6-97a0-ca238574c6f8/f20530d2-b140-4eb5-b229-ad329853d7f3"]</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "hv Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Wilhelm-Dahl-Str. 9"}, "profilePicture": "https://filestore.immowelt.de/ProfilBilder/150_98e1685eae1346a2a90a2847489951ff.jpg", "salutation": "Herr", "firstName": "Hartwig", "lastName": "Vogel", "mobile": "0175-5994950", "phone": "0931/45466333"}</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE", "basicObjectPricEur": 1700, "basicLivingSpace": 153.3, "basicRooms": 3, "basicConstructionYear": 1998, "basicCity": "W\u00fcrzburg", "basicStreet": "Gartenstra\u00dfe 9", "basicUrl": "https://www.immowelt.de/expose/2almm5r", "basicContactPhone": "0931/45466333", "basicContactMobile": "0175-5994950"}</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2asr65p"</t>
+          <t>"https://www.immowelt.de/expose/2upu84s"</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1802,12 +1802,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld "</t>
+          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>900</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1817,54 +1817,54 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>90</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "renoviert", "GAS", "Etagenheizung", "gartennutzung", "Einbauk\u00fcche", "wg_geeignet", "Balkon"]</t>
+          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "Street": "Unterer Kirchbergweg 37", "LocationId": 496013, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2200,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1400, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/bbd4dcbf-c64e-4c60-9789-afc66db53a3f/7fc04ce4-7f84-4ce5-8111-31fcc917306c", "https://ms.immowelt.org/315ff83e-d234-453a-ad52-c4b99bef7055/a979f182-320d-49d1-8002-bcde353d36ee", "https://ms.immowelt.org/6137c704-6a29-47ae-a5a3-88abd0a2fde0/d535204c-f43a-4229-8152-507fc644a211", "https://ms.immowelt.org/1981c2ad-23cb-41f4-825a-77d67f5fbbe7/e968ecc9-ea46-4188-a2c4-968720f069c0", "https://ms.immowelt.org/a4965ee1-de2b-4d90-8333-b793f90a7406/867d9997-6f27-48da-ade0-9096bf31cf3e", "https://ms.immowelt.org/aed0a388-445d-4f8f-9afd-4a146b35d962/3bc7e507-92a3-446a-a3f1-5799c1df7338", "https://ms.immowelt.org/f9d8ba2e-fb1a-4cdd-98ea-ba6ba4973c25/fde9d74e-bd14-4413-a148-81aad236c43f", "https://ms.immowelt.org/e0fbe89c-ecbb-41e9-9ecd-61c2762b9189/3784b2d8-f66d-4f7f-a893-cb9c7b3e982c", "https://ms.immowelt.org/16af38b3-f1c4-4d16-ba17-2685efc0dbe6/b5361690-0608-4e15-8167-e5ab29ac41e7", "https://ms.immowelt.org/fb842589-0c99-45bb-b567-5d04f811adf5/729e7fb7-c4eb-47db-936a-8a406b3efda8", "https://ms.immowelt.org/2f97e2d2-4fcd-40db-bee9-5d4161812bb0/a57df980-0cf8-4352-8cf0-5e867376c343", "https://ms.immowelt.org/79cf67c5-73a5-4097-8b85-e20df2ab786e/363fc58b-d0d5-4f6e-afda-b1d880cf8747", "https://ms.immowelt.org/d9ae7b88-e98c-4d7f-8096-8ede0076f326/e28b854c-9b59-46d6-84a5-28d2595f9ff2", "https://ms.immowelt.org/dffe6319-03a2-4071-98a5-e0f1e3954460/de63d734-7d33-492b-acbf-be5ca5b61e49", "https://ms.immowelt.org/8af5caf8-2627-4044-83b1-a3824003abcd/a9a95b7e-658f-4e56-989c-5a564997561b", "https://ms.immowelt.org/de373ea2-fa91-495b-aa05-ffa24233b025/ff4e0de7-6c79-411b-bec2-3f5b973c460c", "https://ms.immowelt.org/1db3601f-db1c-4e6f-8b1d-e2f17c88804b/e84274ae-8668-49f0-8327-447ff8511752", "https://ms.immowelt.org/6bc525ad-0769-42c3-aaff-a169a251a660/789b8d1b-633d-4989-a0e8-50949ea51d51"]</t>
+          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>{"salutation": "Herr", "firstName": "Arnold", "lastName": "Hammer", "mobile": "017683299994", "phone": "0931/60565"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld ", "basicObjectPricEur": 1100, "basicLivingSpace": 103, "basicRooms": 4, "basicConstructionYear": 1984, "basicCity": "W\u00fcrzburg", "basicStreet": "Unterer Kirchbergweg 37", "basicUrl": "https://www.immowelt.de/expose/2asr65p", "basicContactPhone": "0931/60565", "basicContactMobile": "017683299994"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2upu84s"</t>
+          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1874,12 +1874,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
+          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>580</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1889,12 +1889,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>44</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1904,32 +1904,32 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
+          <t>["WANNE"]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
+          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Progress bars added for full pipeline
</commit_message>
<xml_diff>
--- a/immowelt_price_guide/data/retrain_train_data.xlsx
+++ b/immowelt_price_guide/data/retrain_train_data.xlsx
@@ -496,7 +496,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
+          <t>"https://www.immowelt.de/expose/2am365w"</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -506,12 +506,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
+          <t>"Helle Wohnung mit Balkon in der vorderen Sanderau!"</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1183.37</t>
+          <t>700</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -521,54 +521,54 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>81.32</t>
+          <t>58</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1955</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["Kelleranteil", "GEPFLEGT", "FERN", "kable_sat_tv", "Balkon"]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "LocationId": 496022, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.400,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 190, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 890, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
+          <t>["https://ms.immowelt.org/0cd8c2fc-f0f8-4803-b570-0bc0474a7ed0/ff573215-5a42-4351-ba40-cfa78f0e290f", "https://ms.immowelt.org/9f20ac68-d479-4226-9c79-53570da7eb1d/e2de2ea2-5dcd-44f2-94d5-5e6076766679", "https://ms.immowelt.org/65a23389-315b-4e17-9a6f-c8bcf8e849a7/ef1d6fb2-36ee-4c22-9b98-1f57d5548397", "https://ms.immowelt.org/57d6c377-cfc6-48d1-a1d5-1088cf6393f3/bbd12d5a-7478-4c07-bfbf-ce2e86b907b4", "https://ms.immowelt.org/0a903ef0-4c0b-431f-af10-207debb8ec0e/ced5048e-e943-4b27-acce-5dba9b2424d9", "https://ms.immowelt.org/c5093796-6848-4a03-8695-1e10dfd39fb2/ee4c2860-ca11-43ee-b24a-c8691f01283c"]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+          <t>{"companyName": "arndt immobilien GmbH", "address": {"city": "Rimpar", "zipCode": "97222", "street": "Friedrich-Ebert-Str. 6"}, "salutation": "Frau", "firstName": "Brigitte", "lastName": "Lienert", "phone": "0931 46079392"}</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Helle Wohnung mit Balkon in der vorderen Sanderau!", "basicObjectPricEur": 700, "basicLivingSpace": 58, "basicRooms": 2, "basicConstructionYear": 1955, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2am365w", "basicContactPhone": "0931 46079392"}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
+          <t>"https://www.immowelt.de/expose/2a5ll5v"</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -578,12 +578,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
+          <t>"Exklusive 4-Zimmer-Neubauwohnung W\u00fcrzburg-Frauenland *Gartenstadt Keesburg*"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>554.99</t>
+          <t>1483.93</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,54 +593,54 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>58.42</t>
+          <t>102.34</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Stellplatz"]</t>
+          <t>["Neubau", "gaestewc", "DUSCHE", "Kelleranteil", "Personenaufzug", "Erdgeschoss", "PELLET", "Zentralheizung", "DSL", "PARKETT", "FLIESEN", "frei", "abstellraum", "Tiefgarage", "REINIGUNG", "Loggia", "kable_sat_tv", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Hans-L\u00f6ffler-Stra\u00dfe 3", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1483.93, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 290, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
+          <t>["https://ms.immowelt.org/46db7f7a-e5d8-4eb4-a01b-a2d4e62ab2be/bb78636c-2f3f-4c2e-a53b-ef1fa9683a15", "https://ms.immowelt.org/b16389b6-eb92-42af-8130-0a76d6025358/fce845ed-0986-423b-8c1e-afd09a953917"]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Jendrzej", "phone": "0931/382-7701"}</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Exklusive 4-Zimmer-Neubauwohnung W\u00fcrzburg-Frauenland *Gartenstadt Keesburg*", "basicObjectPricEur": 1483.93, "basicLivingSpace": 102.34, "basicRooms": 4, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Hans-L\u00f6ffler-Stra\u00dfe 3", "basicUrl": "https://www.immowelt.de/expose/2a5ll5v", "basicContactPhone": "0931/382-7701"}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
+          <t>"https://www.immowelt.de/expose/2ayb45v"</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -650,12 +650,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
+          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Gro\u00dfz\u00fcgige 6-Zimmer-Maisonette-Wohnung"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>532.19</t>
+          <t>3601.44</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -665,54 +665,54 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>56.02</t>
+          <t>225.09</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>["Personenaufzug"]</t>
+          <t>["WANNE", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Balkon", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3601.44, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 460, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
+          <t>["https://ms.immowelt.org/b888654a-7be0-4b1f-bb51-2d8dca6a1aa1/5dc0db39-67ad-4630-8a84-004692c1c198", "https://ms.immowelt.org/4cb98d26-30d4-40dd-9345-c05636fc3d6e/3d269755-d356-448a-a4e4-c9c9225867b0", "https://ms.immowelt.org/71ab24a9-6d26-4798-959a-526196ab2526/2338dbdc-85e0-452f-bbf4-cbd765176db2", "https://ms.immowelt.org/e212abae-27ab-4901-ad56-4abbf1ab429a/076c61fa-ae56-43bd-90cc-3d4a1f246534", "https://ms.immowelt.org/45fda28f-bd4b-477c-8e5b-025d3035fc24/25270c0c-e6f1-42be-9bc6-154afc390bde", "https://ms.immowelt.org/250e735d-28bf-4e41-a26e-10bdcc174a72/9ffa4901-709f-4a22-bcf8-4026af4845a8", "https://ms.immowelt.org/47738d72-90e1-400f-8f26-b0c89e0a04d4/b2671ee7-2150-4931-ae87-848ca314834d", "https://ms.immowelt.org/09239b5c-efed-4862-9be0-12284713015c/c50d605a-b30b-4c1e-b8c7-c377d0105c47", "https://ms.immowelt.org/32be8996-eac0-4fda-8211-2d8fadd6467a/c5cb6c3d-45d4-45e6-8603-f3cc8967b34e", "https://ms.immowelt.org/de7996d0-a07e-44a3-a014-b9f228303c3b/f4242060-e83a-4836-b64b-41645c5c5e94", "https://ms.immowelt.org/d9382006-8b3f-46eb-802b-250a8fca3f96/03f39cab-4da2-4c36-80c1-23a7fbd309fe", "https://ms.immowelt.org/36af7108-dfdd-4ff3-ab8b-6e92d3508062/2f20f749-7813-4534-bde5-1a624ad88952", "https://ms.immowelt.org/ba912dea-da2a-4abd-add2-64d03801c9f2/0f910eff-7ebe-4154-9f66-0556d0a42237", "https://ms.immowelt.org/469127b9-c85a-4e77-a7fa-af7365f65cc3/9cd962ef-da29-4690-9168-413036c7882b", "https://ms.immowelt.org/0341b685-a77c-4318-bf97-0b0facbf1946/c0c91076-cd90-41c2-8e29-c3d9b6bc4e76", "https://ms.immowelt.org/349ba8bc-380d-425c-9404-fe30348c76fb/be7df368-083b-4bf6-bb15-c9ee4809e9b4", "https://ms.immowelt.org/769d004b-9208-4258-b045-f78d35bbe304/cab7c6e2-a6fe-44e9-b980-49f912c4dc33", "https://ms.immowelt.org/32a4701e-f4a1-4e08-ac43-7f82a0871c0e/05462d50-f4b2-41fb-94fc-03251da46a31", "https://ms.immowelt.org/c3b62a14-8ad0-4bc1-ad12-407a7b7d45c1/1e082fb8-309d-48fd-9675-1e19df39056b"]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Frau", "firstName": "Heike", "lastName": "Fabiunke", "phone": "0931/382-7708"}</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Gro\u00dfz\u00fcgige 6-Zimmer-Maisonette-Wohnung", "basicObjectPricEur": 3601.44, "basicLivingSpace": 225.09, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2ayb45v", "basicContactPhone": "0931/382-7708"}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2arkq5m"</t>
+          <t>"https://www.immowelt.de/expose/2aeal5v"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -722,12 +722,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City"</t>
+          <t>"**Erstbezug** Renoviertes Studenten-Apartment nahe Uni Hubland und Wittelsbacherplatz"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2175</t>
+          <t>415</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -737,54 +737,54 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>26</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1950</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>["WANNE", "DUSCHE", "FENSTER", "Personenaufzug", "FERNE", "renoviert", "FERN", "Fu\u00dfbodenheizung", "Zentralheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Speisekammer", "Balkon", "Kunststofffenster"]</t>
+          <t>["DUSCHE", "FENSTER", "Souterrain", "GAS", "Zentralheizung", "LAMINAT", "FLIESEN", "frei", "Einbauk\u00fcche", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Rottendorferstra\u00dfe 55", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "\u20ac 6.525,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 2175, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 450, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2625, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "830", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 415, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 145, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/1e8dcfd3-4788-4f09-a3c0-28d3414e57a3/5c7e81c2-8706-4ef4-8899-cfd4e8a5a029"]</t>
+          <t>["https://ms.immowelt.org/a3c1d1a9-92f0-4260-b2b3-41eb1b7cb966/c490aefe-bdcb-4b73-9783-a0bcc158c257", "https://ms.immowelt.org/b05abc2c-f624-4093-86a5-80f153fa6197/05af8f24-b7e4-4ba5-872c-39eed41b4cb5", "https://ms.immowelt.org/5be4bd8f-231a-44d8-8f0b-608a4f6581bd/0af81664-7d97-498f-8adf-3b5b5fe348ae", "https://ms.immowelt.org/725fb4fb-900c-4cd8-9554-dd83fc7bd725/99474ade-0e13-4d47-bf95-373cf4af43ec", "https://ms.immowelt.org/a0bb9c06-d60a-40e4-9521-94d9c183a14d/93799d3a-657d-4385-b487-2691349273e9", "https://ms.immowelt.org/3b4d1b7b-a5fe-4a37-b98d-6fc308d03c5b/c80e2b27-9270-47ef-b292-eb1efd72ee07"]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>{"companyName": "Werner Fleischhacker Immobilien GmbH &amp;a; Co. KG", "address": {"city": "W\u00fcrzburg", "zipCode": "97072", "street": "Valentin-Becker-Stra\u00dfe 8"}, "salutation": "Herr", "firstName": "Werner", "lastName": "Fleischhacker", "phone": "0931/2706700"}</t>
+          <t>{"companyName": "M &amp;a; M Bauprojektierung  und Vertrieb GmbH", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Franz-Brentano-Stra\u00dfe 2"}, "salutation": "Frau", "firstName": "Selina", "lastName": "Wiesner", "mobile": "+49 176 21469496"}</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City", "basicObjectPricEur": 2175, "basicLivingSpace": 150, "basicRooms": 5.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2arkq5m", "basicContactPhone": "0931/2706700"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "**Erstbezug** Renoviertes Studenten-Apartment nahe Uni Hubland und Wittelsbacherplatz", "basicObjectPricEur": 415, "basicLivingSpace": 26, "basicRooms": 1, "basicConstructionYear": 1950, "basicCity": "W\u00fcrzburg", "basicStreet": "Rottendorferstra\u00dfe 55", "basicUrl": "https://www.immowelt.de/expose/2aeal5v", "basicContactMobile": "+49 176 21469496"}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
+          <t>"https://www.immowelt.de/expose/2a4kg5w"</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -794,12 +794,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"2-Zi. Penthouse Wohnung  mit gr. Terrasse, teilm\u00f6bliert, N\u00e4he Uniklinik"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>700</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -809,54 +809,54 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>["Neubau", "Kelleranteil", "GAS", "Zentralheizung", "moebliert", "Einbauk\u00fcche", "Terrasse"]</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Lindleinsm\u00fchle", "ZipCode": "97078", "LocationId": 496017, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1500", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Lindleinsm\u00fchle)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-lindleinsmuehle/mietspiegel"}}, "DataTable": [{"NumberValue": 700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 900, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>["https://ms.immowelt.org/5ffec635-8f46-4cc1-aadb-8b583ac94f49/a055949a-2702-4368-b5b3-7b0ed426b642", "https://ms.immowelt.org/8908f348-9991-4a07-ad66-d7d75614e10a/fca9e8be-88e9-418f-a5eb-9e0d5767a5f4", "https://ms.immowelt.org/cc8d5f7e-0ed9-47a3-818b-45790a8111fc/1ff9a9de-b0c2-4a71-935d-2fd2d9164ad1", "https://ms.immowelt.org/e595bf82-bf35-4dea-bb76-166a24244d92/420389cc-e1aa-4a32-94b8-9d099fca203b", "https://ms.immowelt.org/2512e689-4ae0-4ff9-9611-9f151ac18678/c4e6c45b-c697-41d7-a51f-d244d8f1a417", "https://ms.immowelt.org/e0483e5d-da13-4926-a03f-c238c4a327ae/737d7425-941f-4ec9-a90e-14f51213a74f", "https://ms.immowelt.org/23fe53b7-3d5a-4509-a222-5cb8ed3d516c/a46ccbc0-6aef-4e2f-ac21-6d245e72052d", "https://ms.immowelt.org/349313e4-73e0-40b7-b119-9fe817365e7a/7f23958c-275b-4a0e-8d30-ad6e79f317f7", "https://ms.immowelt.org/ac9b1a48-16e2-4119-98ba-9a1a890ff38b/c3716b49-d728-4b6a-900b-7d66e9cd4354", "https://ms.immowelt.org/e3084b71-0919-4d54-96d4-4d35ce184a9c/c4edd6a6-581b-4387-81e6-1df5e276dda7", "https://ms.immowelt.org/fa543343-fde7-4b91-b370-eee9cd1e0f90/62763f8c-bf88-4f8a-bbfc-b721085c2412", "https://ms.immowelt.org/2a737240-80f0-4710-a8f3-7c4f1c3f6233/08bf7007-717d-4120-b7cb-50bf91a1393b", "https://ms.immowelt.org/727ce8f8-3e8b-4da9-95ec-b855705005c5/07256d94-2372-4172-b756-d7101c994e5e"]</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>""</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>["GAS"]</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "2-Zi. Penthouse Wohnung  mit gr. Terrasse, teilm\u00f6bliert, N\u00e4he Uniklinik", "basicObjectPricEur": 700, "basicLivingSpace": 47, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a4kg5w", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a7j75n"</t>
+          <t>"https://www.immowelt.de/expose/2affg5v"</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -866,12 +866,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon"</t>
+          <t>"M\u00f6blierte Wohnung in W\u00fcrzburg/Mainviertel"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1181.21</t>
+          <t>1125</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>70.87</t>
+          <t>60</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -891,44 +891,44 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1957</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["WANNE", "Etagenheizung", "moebliert", "Einbauk\u00fcche"]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97082", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3540", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1181.21, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 219, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 169, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1629.21, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2.250,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1125, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/0d9ec1ef-21cc-484a-88ae-193c7267a3bb/1e78105c-6490-4468-a6c3-936b8b388b80", "https://ms.immowelt.org/5c55f670-770f-44e9-b26b-7c9164f4a76a/9f56e225-8915-45d3-9af7-0e36ad2d804e", "https://ms.immowelt.org/12a9fd2a-da00-49a5-9999-efb246a9d727/efc35e4b-a860-47d1-823d-1282d60e0bc6", "https://ms.immowelt.org/bb9a6b97-0d40-46d1-9b24-011a5dcc7508/40526838-218d-4a4c-9422-8bd98023d9f6", "https://ms.immowelt.org/1a701923-58c4-4074-92b3-3e6bc100d51c/2f4849ee-2b95-432d-8ed4-b41b0211a117", "https://ms.immowelt.org/4d6aee50-6e8f-423f-b67a-bd01a011592d/4d58cead-e166-4a77-8c0f-2ee869a9e824"]</t>
+          <t>["https://ms.immowelt.org/ed2e6e9a-a8cf-4e9e-89c9-92ebe0bd9ab9/3c8c330e-15e6-439e-be44-6f02de4b9dd5", "https://ms.immowelt.org/e963b58b-6a58-4830-8e37-e9e446a7ca40/edda2664-fb0a-48dc-bfe4-3b20c61c8b1d", "https://ms.immowelt.org/6945f917-297e-4dfb-b166-4245a2333e2c/5a890870-d05f-4063-b0e5-63ad31ca7572", "https://ms.immowelt.org/ffa99189-2ca2-46fb-aa14-f6fda02818ae/6a859704-19f9-4907-92f9-a5b7fcbe4248", "https://ms.immowelt.org/86e1504e-0c46-4800-a6e0-cf24601a2518/bf8eec93-53d3-4368-82bc-ca50c66a45a1", "https://ms.immowelt.org/f15519e3-ee04-4739-b40a-ce0f84fb29ff/2c2c7101-3482-420d-826e-9efd57863f1e", "https://ms.immowelt.org/54ea5d30-e104-4f39-8a41-429b5961bbd1/55bee8cc-3633-4bce-9b47-af1971f0523b", "https://ms.immowelt.org/e88c0a6a-0da8-4b88-8865-a9f37cbd0e2d/9452b370-8d6d-4324-8a35-57b8a433c48a"]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon", "basicObjectPricEur": 1181.21, "basicLivingSpace": 70.87, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a7j75n", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6blierte Wohnung in W\u00fcrzburg/Mainviertel", "basicObjectPricEur": 1125, "basicLivingSpace": 60, "basicRooms": 2, "basicConstructionYear": 1957, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2affg5v", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
+          <t>"https://www.immowelt.de/expose/2a54x5v"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -938,12 +938,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1165</t>
+          <t>900</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -953,12 +953,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>80</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -968,39 +968,39 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["FENSTER", "Kelleranteil", "Personenaufzug", "GAS", "Zentralheizung"]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Rottenbauer", "ZipCode": "97084", "LocationId": 496020, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1800", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Rottenbauer)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-rottenbauer/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1100, "Unit": "EUR"}, {"NumberValue": 20, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"salutation": "Frau", "firstName": "Astrid", "lastName": "Leis"}</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 900, "basicLivingSpace": 80, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a54x5v"}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
+          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1010,12 +1010,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>566.96</t>
+          <t>420</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1025,54 +1025,54 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>59.68</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>["Stellplatz"]</t>
+          <t>["GAS"]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
+          <t>"https://www.immowelt.de/expose/2av845v"</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1082,12 +1082,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
+          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Helle 3-Zimmer-Wohnung mit Balkon"</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>1797.71</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1097,54 +1097,54 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>123.98</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
+          <t>["WANNE", "gaestewc", "DUSCHE", "Kelleranteil", "Personenaufzug", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Balkon", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 1797.71, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 250, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
+          <t>["https://ms.immowelt.org/34aad469-3611-425d-9832-c02c7060cb23/77ba9d6f-e612-4962-9317-bd0107dc25f7", "https://ms.immowelt.org/8ea07a0f-c3a2-4e3e-a9d2-fe6544358d93/58dbc143-5e69-4062-9eae-b767cf0c69b1", "https://ms.immowelt.org/6b6cd2cc-a04d-480c-949a-1a21bbd7e1d4/51babd4b-8fbc-456a-862b-c4ebde7dc41a", "https://ms.immowelt.org/a8f09c5d-403e-4528-a15f-17ef6819f51c/15cf94e1-0865-4970-bdbc-7eeb2e4e321a", "https://ms.immowelt.org/a74342e9-df14-4a0d-b4c6-600423e5e886/caed2534-21fc-4d11-981c-a2164e56802b", "https://ms.immowelt.org/57b465e5-f400-4f58-8856-6a92ccb5dc5c/e24df36d-9d71-44a2-bd39-c0146b4df941", "https://ms.immowelt.org/4d380785-997d-4deb-b741-8c14d08622b6/d794011b-6b71-4e97-adb0-c319032680b3", "https://ms.immowelt.org/a1aeaa9b-89a7-4a5b-b3ed-598756319607/14a91c1a-5084-49dc-b75d-74d20228a8f0", "https://ms.immowelt.org/af2232f0-1ef7-4481-801f-2a5ff59e0092/96a901ff-03de-431d-886e-d860ac84fbc4", "https://ms.immowelt.org/eb83b1d9-acf0-4e74-b0b3-5fa3fcc1ca01/705ad620-364a-4237-968f-e9f4e0c3eb36", "https://ms.immowelt.org/b34e24ec-eac1-4eae-b4db-e1f386853cb1/292b937e-2528-4472-8123-fa7a878ef84b", "https://ms.immowelt.org/4111770b-ae7b-4dce-b625-f990d3c5ba1e/b7539eac-4bf3-4d62-ab60-f12720be1758", "https://ms.immowelt.org/73dc46c5-cb67-4432-b97f-e11d22268b50/6613c506-3bb4-4e53-a0ac-d3296fe50f9c", "https://ms.immowelt.org/d8083607-cc91-46ee-92df-9a6f4eed9d3b/59f57e14-612a-4c44-8a58-7436d9771597"]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Herr", "firstName": "Wolfgang", "lastName": "Roth", "phone": "0931/382-7702"}</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Helle 3-Zimmer-Wohnung mit Balkon", "basicObjectPricEur": 1797.71, "basicLivingSpace": 123.98, "basicRooms": 3, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2av845v", "basicContactPhone": "0931/382-7702"}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
+          <t>"https://www.immowelt.de/expose/2abty5v"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1154,12 +1154,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
+          <t>"[TAUSCHWOHNUNG] Wundersch\u00f6ne helle Altbauwohnung"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2880</t>
+          <t>430</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1169,54 +1169,54 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>64</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 430, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 115, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
+          <t>["https://ms.immowelt.org/7a4af935-fdca-42b8-b470-a905b68d671e/717dc8fc-8461-4d19-89e3-3eaf6c5bfb76"]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "Tauschwohnung GmbH", "address": {"city": "Bonn", "zipCode": "53175", "street": "Graf-von-Lehndorff-Str. 12"}, "profilePicture": "https://filestore.immowelt.de/ProfilBilder/150_13236f6bb6c141cd845d0ac0006487a0.jpg", "salutation": "Herr", "firstName": "John", "lastName": "Weinert", "phone": "+4922892939484"}</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "[TAUSCHWOHNUNG] Wundersch\u00f6ne helle Altbauwohnung", "basicObjectPricEur": 430, "basicLivingSpace": 64, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2abty5v", "basicContactPhone": "+4922892939484"}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
+          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1226,12 +1226,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"Bestlage mit Festungsblick"</t>
+          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>610</t>
+          <t>580</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1241,12 +1241,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>44</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1256,39 +1256,39 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
+          <t>["WANNE"]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
+          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2awv45u"</t>
+          <t>"https://www.immowelt.de/expose/2ay645v"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
+          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Ger\u00e4umige 6-Zimmer-Maisonette-Wohnung"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1720</t>
+          <t>3163.32</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1313,54 +1313,54 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>123.36</t>
+          <t>218.16</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
+          <t>["WANNE", "gaestewc", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "Erdgeschoss", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3163.32, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 440, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
+          <t>["https://ms.immowelt.org/33a10e2d-1546-47e8-8bf4-47024f96365d/8d31a374-f6c2-4671-ba5e-b06a8d7c1f18", "https://ms.immowelt.org/e715d610-ea80-4459-9e3a-1ea8a574c0d7/c594e925-e9d3-4474-88ff-ee637dc4b81a", "https://ms.immowelt.org/f3e49668-7602-45ad-979f-f68f0c60ad46/6da2c38a-e66f-4112-b3c3-70ebaa38a22f", "https://ms.immowelt.org/e4691abb-17a5-41aa-949d-88daa0ab8d3a/42a9ae4f-34fd-4230-8329-9c00ba557222", "https://ms.immowelt.org/62981e85-dc6c-481f-8d77-c7e82c11d711/a90f265f-b3b3-4b6b-a854-a05b00191bac", "https://ms.immowelt.org/c1f1f311-d95b-465f-94a6-317a246989d2/e96a7cca-1527-484c-a8e9-f79e1cf28136", "https://ms.immowelt.org/935854af-6f17-4d5d-b023-6647d4cc8d4d/87cabb52-19fe-4dca-a81d-9b0f6d4daa7c", "https://ms.immowelt.org/d22f872e-159f-4f19-bb2a-75f5b228899d/044b33f6-2258-490a-ae2a-52d9ce17b653", "https://ms.immowelt.org/58dca412-8d3b-415e-9a26-359678019657/0858d4e1-5dc0-4297-8a4f-b5db5dbeb8b8", "https://ms.immowelt.org/f9bab463-404a-46c6-990a-559df575f251/6d53c5c6-d652-4e1d-98e5-448095327b4f", "https://ms.immowelt.org/6559ac4a-0154-4e05-a366-dbf71d55ad3a/29c1a7fd-15be-4a1b-91ca-9db0f1c442f3", "https://ms.immowelt.org/85c20839-cb59-4728-be4d-78d1ffcb9274/f88983a1-2f68-4f01-af1a-cae1794eb9e4", "https://ms.immowelt.org/f0a33cc2-272c-4fe9-a229-0c65344655fb/1911e15f-4afd-4691-a583-109b097d5b1a", "https://ms.immowelt.org/26da2883-f715-4c66-a8d1-3e2b9550fcf3/90d1f6cc-c1ae-4b39-889a-79bf683b589e", "https://ms.immowelt.org/b51072d7-8214-4cb3-b4f1-4c2d9c08cc58/e2548663-d3a0-4cb8-b0f7-5aaacf362ba3", "https://ms.immowelt.org/b5dd6e96-9575-46aa-af37-c7a1914335de/e4d4ff07-527e-4aff-be0a-66c047b2b747", "https://ms.immowelt.org/4c4b10ce-78b2-449d-a1c4-38ef2035555b/8094732c-995f-4ee6-af5f-e52e6a68bac8", "https://ms.immowelt.org/36750323-149d-49f3-8859-a599078cdc7a/0c862b3d-b2f3-4b3a-b234-8e9299775647", "https://ms.immowelt.org/d1d807de-1e05-4eca-b9fd-01dd45660714/8d6cc502-9779-4a2e-bfea-d50b253ff0f3"]</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>{"companyName": "Gute Bude Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 3c"}, "salutation": "Frau", "firstName": "Nelly", "lastName": "Gronau"}</t>
+          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Frau", "firstName": "Heike", "lastName": "Fabiunke", "phone": "0931/382-7708"}</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Ger\u00e4umige 6-Zimmer-Maisonette-Wohnung", "basicObjectPricEur": 3163.32, "basicLivingSpace": 218.16, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2ay645v", "basicContactPhone": "0931/382-7708"}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
+          <t>"https://www.immowelt.de/expose/2aewq5u"</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
+          <t>"Moderne 1,5- Zimmerwohnung in W\u00fcrzburg/Altstadt"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>474.53</t>
+          <t>950</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1385,54 +1385,54 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>49.95</t>
+          <t>37</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1990</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>["Personenaufzug"]</t>
+          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert", "FLIESEN"]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.900,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
+          <t>["https://ms.immowelt.org/f347f786-4652-4c8e-9723-ceb8482ed2a3/16c9950f-4ace-41f5-9ccc-eaaa0aa3dbb9", "https://ms.immowelt.org/60aa648f-6f16-4380-abe5-63e8ae5378dd/1d329405-999e-47ed-b506-8156c516bb9c", "https://ms.immowelt.org/16d637dd-3a33-4bf0-8693-79b7659f1eb0/e2923eba-0c2c-43c0-a404-10acd4276f3a", "https://ms.immowelt.org/7ab4e781-08fe-4bc5-9a39-8cc82d9e56f4/a82e3028-f3d5-4cfe-bd0b-a551438ca593", "https://ms.immowelt.org/0a430e4b-4799-408b-aab0-eb47ee04004d/cebdd699-3ea0-4f8e-b231-dfc611d1523e", "https://ms.immowelt.org/08456fdf-7e5a-4d08-bb25-8826aa6af0b4/8a06e9fe-62da-48f0-b99a-b150ea1634ec", "https://ms.immowelt.org/9100c73b-327e-4e9a-8a72-a66c8a7da1fb/b5084958-c7a1-4b5e-963e-7f9f02d43f7a", "https://ms.immowelt.org/57737cd7-44f5-4687-a55c-2f3d25320540/1f93643c-235f-4804-a283-65554ed0f691", "https://ms.immowelt.org/79943cff-f49b-46a1-a29e-0d545ee5c5b8/a7e253ae-bc77-4373-a712-673cae102a7a"]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Moderne 1,5- Zimmerwohnung in W\u00fcrzburg/Altstadt", "basicObjectPricEur": 950, "basicLivingSpace": 37, "basicRooms": 1.5, "basicConstructionYear": 1990, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aewq5u", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aebr5t"</t>
+          <t>"https://www.immowelt.de/expose/2akwq5u"</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1442,12 +1442,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!"</t>
+          <t>"Hell m\u00f6blierte  2-Zimmerwohnung in W\u00fcrzburg/Frauenland"</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1290</t>
+          <t>1095</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1457,54 +1457,54 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>63</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "PELLET", "Fu\u00dfbodenheizung", "Garten", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["DUSCHE", "moebliert", "PARKETT", "FLIESEN", "Einbauk\u00fcche"]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Eibelstadt", "ZipCode": "97246", "Street": "W\u00fcrzburger Strasse 25", "LocationId": 11869, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2600", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Eibelstadt", "Link": "https://www.immowelt.de/immobilienpreise/eibelstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1290, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1570, "Unit": "EUR"}, {"NumberValue": 40, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2.190,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1095, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7c821767-b600-4ad9-8a2a-50874a2a87cf/92a3b2aa-0393-4e55-ad97-c6c3a803a0d8", "https://ms.immowelt.org/8081e4f6-2ad6-46c7-957d-07597db5c5a8/ee5c7a33-80cd-4c89-bb96-98be1b013e27", "https://ms.immowelt.org/515a3a85-6263-4990-b640-f75ec6075c4b/8456cc16-2fc0-409e-ba1f-f103285c6d18", "https://ms.immowelt.org/340c6f6f-746d-421c-aab8-4850f62a5e6b/e971e1c3-7527-4fb5-a83c-f5221d132bc5", "https://ms.immowelt.org/6205eb16-8906-4267-a472-86439d570e9c/39733ff0-9850-43ab-a6fa-f4f2291ba17d", "https://ms.immowelt.org/3b9c4f71-f8fa-46fa-a1d6-7bab696693cb/eccec98b-d098-4d62-ae2c-f62c71c18721", "https://ms.immowelt.org/ab60445b-088f-4fe5-9554-7448a4a29bb2/0eb8642f-4cb3-4252-b4b5-622b757475d6", "https://ms.immowelt.org/6b12d3cb-5e11-4c67-9c0e-a69e674fc018/3d35f5b5-f31d-4200-8572-5eb83a1079e5", "https://ms.immowelt.org/11466902-020f-43ec-9441-09395d524b18/3136e448-448b-41f8-bcec-58fea52abdd5"]</t>
+          <t>["https://ms.immowelt.org/f58fd648-14ff-458e-b34e-ed1a79e43d74/d87e4e66-4884-409c-b2cb-2157459b3064", "https://ms.immowelt.org/0a87650a-5809-4688-8750-7ae6c25a4099/e24ce7b4-9191-4f35-a1d0-23492c9ab7b0", "https://ms.immowelt.org/791a160a-38a3-4dce-a18c-5ce7143fd3f5/bd4c9b95-f50f-4c31-a999-9365ab6d2f07", "https://ms.immowelt.org/d04e8834-3fb6-41c7-b54a-e8fbd81f4738/544118d8-4448-48cb-b903-f895e30a79c2", "https://ms.immowelt.org/0a28069f-f140-484b-8e74-4397443a7579/52a860be-e6e0-41df-ad9f-635a12c08567", "https://ms.immowelt.org/93620f2c-07ac-40ae-89e8-09de2a90ffff/0aad3bf6-a9a2-41e4-841c-299b26265c3a", "https://ms.immowelt.org/a67d6581-3a59-4dc4-a4f3-965a7168620b/da1adff0-5907-4ab5-8913-e075b2d30c48", "https://ms.immowelt.org/deeb3874-cc27-4a7f-ac51-854d6765dd3f/3218f2ca-a245-4045-af54-619a9b8882e3", "https://ms.immowelt.org/ac67f904-20c4-4c6b-90f1-3d808fa8dae1/795689c7-539e-470a-a2a4-32e423451bd3", "https://ms.immowelt.org/974474bd-d9e3-4117-a672-6922106d164c/a2bb49a6-741b-40b0-8a0b-40d9f75d0f02", "https://ms.immowelt.org/936ffd96-d118-4d3d-8f77-ff73d6726300/5bb5b59e-9b1c-44ee-816e-31d9b28dd5a2", "https://ms.immowelt.org/9e5f7e76-6418-46d5-af9c-45309a550a97/c9909e8a-e4cd-4d4e-826e-4ec43a4165d9", "https://ms.immowelt.org/fc5c4ab6-6dd7-402d-aa17-1d5f9d8e29b0/f9213bf7-281b-4c08-8f0b-e78f6fcb7c71", "https://ms.immowelt.org/efbfc541-75da-4200-8395-1db7a9483e5b/68140100-e86c-4af6-88d7-26d0e819a523", "https://ms.immowelt.org/6069128c-8b73-4678-abc6-ee0b63823860/cceb6f64-a341-4849-9927-b2c5dd025aad", "https://ms.immowelt.org/c13a4106-75b6-444b-87e0-05ccdb99308c/a077d4b3-99d4-474b-b40f-6be9110341d9"]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>{"salutation": "Herr", "firstName": "Maximilian", "lastName": "Kauschke"}</t>
+          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!", "basicObjectPricEur": 1290, "basicLivingSpace": 93, "basicRooms": 3.5, "basicConstructionYear": 2022, "basicCity": "Eibelstadt", "basicStreet": "W\u00fcrzburger Strasse 25", "basicUrl": "https://www.immowelt.de/expose/2aebr5t"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Hell m\u00f6blierte  2-Zimmerwohnung in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 1095, "basicLivingSpace": 63, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2akwq5u", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2asr65p"</t>
+          <t>"https://www.immowelt.de/expose/2abjp5u"</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1514,12 +1514,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld "</t>
+          <t>"6er-Studenten-Wohngemeinschaft - Zi.Nr. 2"</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>320</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1529,54 +1529,54 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>1972</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "renoviert", "GAS", "Etagenheizung", "gartennutzung", "Einbauk\u00fcche", "wg_geeignet", "Balkon"]</t>
+          <t>["Dach ausgebaut", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "GEPFLEGT", "Massivhaus", "GAS", "Zentralheizung", "DSL", "teilweise m\u00f6bliert", "FLIESEN", "frei", "Einbauk\u00fcche", "wg_geeignet", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "Street": "Unterer Kirchbergweg 37", "LocationId": 496013, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Amalienstr. 6", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2200,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1400, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "640", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/bbd4dcbf-c64e-4c60-9789-afc66db53a3f/7fc04ce4-7f84-4ce5-8111-31fcc917306c", "https://ms.immowelt.org/315ff83e-d234-453a-ad52-c4b99bef7055/a979f182-320d-49d1-8002-bcde353d36ee", "https://ms.immowelt.org/6137c704-6a29-47ae-a5a3-88abd0a2fde0/d535204c-f43a-4229-8152-507fc644a211", "https://ms.immowelt.org/1981c2ad-23cb-41f4-825a-77d67f5fbbe7/e968ecc9-ea46-4188-a2c4-968720f069c0", "https://ms.immowelt.org/a4965ee1-de2b-4d90-8333-b793f90a7406/867d9997-6f27-48da-ade0-9096bf31cf3e", "https://ms.immowelt.org/aed0a388-445d-4f8f-9afd-4a146b35d962/3bc7e507-92a3-446a-a3f1-5799c1df7338", "https://ms.immowelt.org/f9d8ba2e-fb1a-4cdd-98ea-ba6ba4973c25/fde9d74e-bd14-4413-a148-81aad236c43f", "https://ms.immowelt.org/e0fbe89c-ecbb-41e9-9ecd-61c2762b9189/3784b2d8-f66d-4f7f-a893-cb9c7b3e982c", "https://ms.immowelt.org/16af38b3-f1c4-4d16-ba17-2685efc0dbe6/b5361690-0608-4e15-8167-e5ab29ac41e7", "https://ms.immowelt.org/fb842589-0c99-45bb-b567-5d04f811adf5/729e7fb7-c4eb-47db-936a-8a406b3efda8", "https://ms.immowelt.org/2f97e2d2-4fcd-40db-bee9-5d4161812bb0/a57df980-0cf8-4352-8cf0-5e867376c343", "https://ms.immowelt.org/79cf67c5-73a5-4097-8b85-e20df2ab786e/363fc58b-d0d5-4f6e-afda-b1d880cf8747", "https://ms.immowelt.org/d9ae7b88-e98c-4d7f-8096-8ede0076f326/e28b854c-9b59-46d6-84a5-28d2595f9ff2", "https://ms.immowelt.org/dffe6319-03a2-4071-98a5-e0f1e3954460/de63d734-7d33-492b-acbf-be5ca5b61e49", "https://ms.immowelt.org/8af5caf8-2627-4044-83b1-a3824003abcd/a9a95b7e-658f-4e56-989c-5a564997561b", "https://ms.immowelt.org/de373ea2-fa91-495b-aa05-ffa24233b025/ff4e0de7-6c79-411b-bec2-3f5b973c460c", "https://ms.immowelt.org/1db3601f-db1c-4e6f-8b1d-e2f17c88804b/e84274ae-8668-49f0-8327-447ff8511752", "https://ms.immowelt.org/6bc525ad-0769-42c3-aaff-a169a251a660/789b8d1b-633d-4989-a0e8-50949ea51d51"]</t>
+          <t>["https://ms.immowelt.org/9ba52a69-6182-42ac-b135-aa03971398d6/ca08d294-c112-4542-9217-884244d0d406", "https://ms.immowelt.org/d2976824-6694-44cf-a9b6-27ee23e5ee7d/3b4552e6-7f48-4f9f-8935-65701930862a", "https://ms.immowelt.org/abd16da6-4e60-4077-9fde-df90d5c35ba9/70090f09-6bb6-46bb-8d61-ad69a6f9d337", "https://ms.immowelt.org/9241bd02-41ac-4193-ac08-cb9f982e4abd/4fa1546f-a5f4-4860-b778-44b40407edcb", "https://ms.immowelt.org/297cca9d-a7ba-4a67-92d9-93365151b7c5/d95e6e27-06ec-47b3-b787-69c008ab106a", "https://ms.immowelt.org/3b016415-9aa0-4c6f-bf4a-a08f53671a65/e9132359-9ac5-4683-82f7-c4fc218d8306", "https://ms.immowelt.org/4282be92-39da-4459-a8c5-34173ddc7b9f/a8aeb00d-0b5a-48c1-b780-9278afd054ca", "https://ms.immowelt.org/3f00ed7e-8bf1-401b-8f25-642aae0303e9/8f662276-261e-4853-9a0e-c16cf1a0cf16", "https://ms.immowelt.org/33cac6b2-f066-48ee-b86f-8f34b674b64f/8da9104b-a492-47aa-af05-5e118833566f", "https://ms.immowelt.org/ac6357bc-41cd-473b-8073-52aba4823641/a4383c9d-9081-4f5f-afb3-b59a77fa5b00", "https://ms.immowelt.org/d4734ed1-2904-4290-956a-e971b09473c8/b9a53b6e-72d5-418d-a421-3175e22ad8b1", "https://ms.immowelt.org/e5fc4d4c-767b-44a4-ac3c-a5c84a34fe37/4bf5f24d-e49d-4e14-bae7-18735aba7802", "https://ms.immowelt.org/2fa16c88-73cf-4bf1-9ce3-d457a8a03c5e/caa28f6b-695e-4ee6-bc27-d83d081028ad", "https://ms.immowelt.org/600d4913-62e1-4dd5-9431-46e3dc04f5c0/31f22258-60a5-4acd-874e-d498ea457528", "https://ms.immowelt.org/c78f9909-a0a5-427d-9b1f-a8553957ae21/3eb778af-08e1-40d5-b415-3df323797a59", "https://ms.immowelt.org/de687aba-16ee-476d-a8f9-30df0fe0ec6a/a9787e5c-ea67-488e-af3c-076b4e47fea9", "https://ms.immowelt.org/8b1beea6-698d-4888-97b4-de46bd7498ed/4f90c6e0-1013-4950-9c20-5c0ff18aad7d", "https://ms.immowelt.org/da588edf-b340-4add-adc0-fb3f0c96ad72/59acdf1e-b87f-4ddb-b8d5-ab9ae3aee1eb", "https://ms.immowelt.org/9642eeca-e631-4ac4-ae64-100ae2a9f0e9/996373fc-c623-4411-afbc-f2104a65e4a7", "https://ms.immowelt.org/773ea5c5-cb8c-413d-a62d-d05b7ed9e19e/ca6e755b-48d9-4b44-9df9-56eb13fc5024", "https://ms.immowelt.org/e7f711ba-ac7b-44fc-90e8-deda2cee8b0c/bd0ca932-727d-4d26-8518-5c0e19bf2160"]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>{"salutation": "Herr", "firstName": "Arnold", "lastName": "Hammer", "mobile": "017683299994", "phone": "0931/60565"}</t>
+          <t>{"companyName": "M &amp;a; M Bauprojektierung  und Vertrieb GmbH", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Franz-Brentano-Stra\u00dfe 2"}, "salutation": "Herr", "firstName": "Sascha", "lastName": "Mannel"}</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld ", "basicObjectPricEur": 1100, "basicLivingSpace": 103, "basicRooms": 4, "basicConstructionYear": 1984, "basicCity": "W\u00fcrzburg", "basicStreet": "Unterer Kirchbergweg 37", "basicUrl": "https://www.immowelt.de/expose/2asr65p", "basicContactPhone": "0931/60565", "basicContactMobile": "017683299994"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "6er-Studenten-Wohngemeinschaft - Zi.Nr. 2", "basicObjectPricEur": 320, "basicRooms": 1, "basicConstructionYear": 1972, "basicCity": "W\u00fcrzburg", "basicStreet": "Amalienstr. 6", "basicUrl": "https://www.immowelt.de/expose/2abjp5u"}</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
+          <t>"https://www.immowelt.de/expose/2agwq5u"</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
+          <t>"M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>950</t>
+          <t>649</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1601,54 +1601,54 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>21</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1911</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
+          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert"]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.298,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 649, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
+          <t>["https://ms.immowelt.org/cf8697dc-afcd-47ae-aadc-64c4cc78569c/35b4d352-660a-4816-94a6-619497123ae8", "https://ms.immowelt.org/a32b8f72-a566-4394-bea1-04e883e8fce2/7099cff9-9eea-4d1f-bad4-4033626afe54", "https://ms.immowelt.org/105a8a3c-c718-4c20-83ac-d0a5ef1a7f53/9db73218-715a-4963-942c-e41a29ef7b07", "https://ms.immowelt.org/64d9efa5-0a66-44fe-aa1e-b89f834ad546/6f687f3d-4a05-4f47-a1f8-8b78ca7e8bfe", "https://ms.immowelt.org/a3fe7335-2ba5-4c30-a137-cbfb5fd2a35c/20496698-5e1f-4243-9338-f56821682d4a", "https://ms.immowelt.org/a449833e-f4f4-43ff-8ebf-01bc5160e5c9/ccc566af-477b-4888-b03f-1cc64f4f1c45", "https://ms.immowelt.org/a6d17184-1155-46e9-af2c-d83d9e1be344/aab72d40-469f-486c-9add-806a5481ac6a", "https://ms.immowelt.org/a5271f16-acef-4db4-84ba-2b1a9ddc5892/57e11dd6-6321-45eb-85e0-aaa0f1e15bfe", "https://ms.immowelt.org/921ae069-2035-4dbb-a619-8ad9012a2442/0e6324ba-04b0-4141-bcc2-3b6cb33ac8ea", "https://ms.immowelt.org/6dc638c1-e4cd-4f0c-87b2-169cc34b0bd8/2af01fd5-93ce-4fc8-ae87-9a3817a2ef84", "https://ms.immowelt.org/a5894c49-800c-4d59-bb53-e598cf560634/0aa6a439-1071-40bd-a3ef-3bd2192fad8c", "https://ms.immowelt.org/1824d009-9f1e-4248-ac1b-d6198f9c17f3/ffd7b610-0d17-43b2-b15c-614cccf8be14", "https://ms.immowelt.org/45f31b8e-c2fc-45ff-8dac-c0bf8fea6e03/a11c6ffd-ddba-4524-9aca-520b2604d193", "https://ms.immowelt.org/5ec8ff49-d6b8-4dd0-bd1b-a04062520b58/b2e43f71-c2eb-4713-a428-6da937a58826"]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 649, "basicLivingSpace": 21, "basicRooms": 1, "basicConstructionYear": 2015, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2agwq5u", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2gr494f"</t>
+          <t>"https://www.immowelt.de/expose/2a9245v"</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1658,12 +1658,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"Sch\u00f6ne 3-Zimmer Wohnung - Zell am Main  Hauptstra\u00dfe"</t>
+          <t>"Neu m\u00f6blierte Wohnung im Herzen der W\u00fcrzburger Altstadt unweit des Marktplatzes mit Wlan"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>715</t>
+          <t>815</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1673,54 +1673,54 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>82.2</t>
+          <t>40</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1900</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Erdgeschoss", "GAS", "Etagenheizung", "DSL", "KUNSTSTOFF", "Sat", "Kunststofffenster"]</t>
+          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert", "TEPPICH", "FLIESEN", "Balkon"]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Zell a. Main", "ZipCode": "97299", "Street": "Hauptstra\u00dfe", "LocationId": 12631, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2145", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Zell a. Main", "Link": "https://www.immowelt.de/immobilienpreise/zell-a-main/mietspiegel"}}, "DataTable": [{"NumberValue": 715, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 110, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 125, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.630,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 815, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/843e2d49-84f6-4e47-b77d-63d29ab1066e/26140dff-55d6-4812-bc01-0d9e6c646fa0", "https://ms.immowelt.org/41f37c51-8639-4424-8ee1-7a2fefff4273/d88e819f-e564-4c41-bbac-99323793838a", "https://ms.immowelt.org/662f3397-8654-43ec-b435-d79bacab8763/2fc81c17-dad7-4a2f-a9bb-77e7f8fa27dc", "https://ms.immowelt.org/f8805103-18da-476d-9f24-d04169f73813/a5cf5830-f53c-4a5e-9f1b-78a790ec5d0a", "https://ms.immowelt.org/460515a3-d738-48d8-9c73-c7c11596d325/5bbddf00-b1c1-4704-9731-886ba0a1b78a", "https://ms.immowelt.org/525c5aa4-226e-4419-bb47-0d14c2e5bd62/73fae45a-7a74-4082-b2ad-c3876b95942d", "https://ms.immowelt.org/863f8610-efdb-47dd-9cc5-249b10b8d350/fc44d80c-bb9d-44f0-afb1-dbe1a240157a"]</t>
+          <t>["https://ms.immowelt.org/56dbfa19-0b11-4212-a585-a3bb9055fc6c/55af236d-1cf3-446a-a9ea-5d847c1f3c78", "https://ms.immowelt.org/2321a506-3294-4da0-8ed9-9c32a877cc19/568e9ef6-6f64-4112-9523-9eaf25a3f970", "https://ms.immowelt.org/c49d4e0e-c519-4110-bf9d-48d46975f264/51ad8f90-ae3d-4f54-9436-a3ce93d787e0", "https://ms.immowelt.org/1efec59d-a37f-4e4e-81e0-d2638e029208/c9bd61b7-4af9-4819-822e-916b4c491efd", "https://ms.immowelt.org/35f3c816-30ad-4cfa-a370-9fd3df5a890b/0f5a8622-ff9b-48a3-b656-48f75cd9c811", "https://ms.immowelt.org/1d11277d-e06d-43d1-807a-35d99c5f5cd5/51935719-85d7-4a46-a718-1c1a7bedba2c", "https://ms.immowelt.org/3f9f17e0-3b0f-42d8-9623-bd41d7d12fc4/d88f57cc-ca14-47d1-b0ac-e5d037c3114a", "https://ms.immowelt.org/4c16ccd5-7611-496f-9fc2-a5cc9e95ca96/0cc9afbf-324b-4dc0-a841-e5417e3c909f", "https://ms.immowelt.org/23f4ce8d-d0f3-42f3-b7c2-cbea89a39473/eb285820-0b71-4189-8a94-494d832c127b", "https://ms.immowelt.org/36d590ab-2de9-46f3-8cef-b4af4efd9be0/8e11440a-7fe1-49cf-a002-13e4285760be", "https://ms.immowelt.org/8099beb8-56a4-493f-b95f-2490484605d5/fbb624d4-8b55-48d5-8b8f-5535a08872c5", "https://ms.immowelt.org/1978dbc1-a0ed-458a-abcd-d22f103809ef/1a5cc04f-0b65-48af-8e69-c835714ab2e7", "https://ms.immowelt.org/6b1ab129-3f95-42da-9d53-8088db0a9349/25c6e471-016e-4261-b4ae-a73987e4f403", "https://ms.immowelt.org/9b310d23-aa9d-41f5-8f34-29a9b7aa4471/bae39b36-c4b5-4cf8-882a-aca3ba40538c", "https://ms.immowelt.org/20713457-85cd-4f26-970b-eca4af0b6b71/be6308f1-d0c9-4aa5-8a10-3a4f1f28ff33"]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Sch\u00f6ne 3-Zimmer Wohnung - Zell am Main  Hauptstra\u00dfe", "basicObjectPricEur": 715, "basicLivingSpace": 82.2, "basicRooms": 3, "basicConstructionYear": 1900, "basicCity": "Zell a. Main", "basicStreet": "Hauptstra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2gr494f", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Neu m\u00f6blierte Wohnung im Herzen der W\u00fcrzburger Altstadt unweit des Marktplatzes mit Wlan", "basicObjectPricEur": 815, "basicLivingSpace": 40, "basicRooms": 1.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a9245v", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2almm5r"</t>
+          <t>"https://www.immowelt.de/expose/2acjp5u"</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1730,12 +1730,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE"</t>
+          <t>"6er-Studenten-Wohngemeinschaft - Zi.Nr. 4"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1700</t>
+          <t>350</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1745,54 +1745,54 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>153.3</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>1972</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "GAS", "Zentralheizung", "teilweise m\u00f6bliert", "TEPPICH", "PARKETT", "FLIESEN", "Einbauk\u00fcche", "offene K\u00fcche", "Stellplatz", "Tiefgarage", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
+          <t>["Dach ausgebaut", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "GEPFLEGT", "Massivhaus", "GAS", "Zentralheizung", "DSL", "teilweise m\u00f6bliert", "FLIESEN", "frei", "Einbauk\u00fcche", "wg_geeignet", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Gartenstra\u00dfe 9", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Amalienstr. 6", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5.400,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 1700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 240, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten", "Comments": ["in Warmmiete enthalten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2340, "Unit": "EUR"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 350, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 450, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/338d1cbc-cb3f-423f-8523-42cc120d72f9/e4b563bc-671f-4dea-a726-71d7b9386009", "https://ms.immowelt.org/4da068e4-1a27-465c-b0e7-ffb77b79880b/908c43fa-aa39-4e85-97c8-98295a3c363c", "https://ms.immowelt.org/cab19ffc-0f4a-42a9-89e9-7189e9dafd92/2a5e6769-ad31-4185-a454-e8d753be9cdb", "https://ms.immowelt.org/f6511334-9f04-476c-9659-9f19a5df115f/ff04d8f5-f770-493d-9394-6ac1a456d4ef", "https://ms.immowelt.org/733f5f85-bc20-4e60-ba25-388eeb6563cf/4094751f-b73c-432d-b6b4-6d68ba45d6d9", "https://ms.immowelt.org/05e1b42e-75a4-4206-aaad-48ffa57f162d/a3aafbff-20b6-4c17-a8a1-b916eb14b8aa", "https://ms.immowelt.org/1233e75d-2ab4-4291-8b67-e87c5a4898f1/6153dd66-9325-4066-80d3-ed8642487cd8", "https://ms.immowelt.org/99f6825d-9789-4ae1-9a78-4e6acb5853a7/f727c1c7-69a0-420d-adf8-9119f5849a16", "https://ms.immowelt.org/19d94014-cd12-4f9a-81a5-8f9745f63b90/48988be8-85bb-4980-a25a-276af2606ac6", "https://ms.immowelt.org/f351ce35-7e50-4939-b806-4f6dc375cc86/84c997d9-1332-4173-9248-fb7b75a10943", "https://ms.immowelt.org/cdd250a7-47f6-4535-ac59-6ea51157c95e/bed7b410-ef26-42d6-a562-595eafba5999", "https://ms.immowelt.org/644f0235-e6ba-482b-bb26-2fea622cd4a1/6d2746f3-ea97-4996-8617-e82aeced34e0", "https://ms.immowelt.org/0174f587-e7b3-4c39-8603-c1d8465305ec/508d427a-f8c5-4d05-bd55-06ee858889be", "https://ms.immowelt.org/e3dbe0a9-b856-43a6-97a0-ca238574c6f8/f20530d2-b140-4eb5-b229-ad329853d7f3"]</t>
+          <t>["https://ms.immowelt.org/ea4c2f0b-394f-42bd-abb7-a4b389c1d47d/ff497d04-808a-4337-a3e3-2cf5516bba7a", "https://ms.immowelt.org/366939ca-53fe-483d-98bf-f2ee6195dfc0/05b63755-5ed7-47a4-8dff-3f7fe160860a", "https://ms.immowelt.org/985ea057-3cd8-4f50-902d-75b4fdfd5d80/985af61d-8d10-46f1-8973-3ca9e3128892", "https://ms.immowelt.org/d60ab3e7-f8b1-4a56-9fe7-cb3d6b251fde/39119cc8-1171-4282-96e2-7cd5703d138e", "https://ms.immowelt.org/74ddb531-c432-441d-a6d9-f10cae01c815/df9fece6-1aa2-4522-9459-fe31c0fdf7be", "https://ms.immowelt.org/90f66d94-cf4f-4975-a300-fd5fdaa057dd/e4aca2a3-3782-48dc-8ebd-01cb1c5d26af", "https://ms.immowelt.org/ed2b2673-027a-4c7d-b469-2d88936aa895/c5525e35-fb10-4c05-a6b3-3903c73a1cd5", "https://ms.immowelt.org/f444609a-1c93-44de-bc86-3bb35bbe475e/7d9d6f63-18c3-4a57-b866-759c4f01d683", "https://ms.immowelt.org/12808aff-d0d3-4ce7-90a1-158e4dc99040/43dea702-8f33-4bc8-b0cf-8fae834b567c", "https://ms.immowelt.org/8bff2dd9-2249-43dc-900d-40ea65a23212/251524b5-e8c7-49a9-b995-00de0bb85ffe", "https://ms.immowelt.org/64561934-cc49-4074-b25f-6a6806f1cdd0/7971880f-b488-43df-a3e6-ee4aec51ae9a", "https://ms.immowelt.org/3ed2c2ec-6223-4e04-99ae-df359a6754c4/1aa90e24-28b3-4bc9-99dd-a8b18c2af3bb", "https://ms.immowelt.org/43927a50-d329-414c-b0f5-ca4f4cd70c2d/5a27d374-b073-4a66-9c71-23db210c7bc5", "https://ms.immowelt.org/49b01679-3040-4664-8c50-17d1e81e7a90/6a4baaaa-1b65-421e-8e20-4ce145d2b6c7", "https://ms.immowelt.org/5be96dee-5832-445f-8d62-264839c37343/d5b9dc02-555e-49f4-8a72-b5fdde07f935", "https://ms.immowelt.org/6bc5b40d-e97f-4fba-8c44-222645648458/42d69790-b9a5-40e9-8b43-b7529c138a8a", "https://ms.immowelt.org/60dec9ad-25a6-4596-8475-c20d723fe05a/3ddd5c6e-9448-40f9-be5d-4065443127a7", "https://ms.immowelt.org/e105af84-a45f-4370-b285-74bee821da08/e6dc5c1d-ad19-4038-ada0-3eecaf37fcc2", "https://ms.immowelt.org/927559a3-db2e-471f-8de6-33b5b3a3a96a/45e4cf6e-8048-4fa0-a7e4-5494ea0506a4", "https://ms.immowelt.org/3b19e507-1683-467a-bcb1-c424c524ca2f/dc5a81f4-1daf-4f1f-b9c9-c23df92dcb8b", "https://ms.immowelt.org/f136ae8b-8c04-4e1f-be49-5859e9cc12aa/45b449b8-53d3-4136-a7a7-bb156ed3b3c2"]</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>{"companyName": "hv Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Wilhelm-Dahl-Str. 9"}, "profilePicture": "https://filestore.immowelt.de/ProfilBilder/150_98e1685eae1346a2a90a2847489951ff.jpg", "salutation": "Herr", "firstName": "Hartwig", "lastName": "Vogel", "mobile": "0175-5994950", "phone": "0931/45466333"}</t>
+          <t>{"companyName": "M &amp;a; M Bauprojektierung  und Vertrieb GmbH", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Franz-Brentano-Stra\u00dfe 2"}, "salutation": "Herr", "firstName": "Sascha", "lastName": "Mannel"}</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE", "basicObjectPricEur": 1700, "basicLivingSpace": 153.3, "basicRooms": 3, "basicConstructionYear": 1998, "basicCity": "W\u00fcrzburg", "basicStreet": "Gartenstra\u00dfe 9", "basicUrl": "https://www.immowelt.de/expose/2almm5r", "basicContactPhone": "0931/45466333", "basicContactMobile": "0175-5994950"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "6er-Studenten-Wohngemeinschaft - Zi.Nr. 4", "basicObjectPricEur": 350, "basicRooms": 1, "basicConstructionYear": 1972, "basicCity": "W\u00fcrzburg", "basicStreet": "Amalienstr. 6", "basicUrl": "https://www.immowelt.de/expose/2acjp5u"}</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2upu84s"</t>
+          <t>"https://www.immowelt.de/expose/2af545v"</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1802,12 +1802,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
+          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Exklusive Penthouse-Maisonette-Wohnung"</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>3030.93</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1817,54 +1817,54 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>178.29</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
+          <t>["barriefrei", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3030.93, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 360, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
+          <t>["https://ms.immowelt.org/2b7c4c91-7fac-4ddb-a032-3a51184dbb59/8f34d9b5-fec8-4e21-99c7-6f7a2921d4d1", "https://ms.immowelt.org/61a862a4-1bd5-4769-abb9-5e1d7113f8bc/88d5b2b5-7ef0-4388-8eb9-b7042670aee5", "https://ms.immowelt.org/37c438a9-8ae7-4d42-8006-bc3a55265670/12a6e3ea-2554-4920-bec1-7d536539c02d", "https://ms.immowelt.org/49abcb3b-4395-4691-8e92-b525edda30d4/f7c44e0e-0db0-456e-8cb8-845d816e37ec", "https://ms.immowelt.org/ce95a7e7-0ad6-4282-8ca2-5ce205488707/dbfb5e54-2bfb-4d01-91ec-1ca118a3a922", "https://ms.immowelt.org/b3cc6d40-e3b5-407e-ae5e-be0785a5a218/686cb7a1-8858-4011-a5e0-a8fd590fe4e6", "https://ms.immowelt.org/424d3898-11a5-419c-a472-b6bb5eed3e76/e7d72403-5394-43c9-a960-10468f29d064", "https://ms.immowelt.org/19d6858d-2cb5-437d-8cdb-6fb75d54c5e4/8e3114ed-77c5-47c0-8dce-725b44e8785c", "https://ms.immowelt.org/f536fdcb-a38d-4b90-beab-277e244cf6a7/ce23ee46-5ee8-4496-b672-c3ea031e92ac", "https://ms.immowelt.org/933295a3-d9da-4860-ad95-06490c6fddf4/182424c9-5902-4b40-be26-512097b49929", "https://ms.immowelt.org/a77d50f5-f8e0-4928-bcdc-2fa7c6e36e7d/05824030-0135-4ec2-93dc-52a0bf313587", "https://ms.immowelt.org/dbfe5771-25b1-460e-a2dd-140a19fae05f/4dd99d70-1f73-40c8-aab7-49051e0e90ec", "https://ms.immowelt.org/9689e92f-fdee-4ff1-99c1-89400857e515/a07a7b18-a41e-45a3-9fe1-f64211e577cd", "https://ms.immowelt.org/c3fdabd3-6c7c-4da9-9941-17117007bd14/16545b70-e49d-4309-85c5-a84123f7c8a2", "https://ms.immowelt.org/ec2b29d2-9e49-4ccb-965f-e26d155e848a/1c4de27d-2032-41cc-a466-04b10ad4f27d", "https://ms.immowelt.org/c2913eaa-8856-44c1-901b-0ae4b9a9ffa2/387a24b5-3c67-4740-ac58-0de078b68ff8", "https://ms.immowelt.org/81e05570-c572-4168-acf8-500cd9f74a65/796a2975-473d-4971-bd18-d2765832485e", "https://ms.immowelt.org/2c90ddab-a797-471f-a2aa-53b9ac172a1c/43c8617b-2da6-4fae-99be-395aaf2774e3", "https://ms.immowelt.org/24b3e778-e131-4042-ba05-7b63afaf1ce0/b0dfb227-b3fc-4605-b1c3-58573b4f24d1", "https://ms.immowelt.org/1d31929b-a5c2-410f-9bef-afc44f5e68c1/bc515335-0e9c-453b-bfcf-ae09a83fd65d", "https://ms.immowelt.org/d6e04616-c252-4d95-8d95-9d504b0fb3f4/07aa7bfb-71ab-4b13-bba6-99ba35097b80"]</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Jendrzej", "phone": "0931/382-7701"}</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Exklusive Penthouse-Maisonette-Wohnung", "basicObjectPricEur": 3030.93, "basicLivingSpace": 178.29, "basicRooms": 5, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2af545v", "basicContactPhone": "0931/382-7701"}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
+          <t>"https://www.immowelt.de/expose/2auvq5u"</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1874,12 +1874,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
+          <t>"M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland"</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>649</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1889,47 +1889,47 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>21</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>["WANNE"]</t>
+          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert"]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.298,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 649, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
+          <t>["https://ms.immowelt.org/231cfc3d-f3ec-4eea-b3d8-d3f27a286b40/3058b16a-8a05-47d3-8512-63886059b512", "https://ms.immowelt.org/2660e3fb-eb65-4bd8-8844-5b667e3b062d/adc4fedc-4170-4ee1-a6c7-2d63780cfd0e", "https://ms.immowelt.org/dcb8e961-2856-45f0-8df9-13b8f9f4cadd/19a60ab9-5a93-4d74-be47-9ec0408e6e89", "https://ms.immowelt.org/4f79f7ef-0e51-49b2-ab74-287b9836cc3d/83e20f80-c025-439d-aace-e927f852a97b", "https://ms.immowelt.org/08d42db4-e036-4159-8269-dcb7bd5631a1/9cf8e0c1-3269-44d4-986b-bd625c8101ae", "https://ms.immowelt.org/2f13d3b5-8df8-4ac9-95af-5ba7f89e3dc1/d94afc12-acd9-4275-be9b-8fae1c182d5f", "https://ms.immowelt.org/0308a23f-5076-4db4-9f3b-c6024f595313/7143a6d8-6101-40b4-a19f-aba8e2a5a145", "https://ms.immowelt.org/814288ea-742a-4172-affa-ff8454f45731/e6ca30e2-64eb-4733-9789-940742a1d5d5", "https://ms.immowelt.org/ba83b81a-c23e-4eb8-8f5f-47a680847e30/7b794550-2c44-4fa8-9bb7-a6f8c6820a8a"]</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
+          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 649, "basicLivingSpace": 21, "basicRooms": 1, "basicConstructionYear": 2015, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2auvq5u", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Progress Bar added + MLFlow runs
</commit_message>
<xml_diff>
--- a/immowelt_price_guide/data/retrain_train_data.xlsx
+++ b/immowelt_price_guide/data/retrain_train_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,11 +484,6 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>ContactData</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
           <t>BasicInfo</t>
         </is>
       </c>
@@ -496,7 +491,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2am365w"</t>
+          <t>"https://www.immowelt.de/expose/2a4kg5w"</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -506,7 +501,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"Helle Wohnung mit Balkon in der vorderen Sanderau!"</t>
+          <t>"2-Zi. Penthouse Wohnung  mit gr. Terrasse, teilm\u00f6bliert, N\u00e4he Uniklinik"</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -521,7 +516,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>47</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -531,44 +526,39 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1955</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>["Kelleranteil", "GEPFLEGT", "FERN", "kable_sat_tv", "Balkon"]</t>
+          <t>["Neubau", "Kelleranteil", "GAS", "Zentralheizung", "moebliert", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "LocationId": 496022, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Lindleinsm\u00fchle", "ZipCode": "97078", "LocationId": 496017, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.400,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 190, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 890, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1500", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Lindleinsm\u00fchle)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-lindleinsmuehle/mietspiegel"}}, "DataTable": [{"NumberValue": 700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 900, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/0cd8c2fc-f0f8-4803-b570-0bc0474a7ed0/ff573215-5a42-4351-ba40-cfa78f0e290f", "https://ms.immowelt.org/9f20ac68-d479-4226-9c79-53570da7eb1d/e2de2ea2-5dcd-44f2-94d5-5e6076766679", "https://ms.immowelt.org/65a23389-315b-4e17-9a6f-c8bcf8e849a7/ef1d6fb2-36ee-4c22-9b98-1f57d5548397", "https://ms.immowelt.org/57d6c377-cfc6-48d1-a1d5-1088cf6393f3/bbd12d5a-7478-4c07-bfbf-ce2e86b907b4", "https://ms.immowelt.org/0a903ef0-4c0b-431f-af10-207debb8ec0e/ced5048e-e943-4b27-acce-5dba9b2424d9", "https://ms.immowelt.org/c5093796-6848-4a03-8695-1e10dfd39fb2/ee4c2860-ca11-43ee-b24a-c8691f01283c"]</t>
+          <t>["https://ms.immowelt.org/5ffec635-8f46-4cc1-aadb-8b583ac94f49/a055949a-2702-4368-b5b3-7b0ed426b642", "https://ms.immowelt.org/8908f348-9991-4a07-ad66-d7d75614e10a/fca9e8be-88e9-418f-a5eb-9e0d5767a5f4", "https://ms.immowelt.org/cc8d5f7e-0ed9-47a3-818b-45790a8111fc/1ff9a9de-b0c2-4a71-935d-2fd2d9164ad1", "https://ms.immowelt.org/e595bf82-bf35-4dea-bb76-166a24244d92/420389cc-e1aa-4a32-94b8-9d099fca203b", "https://ms.immowelt.org/2512e689-4ae0-4ff9-9611-9f151ac18678/c4e6c45b-c697-41d7-a51f-d244d8f1a417", "https://ms.immowelt.org/e0483e5d-da13-4926-a03f-c238c4a327ae/737d7425-941f-4ec9-a90e-14f51213a74f", "https://ms.immowelt.org/23fe53b7-3d5a-4509-a222-5cb8ed3d516c/a46ccbc0-6aef-4e2f-ac21-6d245e72052d", "https://ms.immowelt.org/349313e4-73e0-40b7-b119-9fe817365e7a/7f23958c-275b-4a0e-8d30-ad6e79f317f7", "https://ms.immowelt.org/ac9b1a48-16e2-4119-98ba-9a1a890ff38b/c3716b49-d728-4b6a-900b-7d66e9cd4354", "https://ms.immowelt.org/e3084b71-0919-4d54-96d4-4d35ce184a9c/c4edd6a6-581b-4387-81e6-1df5e276dda7", "https://ms.immowelt.org/fa543343-fde7-4b91-b370-eee9cd1e0f90/62763f8c-bf88-4f8a-bbfc-b721085c2412", "https://ms.immowelt.org/2a737240-80f0-4710-a8f3-7c4f1c3f6233/08bf7007-717d-4120-b7cb-50bf91a1393b", "https://ms.immowelt.org/727ce8f8-3e8b-4da9-95ec-b855705005c5/07256d94-2372-4172-b756-d7101c994e5e"]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>{"companyName": "arndt immobilien GmbH", "address": {"city": "Rimpar", "zipCode": "97222", "street": "Friedrich-Ebert-Str. 6"}, "salutation": "Frau", "firstName": "Brigitte", "lastName": "Lienert", "phone": "0931 46079392"}</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Helle Wohnung mit Balkon in der vorderen Sanderau!", "basicObjectPricEur": 700, "basicLivingSpace": 58, "basicRooms": 2, "basicConstructionYear": 1955, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2am365w", "basicContactPhone": "0931 46079392"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "2-Zi. Penthouse Wohnung  mit gr. Terrasse, teilm\u00f6bliert, N\u00e4he Uniklinik", "basicObjectPricEur": 700, "basicLivingSpace": 47, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a4kg5w", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a5ll5v"</t>
+          <t>"https://www.immowelt.de/expose/2am365w"</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -578,12 +568,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Exklusive 4-Zimmer-Neubauwohnung W\u00fcrzburg-Frauenland *Gartenstadt Keesburg*"</t>
+          <t>"Helle Wohnung mit Balkon in der vorderen Sanderau!"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1483.93</t>
+          <t>700</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,54 +583,49 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>102.34</t>
+          <t>58</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1955</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>["Neubau", "gaestewc", "DUSCHE", "Kelleranteil", "Personenaufzug", "Erdgeschoss", "PELLET", "Zentralheizung", "DSL", "PARKETT", "FLIESEN", "frei", "abstellraum", "Tiefgarage", "REINIGUNG", "Loggia", "kable_sat_tv", "Kunststofffenster"]</t>
+          <t>["Kelleranteil", "GEPFLEGT", "FERN", "kable_sat_tv", "Balkon"]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Hans-L\u00f6ffler-Stra\u00dfe 3", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "LocationId": 496022, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1483.93, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 290, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.400,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 190, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 890, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/46db7f7a-e5d8-4eb4-a01b-a2d4e62ab2be/bb78636c-2f3f-4c2e-a53b-ef1fa9683a15", "https://ms.immowelt.org/b16389b6-eb92-42af-8130-0a76d6025358/fce845ed-0986-423b-8c1e-afd09a953917"]</t>
+          <t>["https://ms.immowelt.org/0cd8c2fc-f0f8-4803-b570-0bc0474a7ed0/ff573215-5a42-4351-ba40-cfa78f0e290f", "https://ms.immowelt.org/9f20ac68-d479-4226-9c79-53570da7eb1d/e2de2ea2-5dcd-44f2-94d5-5e6076766679", "https://ms.immowelt.org/65a23389-315b-4e17-9a6f-c8bcf8e849a7/ef1d6fb2-36ee-4c22-9b98-1f57d5548397", "https://ms.immowelt.org/57d6c377-cfc6-48d1-a1d5-1088cf6393f3/bbd12d5a-7478-4c07-bfbf-ce2e86b907b4", "https://ms.immowelt.org/0a903ef0-4c0b-431f-af10-207debb8ec0e/ced5048e-e943-4b27-acce-5dba9b2424d9", "https://ms.immowelt.org/c5093796-6848-4a03-8695-1e10dfd39fb2/ee4c2860-ca11-43ee-b24a-c8691f01283c"]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Jendrzej", "phone": "0931/382-7701"}</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Exklusive 4-Zimmer-Neubauwohnung W\u00fcrzburg-Frauenland *Gartenstadt Keesburg*", "basicObjectPricEur": 1483.93, "basicLivingSpace": 102.34, "basicRooms": 4, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Hans-L\u00f6ffler-Stra\u00dfe 3", "basicUrl": "https://www.immowelt.de/expose/2a5ll5v", "basicContactPhone": "0931/382-7701"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Helle Wohnung mit Balkon in der vorderen Sanderau!", "basicObjectPricEur": 700, "basicLivingSpace": 58, "basicRooms": 2, "basicConstructionYear": 1955, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2am365w", "basicContactPhone": "0931 46079392"}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ayb45v"</t>
+          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -650,12 +635,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Gro\u00dfz\u00fcgige 6-Zimmer-Maisonette-Wohnung"</t>
+          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3601.44</t>
+          <t>580</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -665,54 +650,49 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>225.09</t>
+          <t>44</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>["WANNE", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Balkon", "Kunststofffenster"]</t>
+          <t>["WANNE"]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3601.44, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 460, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/b888654a-7be0-4b1f-bb51-2d8dca6a1aa1/5dc0db39-67ad-4630-8a84-004692c1c198", "https://ms.immowelt.org/4cb98d26-30d4-40dd-9345-c05636fc3d6e/3d269755-d356-448a-a4e4-c9c9225867b0", "https://ms.immowelt.org/71ab24a9-6d26-4798-959a-526196ab2526/2338dbdc-85e0-452f-bbf4-cbd765176db2", "https://ms.immowelt.org/e212abae-27ab-4901-ad56-4abbf1ab429a/076c61fa-ae56-43bd-90cc-3d4a1f246534", "https://ms.immowelt.org/45fda28f-bd4b-477c-8e5b-025d3035fc24/25270c0c-e6f1-42be-9bc6-154afc390bde", "https://ms.immowelt.org/250e735d-28bf-4e41-a26e-10bdcc174a72/9ffa4901-709f-4a22-bcf8-4026af4845a8", "https://ms.immowelt.org/47738d72-90e1-400f-8f26-b0c89e0a04d4/b2671ee7-2150-4931-ae87-848ca314834d", "https://ms.immowelt.org/09239b5c-efed-4862-9be0-12284713015c/c50d605a-b30b-4c1e-b8c7-c377d0105c47", "https://ms.immowelt.org/32be8996-eac0-4fda-8211-2d8fadd6467a/c5cb6c3d-45d4-45e6-8603-f3cc8967b34e", "https://ms.immowelt.org/de7996d0-a07e-44a3-a014-b9f228303c3b/f4242060-e83a-4836-b64b-41645c5c5e94", "https://ms.immowelt.org/d9382006-8b3f-46eb-802b-250a8fca3f96/03f39cab-4da2-4c36-80c1-23a7fbd309fe", "https://ms.immowelt.org/36af7108-dfdd-4ff3-ab8b-6e92d3508062/2f20f749-7813-4534-bde5-1a624ad88952", "https://ms.immowelt.org/ba912dea-da2a-4abd-add2-64d03801c9f2/0f910eff-7ebe-4154-9f66-0556d0a42237", "https://ms.immowelt.org/469127b9-c85a-4e77-a7fa-af7365f65cc3/9cd962ef-da29-4690-9168-413036c7882b", "https://ms.immowelt.org/0341b685-a77c-4318-bf97-0b0facbf1946/c0c91076-cd90-41c2-8e29-c3d9b6bc4e76", "https://ms.immowelt.org/349ba8bc-380d-425c-9404-fe30348c76fb/be7df368-083b-4bf6-bb15-c9ee4809e9b4", "https://ms.immowelt.org/769d004b-9208-4258-b045-f78d35bbe304/cab7c6e2-a6fe-44e9-b980-49f912c4dc33", "https://ms.immowelt.org/32a4701e-f4a1-4e08-ac43-7f82a0871c0e/05462d50-f4b2-41fb-94fc-03251da46a31", "https://ms.immowelt.org/c3b62a14-8ad0-4bc1-ad12-407a7b7d45c1/1e082fb8-309d-48fd-9675-1e19df39056b"]</t>
+          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Frau", "firstName": "Heike", "lastName": "Fabiunke", "phone": "0931/382-7708"}</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Gro\u00dfz\u00fcgige 6-Zimmer-Maisonette-Wohnung", "basicObjectPricEur": 3601.44, "basicLivingSpace": 225.09, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2ayb45v", "basicContactPhone": "0931/382-7708"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aeal5v"</t>
+          <t>"https://www.immowelt.de/expose/2affg5v"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -722,12 +702,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"**Erstbezug** Renoviertes Studenten-Apartment nahe Uni Hubland und Wittelsbacherplatz"</t>
+          <t>"M\u00f6blierte Wohnung in W\u00fcrzburg/Mainviertel"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>415</t>
+          <t>1125</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -737,54 +717,49 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>60</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>1957</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>["DUSCHE", "FENSTER", "Souterrain", "GAS", "Zentralheizung", "LAMINAT", "FLIESEN", "frei", "Einbauk\u00fcche", "Kunststofffenster"]</t>
+          <t>["WANNE", "Etagenheizung", "moebliert", "Einbauk\u00fcche"]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Rottendorferstra\u00dfe 55", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97082", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "830", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 415, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 145, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2.250,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1125, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/a3c1d1a9-92f0-4260-b2b3-41eb1b7cb966/c490aefe-bdcb-4b73-9783-a0bcc158c257", "https://ms.immowelt.org/b05abc2c-f624-4093-86a5-80f153fa6197/05af8f24-b7e4-4ba5-872c-39eed41b4cb5", "https://ms.immowelt.org/5be4bd8f-231a-44d8-8f0b-608a4f6581bd/0af81664-7d97-498f-8adf-3b5b5fe348ae", "https://ms.immowelt.org/725fb4fb-900c-4cd8-9554-dd83fc7bd725/99474ade-0e13-4d47-bf95-373cf4af43ec", "https://ms.immowelt.org/a0bb9c06-d60a-40e4-9521-94d9c183a14d/93799d3a-657d-4385-b487-2691349273e9", "https://ms.immowelt.org/3b4d1b7b-a5fe-4a37-b98d-6fc308d03c5b/c80e2b27-9270-47ef-b292-eb1efd72ee07"]</t>
+          <t>["https://ms.immowelt.org/ed2e6e9a-a8cf-4e9e-89c9-92ebe0bd9ab9/3c8c330e-15e6-439e-be44-6f02de4b9dd5", "https://ms.immowelt.org/e963b58b-6a58-4830-8e37-e9e446a7ca40/edda2664-fb0a-48dc-bfe4-3b20c61c8b1d", "https://ms.immowelt.org/6945f917-297e-4dfb-b166-4245a2333e2c/5a890870-d05f-4063-b0e5-63ad31ca7572", "https://ms.immowelt.org/ffa99189-2ca2-46fb-aa14-f6fda02818ae/6a859704-19f9-4907-92f9-a5b7fcbe4248", "https://ms.immowelt.org/86e1504e-0c46-4800-a6e0-cf24601a2518/bf8eec93-53d3-4368-82bc-ca50c66a45a1", "https://ms.immowelt.org/f15519e3-ee04-4739-b40a-ce0f84fb29ff/2c2c7101-3482-420d-826e-9efd57863f1e", "https://ms.immowelt.org/54ea5d30-e104-4f39-8a41-429b5961bbd1/55bee8cc-3633-4bce-9b47-af1971f0523b", "https://ms.immowelt.org/e88c0a6a-0da8-4b88-8865-a9f37cbd0e2d/9452b370-8d6d-4324-8a35-57b8a433c48a"]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>{"companyName": "M &amp;a; M Bauprojektierung  und Vertrieb GmbH", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Franz-Brentano-Stra\u00dfe 2"}, "salutation": "Frau", "firstName": "Selina", "lastName": "Wiesner", "mobile": "+49 176 21469496"}</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "**Erstbezug** Renoviertes Studenten-Apartment nahe Uni Hubland und Wittelsbacherplatz", "basicObjectPricEur": 415, "basicLivingSpace": 26, "basicRooms": 1, "basicConstructionYear": 1950, "basicCity": "W\u00fcrzburg", "basicStreet": "Rottendorferstra\u00dfe 55", "basicUrl": "https://www.immowelt.de/expose/2aeal5v", "basicContactMobile": "+49 176 21469496"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6blierte Wohnung in W\u00fcrzburg/Mainviertel", "basicObjectPricEur": 1125, "basicLivingSpace": 60, "basicRooms": 2, "basicConstructionYear": 1957, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2affg5v", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a4kg5w"</t>
+          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -794,12 +769,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"2-Zi. Penthouse Wohnung  mit gr. Terrasse, teilm\u00f6bliert, N\u00e4he Uniklinik"</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>420</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -809,54 +784,49 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>["Neubau", "Kelleranteil", "GAS", "Zentralheizung", "moebliert", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["GAS"]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Lindleinsm\u00fchle", "ZipCode": "97078", "LocationId": 496017, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1500", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Lindleinsm\u00fchle)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-lindleinsmuehle/mietspiegel"}}, "DataTable": [{"NumberValue": 700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 900, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/5ffec635-8f46-4cc1-aadb-8b583ac94f49/a055949a-2702-4368-b5b3-7b0ed426b642", "https://ms.immowelt.org/8908f348-9991-4a07-ad66-d7d75614e10a/fca9e8be-88e9-418f-a5eb-9e0d5767a5f4", "https://ms.immowelt.org/cc8d5f7e-0ed9-47a3-818b-45790a8111fc/1ff9a9de-b0c2-4a71-935d-2fd2d9164ad1", "https://ms.immowelt.org/e595bf82-bf35-4dea-bb76-166a24244d92/420389cc-e1aa-4a32-94b8-9d099fca203b", "https://ms.immowelt.org/2512e689-4ae0-4ff9-9611-9f151ac18678/c4e6c45b-c697-41d7-a51f-d244d8f1a417", "https://ms.immowelt.org/e0483e5d-da13-4926-a03f-c238c4a327ae/737d7425-941f-4ec9-a90e-14f51213a74f", "https://ms.immowelt.org/23fe53b7-3d5a-4509-a222-5cb8ed3d516c/a46ccbc0-6aef-4e2f-ac21-6d245e72052d", "https://ms.immowelt.org/349313e4-73e0-40b7-b119-9fe817365e7a/7f23958c-275b-4a0e-8d30-ad6e79f317f7", "https://ms.immowelt.org/ac9b1a48-16e2-4119-98ba-9a1a890ff38b/c3716b49-d728-4b6a-900b-7d66e9cd4354", "https://ms.immowelt.org/e3084b71-0919-4d54-96d4-4d35ce184a9c/c4edd6a6-581b-4387-81e6-1df5e276dda7", "https://ms.immowelt.org/fa543343-fde7-4b91-b370-eee9cd1e0f90/62763f8c-bf88-4f8a-bbfc-b721085c2412", "https://ms.immowelt.org/2a737240-80f0-4710-a8f3-7c4f1c3f6233/08bf7007-717d-4120-b7cb-50bf91a1393b", "https://ms.immowelt.org/727ce8f8-3e8b-4da9-95ec-b855705005c5/07256d94-2372-4172-b756-d7101c994e5e"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "2-Zi. Penthouse Wohnung  mit gr. Terrasse, teilm\u00f6bliert, N\u00e4he Uniklinik", "basicObjectPricEur": 700, "basicLivingSpace": 47, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a4kg5w", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2affg5v"</t>
+          <t>"https://www.immowelt.de/expose/2a54x5v"</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -866,12 +836,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"M\u00f6blierte Wohnung in W\u00fcrzburg/Mainviertel"</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1125</t>
+          <t>900</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -881,54 +851,49 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>80</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1957</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>["WANNE", "Etagenheizung", "moebliert", "Einbauk\u00fcche"]</t>
+          <t>["FENSTER", "Kelleranteil", "Personenaufzug", "GAS", "Zentralheizung"]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97082", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Rottenbauer", "ZipCode": "97084", "LocationId": 496020, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2.250,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1125, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1800", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Rottenbauer)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-rottenbauer/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1100, "Unit": "EUR"}, {"NumberValue": 20, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/ed2e6e9a-a8cf-4e9e-89c9-92ebe0bd9ab9/3c8c330e-15e6-439e-be44-6f02de4b9dd5", "https://ms.immowelt.org/e963b58b-6a58-4830-8e37-e9e446a7ca40/edda2664-fb0a-48dc-bfe4-3b20c61c8b1d", "https://ms.immowelt.org/6945f917-297e-4dfb-b166-4245a2333e2c/5a890870-d05f-4063-b0e5-63ad31ca7572", "https://ms.immowelt.org/ffa99189-2ca2-46fb-aa14-f6fda02818ae/6a859704-19f9-4907-92f9-a5b7fcbe4248", "https://ms.immowelt.org/86e1504e-0c46-4800-a6e0-cf24601a2518/bf8eec93-53d3-4368-82bc-ca50c66a45a1", "https://ms.immowelt.org/f15519e3-ee04-4739-b40a-ce0f84fb29ff/2c2c7101-3482-420d-826e-9efd57863f1e", "https://ms.immowelt.org/54ea5d30-e104-4f39-8a41-429b5961bbd1/55bee8cc-3633-4bce-9b47-af1971f0523b", "https://ms.immowelt.org/e88c0a6a-0da8-4b88-8865-a9f37cbd0e2d/9452b370-8d6d-4324-8a35-57b8a433c48a"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6blierte Wohnung in W\u00fcrzburg/Mainviertel", "basicObjectPricEur": 1125, "basicLivingSpace": 60, "basicRooms": 2, "basicConstructionYear": 1957, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2affg5v", "basicContactPhone": "+49 931 416616"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 900, "basicLivingSpace": 80, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a54x5v"}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a54x5v"</t>
+          <t>"https://www.immowelt.de/expose/2a5ll5v"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -938,12 +903,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"Exklusive 4-Zimmer-Neubauwohnung W\u00fcrzburg-Frauenland *Gartenstadt Keesburg*"</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>1483.93</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -953,54 +918,49 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>102.34</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>["FENSTER", "Kelleranteil", "Personenaufzug", "GAS", "Zentralheizung"]</t>
+          <t>["Neubau", "gaestewc", "DUSCHE", "Kelleranteil", "Personenaufzug", "Erdgeschoss", "PELLET", "Zentralheizung", "DSL", "PARKETT", "FLIESEN", "frei", "abstellraum", "Tiefgarage", "REINIGUNG", "Loggia", "kable_sat_tv", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Rottenbauer", "ZipCode": "97084", "LocationId": 496020, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Hans-L\u00f6ffler-Stra\u00dfe 3", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1800", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Rottenbauer)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-rottenbauer/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1100, "Unit": "EUR"}, {"NumberValue": 20, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1483.93, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 290, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["https://ms.immowelt.org/46db7f7a-e5d8-4eb4-a01b-a2d4e62ab2be/bb78636c-2f3f-4c2e-a53b-ef1fa9683a15", "https://ms.immowelt.org/b16389b6-eb92-42af-8130-0a76d6025358/fce845ed-0986-423b-8c1e-afd09a953917"]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>{"salutation": "Frau", "firstName": "Astrid", "lastName": "Leis"}</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 900, "basicLivingSpace": 80, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a54x5v"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Exklusive 4-Zimmer-Neubauwohnung W\u00fcrzburg-Frauenland *Gartenstadt Keesburg*", "basicObjectPricEur": 1483.93, "basicLivingSpace": 102.34, "basicRooms": 4, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Hans-L\u00f6ffler-Stra\u00dfe 3", "basicUrl": "https://www.immowelt.de/expose/2a5ll5v", "basicContactPhone": "0931/382-7701"}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
+          <t>"https://www.immowelt.de/expose/2abty5v"</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1010,12 +970,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"[TAUSCHWOHNUNG] Wundersch\u00f6ne helle Altbauwohnung"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>430</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1025,12 +985,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>64</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1040,7 +1000,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>["GAS"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1050,29 +1010,24 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 430, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 115, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["https://ms.immowelt.org/7a4af935-fdca-42b8-b470-a905b68d671e/717dc8fc-8461-4d19-89e3-3eaf6c5bfb76"]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "[TAUSCHWOHNUNG] Wundersch\u00f6ne helle Altbauwohnung", "basicObjectPricEur": 430, "basicLivingSpace": 64, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2abty5v", "basicContactPhone": "+4922892939484"}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2av845v"</t>
+          <t>"https://www.immowelt.de/expose/2aeal5v"</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1082,12 +1037,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Helle 3-Zimmer-Wohnung mit Balkon"</t>
+          <t>"**Erstbezug** Renoviertes Studenten-Apartment nahe Uni Hubland und Wittelsbacherplatz"</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1797.71</t>
+          <t>415</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1097,54 +1052,49 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>123.98</t>
+          <t>26</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1950</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "DUSCHE", "Kelleranteil", "Personenaufzug", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Balkon", "Kunststofffenster"]</t>
+          <t>["DUSCHE", "FENSTER", "Souterrain", "GAS", "Zentralheizung", "LAMINAT", "FLIESEN", "frei", "Einbauk\u00fcche", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Rottendorferstra\u00dfe 55", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 1797.71, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 250, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "830", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 415, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 145, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/34aad469-3611-425d-9832-c02c7060cb23/77ba9d6f-e612-4962-9317-bd0107dc25f7", "https://ms.immowelt.org/8ea07a0f-c3a2-4e3e-a9d2-fe6544358d93/58dbc143-5e69-4062-9eae-b767cf0c69b1", "https://ms.immowelt.org/6b6cd2cc-a04d-480c-949a-1a21bbd7e1d4/51babd4b-8fbc-456a-862b-c4ebde7dc41a", "https://ms.immowelt.org/a8f09c5d-403e-4528-a15f-17ef6819f51c/15cf94e1-0865-4970-bdbc-7eeb2e4e321a", "https://ms.immowelt.org/a74342e9-df14-4a0d-b4c6-600423e5e886/caed2534-21fc-4d11-981c-a2164e56802b", "https://ms.immowelt.org/57b465e5-f400-4f58-8856-6a92ccb5dc5c/e24df36d-9d71-44a2-bd39-c0146b4df941", "https://ms.immowelt.org/4d380785-997d-4deb-b741-8c14d08622b6/d794011b-6b71-4e97-adb0-c319032680b3", "https://ms.immowelt.org/a1aeaa9b-89a7-4a5b-b3ed-598756319607/14a91c1a-5084-49dc-b75d-74d20228a8f0", "https://ms.immowelt.org/af2232f0-1ef7-4481-801f-2a5ff59e0092/96a901ff-03de-431d-886e-d860ac84fbc4", "https://ms.immowelt.org/eb83b1d9-acf0-4e74-b0b3-5fa3fcc1ca01/705ad620-364a-4237-968f-e9f4e0c3eb36", "https://ms.immowelt.org/b34e24ec-eac1-4eae-b4db-e1f386853cb1/292b937e-2528-4472-8123-fa7a878ef84b", "https://ms.immowelt.org/4111770b-ae7b-4dce-b625-f990d3c5ba1e/b7539eac-4bf3-4d62-ab60-f12720be1758", "https://ms.immowelt.org/73dc46c5-cb67-4432-b97f-e11d22268b50/6613c506-3bb4-4e53-a0ac-d3296fe50f9c", "https://ms.immowelt.org/d8083607-cc91-46ee-92df-9a6f4eed9d3b/59f57e14-612a-4c44-8a58-7436d9771597"]</t>
+          <t>["https://ms.immowelt.org/a3c1d1a9-92f0-4260-b2b3-41eb1b7cb966/c490aefe-bdcb-4b73-9783-a0bcc158c257", "https://ms.immowelt.org/b05abc2c-f624-4093-86a5-80f153fa6197/05af8f24-b7e4-4ba5-872c-39eed41b4cb5", "https://ms.immowelt.org/5be4bd8f-231a-44d8-8f0b-608a4f6581bd/0af81664-7d97-498f-8adf-3b5b5fe348ae", "https://ms.immowelt.org/725fb4fb-900c-4cd8-9554-dd83fc7bd725/99474ade-0e13-4d47-bf95-373cf4af43ec", "https://ms.immowelt.org/a0bb9c06-d60a-40e4-9521-94d9c183a14d/93799d3a-657d-4385-b487-2691349273e9", "https://ms.immowelt.org/3b4d1b7b-a5fe-4a37-b98d-6fc308d03c5b/c80e2b27-9270-47ef-b292-eb1efd72ee07"]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Herr", "firstName": "Wolfgang", "lastName": "Roth", "phone": "0931/382-7702"}</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Helle 3-Zimmer-Wohnung mit Balkon", "basicObjectPricEur": 1797.71, "basicLivingSpace": 123.98, "basicRooms": 3, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2av845v", "basicContactPhone": "0931/382-7702"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "**Erstbezug** Renoviertes Studenten-Apartment nahe Uni Hubland und Wittelsbacherplatz", "basicObjectPricEur": 415, "basicLivingSpace": 26, "basicRooms": 1, "basicConstructionYear": 1950, "basicCity": "W\u00fcrzburg", "basicStreet": "Rottendorferstra\u00dfe 55", "basicUrl": "https://www.immowelt.de/expose/2aeal5v", "basicContactMobile": "+49 176 21469496"}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2abty5v"</t>
+          <t>"https://www.immowelt.de/expose/2av845v"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1154,12 +1104,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"[TAUSCHWOHNUNG] Wundersch\u00f6ne helle Altbauwohnung"</t>
+          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Helle 3-Zimmer-Wohnung mit Balkon"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>430</t>
+          <t>1797.71</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1169,54 +1119,49 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>123.98</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["WANNE", "gaestewc", "DUSCHE", "Kelleranteil", "Personenaufzug", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Balkon", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 430, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 115, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 1797.71, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 250, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7a4af935-fdca-42b8-b470-a905b68d671e/717dc8fc-8461-4d19-89e3-3eaf6c5bfb76"]</t>
+          <t>["https://ms.immowelt.org/34aad469-3611-425d-9832-c02c7060cb23/77ba9d6f-e612-4962-9317-bd0107dc25f7", "https://ms.immowelt.org/8ea07a0f-c3a2-4e3e-a9d2-fe6544358d93/58dbc143-5e69-4062-9eae-b767cf0c69b1", "https://ms.immowelt.org/6b6cd2cc-a04d-480c-949a-1a21bbd7e1d4/51babd4b-8fbc-456a-862b-c4ebde7dc41a", "https://ms.immowelt.org/a8f09c5d-403e-4528-a15f-17ef6819f51c/15cf94e1-0865-4970-bdbc-7eeb2e4e321a", "https://ms.immowelt.org/a74342e9-df14-4a0d-b4c6-600423e5e886/caed2534-21fc-4d11-981c-a2164e56802b", "https://ms.immowelt.org/57b465e5-f400-4f58-8856-6a92ccb5dc5c/e24df36d-9d71-44a2-bd39-c0146b4df941", "https://ms.immowelt.org/4d380785-997d-4deb-b741-8c14d08622b6/d794011b-6b71-4e97-adb0-c319032680b3", "https://ms.immowelt.org/a1aeaa9b-89a7-4a5b-b3ed-598756319607/14a91c1a-5084-49dc-b75d-74d20228a8f0", "https://ms.immowelt.org/af2232f0-1ef7-4481-801f-2a5ff59e0092/96a901ff-03de-431d-886e-d860ac84fbc4", "https://ms.immowelt.org/eb83b1d9-acf0-4e74-b0b3-5fa3fcc1ca01/705ad620-364a-4237-968f-e9f4e0c3eb36", "https://ms.immowelt.org/b34e24ec-eac1-4eae-b4db-e1f386853cb1/292b937e-2528-4472-8123-fa7a878ef84b", "https://ms.immowelt.org/4111770b-ae7b-4dce-b625-f990d3c5ba1e/b7539eac-4bf3-4d62-ab60-f12720be1758", "https://ms.immowelt.org/73dc46c5-cb67-4432-b97f-e11d22268b50/6613c506-3bb4-4e53-a0ac-d3296fe50f9c", "https://ms.immowelt.org/d8083607-cc91-46ee-92df-9a6f4eed9d3b/59f57e14-612a-4c44-8a58-7436d9771597"]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>{"companyName": "Tauschwohnung GmbH", "address": {"city": "Bonn", "zipCode": "53175", "street": "Graf-von-Lehndorff-Str. 12"}, "profilePicture": "https://filestore.immowelt.de/ProfilBilder/150_13236f6bb6c141cd845d0ac0006487a0.jpg", "salutation": "Herr", "firstName": "John", "lastName": "Weinert", "phone": "+4922892939484"}</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "[TAUSCHWOHNUNG] Wundersch\u00f6ne helle Altbauwohnung", "basicObjectPricEur": 430, "basicLivingSpace": 64, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2abty5v", "basicContactPhone": "+4922892939484"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Helle 3-Zimmer-Wohnung mit Balkon", "basicObjectPricEur": 1797.71, "basicLivingSpace": 123.98, "basicRooms": 3, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2av845v", "basicContactPhone": "0931/382-7702"}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
+          <t>"https://www.immowelt.de/expose/2ayb45v"</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1226,12 +1171,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
+          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Gro\u00dfz\u00fcgige 6-Zimmer-Maisonette-Wohnung"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>3601.44</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1241,54 +1186,49 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>225.09</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>["WANNE"]</t>
+          <t>["WANNE", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Balkon", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3601.44, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 460, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
+          <t>["https://ms.immowelt.org/b888654a-7be0-4b1f-bb51-2d8dca6a1aa1/5dc0db39-67ad-4630-8a84-004692c1c198", "https://ms.immowelt.org/4cb98d26-30d4-40dd-9345-c05636fc3d6e/3d269755-d356-448a-a4e4-c9c9225867b0", "https://ms.immowelt.org/71ab24a9-6d26-4798-959a-526196ab2526/2338dbdc-85e0-452f-bbf4-cbd765176db2", "https://ms.immowelt.org/e212abae-27ab-4901-ad56-4abbf1ab429a/076c61fa-ae56-43bd-90cc-3d4a1f246534", "https://ms.immowelt.org/45fda28f-bd4b-477c-8e5b-025d3035fc24/25270c0c-e6f1-42be-9bc6-154afc390bde", "https://ms.immowelt.org/250e735d-28bf-4e41-a26e-10bdcc174a72/9ffa4901-709f-4a22-bcf8-4026af4845a8", "https://ms.immowelt.org/47738d72-90e1-400f-8f26-b0c89e0a04d4/b2671ee7-2150-4931-ae87-848ca314834d", "https://ms.immowelt.org/09239b5c-efed-4862-9be0-12284713015c/c50d605a-b30b-4c1e-b8c7-c377d0105c47", "https://ms.immowelt.org/32be8996-eac0-4fda-8211-2d8fadd6467a/c5cb6c3d-45d4-45e6-8603-f3cc8967b34e", "https://ms.immowelt.org/de7996d0-a07e-44a3-a014-b9f228303c3b/f4242060-e83a-4836-b64b-41645c5c5e94", "https://ms.immowelt.org/d9382006-8b3f-46eb-802b-250a8fca3f96/03f39cab-4da2-4c36-80c1-23a7fbd309fe", "https://ms.immowelt.org/36af7108-dfdd-4ff3-ab8b-6e92d3508062/2f20f749-7813-4534-bde5-1a624ad88952", "https://ms.immowelt.org/ba912dea-da2a-4abd-add2-64d03801c9f2/0f910eff-7ebe-4154-9f66-0556d0a42237", "https://ms.immowelt.org/469127b9-c85a-4e77-a7fa-af7365f65cc3/9cd962ef-da29-4690-9168-413036c7882b", "https://ms.immowelt.org/0341b685-a77c-4318-bf97-0b0facbf1946/c0c91076-cd90-41c2-8e29-c3d9b6bc4e76", "https://ms.immowelt.org/349ba8bc-380d-425c-9404-fe30348c76fb/be7df368-083b-4bf6-bb15-c9ee4809e9b4", "https://ms.immowelt.org/769d004b-9208-4258-b045-f78d35bbe304/cab7c6e2-a6fe-44e9-b980-49f912c4dc33", "https://ms.immowelt.org/32a4701e-f4a1-4e08-ac43-7f82a0871c0e/05462d50-f4b2-41fb-94fc-03251da46a31", "https://ms.immowelt.org/c3b62a14-8ad0-4bc1-ad12-407a7b7d45c1/1e082fb8-309d-48fd-9675-1e19df39056b"]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Gro\u00dfz\u00fcgige 6-Zimmer-Maisonette-Wohnung", "basicObjectPricEur": 3601.44, "basicLivingSpace": 225.09, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2ayb45v", "basicContactPhone": "0931/382-7708"}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ay645v"</t>
+          <t>"https://www.immowelt.de/expose/2acjp5u"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1298,12 +1238,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Ger\u00e4umige 6-Zimmer-Maisonette-Wohnung"</t>
+          <t>"6er-Studenten-Wohngemeinschaft - Zi.Nr. 4"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3163.32</t>
+          <t>350</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1313,47 +1253,42 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>218.16</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1972</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "Erdgeschoss", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
+          <t>["Dach ausgebaut", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "GEPFLEGT", "Massivhaus", "GAS", "Zentralheizung", "DSL", "teilweise m\u00f6bliert", "FLIESEN", "frei", "Einbauk\u00fcche", "wg_geeignet", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Amalienstr. 6", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3163.32, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 440, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 350, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 450, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/33a10e2d-1546-47e8-8bf4-47024f96365d/8d31a374-f6c2-4671-ba5e-b06a8d7c1f18", "https://ms.immowelt.org/e715d610-ea80-4459-9e3a-1ea8a574c0d7/c594e925-e9d3-4474-88ff-ee637dc4b81a", "https://ms.immowelt.org/f3e49668-7602-45ad-979f-f68f0c60ad46/6da2c38a-e66f-4112-b3c3-70ebaa38a22f", "https://ms.immowelt.org/e4691abb-17a5-41aa-949d-88daa0ab8d3a/42a9ae4f-34fd-4230-8329-9c00ba557222", "https://ms.immowelt.org/62981e85-dc6c-481f-8d77-c7e82c11d711/a90f265f-b3b3-4b6b-a854-a05b00191bac", "https://ms.immowelt.org/c1f1f311-d95b-465f-94a6-317a246989d2/e96a7cca-1527-484c-a8e9-f79e1cf28136", "https://ms.immowelt.org/935854af-6f17-4d5d-b023-6647d4cc8d4d/87cabb52-19fe-4dca-a81d-9b0f6d4daa7c", "https://ms.immowelt.org/d22f872e-159f-4f19-bb2a-75f5b228899d/044b33f6-2258-490a-ae2a-52d9ce17b653", "https://ms.immowelt.org/58dca412-8d3b-415e-9a26-359678019657/0858d4e1-5dc0-4297-8a4f-b5db5dbeb8b8", "https://ms.immowelt.org/f9bab463-404a-46c6-990a-559df575f251/6d53c5c6-d652-4e1d-98e5-448095327b4f", "https://ms.immowelt.org/6559ac4a-0154-4e05-a366-dbf71d55ad3a/29c1a7fd-15be-4a1b-91ca-9db0f1c442f3", "https://ms.immowelt.org/85c20839-cb59-4728-be4d-78d1ffcb9274/f88983a1-2f68-4f01-af1a-cae1794eb9e4", "https://ms.immowelt.org/f0a33cc2-272c-4fe9-a229-0c65344655fb/1911e15f-4afd-4691-a583-109b097d5b1a", "https://ms.immowelt.org/26da2883-f715-4c66-a8d1-3e2b9550fcf3/90d1f6cc-c1ae-4b39-889a-79bf683b589e", "https://ms.immowelt.org/b51072d7-8214-4cb3-b4f1-4c2d9c08cc58/e2548663-d3a0-4cb8-b0f7-5aaacf362ba3", "https://ms.immowelt.org/b5dd6e96-9575-46aa-af37-c7a1914335de/e4d4ff07-527e-4aff-be0a-66c047b2b747", "https://ms.immowelt.org/4c4b10ce-78b2-449d-a1c4-38ef2035555b/8094732c-995f-4ee6-af5f-e52e6a68bac8", "https://ms.immowelt.org/36750323-149d-49f3-8859-a599078cdc7a/0c862b3d-b2f3-4b3a-b234-8e9299775647", "https://ms.immowelt.org/d1d807de-1e05-4eca-b9fd-01dd45660714/8d6cc502-9779-4a2e-bfea-d50b253ff0f3"]</t>
+          <t>["https://ms.immowelt.org/ea4c2f0b-394f-42bd-abb7-a4b389c1d47d/ff497d04-808a-4337-a3e3-2cf5516bba7a", "https://ms.immowelt.org/366939ca-53fe-483d-98bf-f2ee6195dfc0/05b63755-5ed7-47a4-8dff-3f7fe160860a", "https://ms.immowelt.org/985ea057-3cd8-4f50-902d-75b4fdfd5d80/985af61d-8d10-46f1-8973-3ca9e3128892", "https://ms.immowelt.org/d60ab3e7-f8b1-4a56-9fe7-cb3d6b251fde/39119cc8-1171-4282-96e2-7cd5703d138e", "https://ms.immowelt.org/74ddb531-c432-441d-a6d9-f10cae01c815/df9fece6-1aa2-4522-9459-fe31c0fdf7be", "https://ms.immowelt.org/90f66d94-cf4f-4975-a300-fd5fdaa057dd/e4aca2a3-3782-48dc-8ebd-01cb1c5d26af", "https://ms.immowelt.org/ed2b2673-027a-4c7d-b469-2d88936aa895/c5525e35-fb10-4c05-a6b3-3903c73a1cd5", "https://ms.immowelt.org/f444609a-1c93-44de-bc86-3bb35bbe475e/7d9d6f63-18c3-4a57-b866-759c4f01d683", "https://ms.immowelt.org/12808aff-d0d3-4ce7-90a1-158e4dc99040/43dea702-8f33-4bc8-b0cf-8fae834b567c", "https://ms.immowelt.org/8bff2dd9-2249-43dc-900d-40ea65a23212/251524b5-e8c7-49a9-b995-00de0bb85ffe", "https://ms.immowelt.org/64561934-cc49-4074-b25f-6a6806f1cdd0/7971880f-b488-43df-a3e6-ee4aec51ae9a", "https://ms.immowelt.org/3ed2c2ec-6223-4e04-99ae-df359a6754c4/1aa90e24-28b3-4bc9-99dd-a8b18c2af3bb", "https://ms.immowelt.org/43927a50-d329-414c-b0f5-ca4f4cd70c2d/5a27d374-b073-4a66-9c71-23db210c7bc5", "https://ms.immowelt.org/49b01679-3040-4664-8c50-17d1e81e7a90/6a4baaaa-1b65-421e-8e20-4ce145d2b6c7", "https://ms.immowelt.org/5be96dee-5832-445f-8d62-264839c37343/d5b9dc02-555e-49f4-8a72-b5fdde07f935", "https://ms.immowelt.org/6bc5b40d-e97f-4fba-8c44-222645648458/42d69790-b9a5-40e9-8b43-b7529c138a8a", "https://ms.immowelt.org/60dec9ad-25a6-4596-8475-c20d723fe05a/3ddd5c6e-9448-40f9-be5d-4065443127a7", "https://ms.immowelt.org/e105af84-a45f-4370-b285-74bee821da08/e6dc5c1d-ad19-4038-ada0-3eecaf37fcc2", "https://ms.immowelt.org/927559a3-db2e-471f-8de6-33b5b3a3a96a/45e4cf6e-8048-4fa0-a7e4-5494ea0506a4", "https://ms.immowelt.org/3b19e507-1683-467a-bcb1-c424c524ca2f/dc5a81f4-1daf-4f1f-b9c9-c23df92dcb8b", "https://ms.immowelt.org/f136ae8b-8c04-4e1f-be49-5859e9cc12aa/45b449b8-53d3-4136-a7a7-bb156ed3b3c2"]</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Frau", "firstName": "Heike", "lastName": "Fabiunke", "phone": "0931/382-7708"}</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Ger\u00e4umige 6-Zimmer-Maisonette-Wohnung", "basicObjectPricEur": 3163.32, "basicLivingSpace": 218.16, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2ay645v", "basicContactPhone": "0931/382-7708"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "6er-Studenten-Wohngemeinschaft - Zi.Nr. 4", "basicObjectPricEur": 350, "basicRooms": 1, "basicConstructionYear": 1972, "basicCity": "W\u00fcrzburg", "basicStreet": "Amalienstr. 6", "basicUrl": "https://www.immowelt.de/expose/2acjp5u"}</t>
         </is>
       </c>
     </row>
@@ -1420,11 +1355,6 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
           <t>{"basicTranactionType": "RENT", "basicTitle": "Moderne 1,5- Zimmerwohnung in W\u00fcrzburg/Altstadt", "basicObjectPricEur": 950, "basicLivingSpace": 37, "basicRooms": 1.5, "basicConstructionYear": 1990, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aewq5u", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
@@ -1492,11 +1422,6 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
           <t>{"basicTranactionType": "RENT", "basicTitle": "Hell m\u00f6blierte  2-Zimmerwohnung in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 1095, "basicLivingSpace": 63, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2akwq5u", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
@@ -1504,7 +1429,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2abjp5u"</t>
+          <t>"https://www.immowelt.de/expose/2auvq5u"</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1514,12 +1439,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"6er-Studenten-Wohngemeinschaft - Zi.Nr. 2"</t>
+          <t>"M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland"</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>649</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1529,7 +1454,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>21</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1539,44 +1464,39 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1972</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>["Dach ausgebaut", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "GEPFLEGT", "Massivhaus", "GAS", "Zentralheizung", "DSL", "teilweise m\u00f6bliert", "FLIESEN", "frei", "Einbauk\u00fcche", "wg_geeignet", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
+          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert"]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Amalienstr. 6", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "640", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.298,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 649, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/9ba52a69-6182-42ac-b135-aa03971398d6/ca08d294-c112-4542-9217-884244d0d406", "https://ms.immowelt.org/d2976824-6694-44cf-a9b6-27ee23e5ee7d/3b4552e6-7f48-4f9f-8935-65701930862a", "https://ms.immowelt.org/abd16da6-4e60-4077-9fde-df90d5c35ba9/70090f09-6bb6-46bb-8d61-ad69a6f9d337", "https://ms.immowelt.org/9241bd02-41ac-4193-ac08-cb9f982e4abd/4fa1546f-a5f4-4860-b778-44b40407edcb", "https://ms.immowelt.org/297cca9d-a7ba-4a67-92d9-93365151b7c5/d95e6e27-06ec-47b3-b787-69c008ab106a", "https://ms.immowelt.org/3b016415-9aa0-4c6f-bf4a-a08f53671a65/e9132359-9ac5-4683-82f7-c4fc218d8306", "https://ms.immowelt.org/4282be92-39da-4459-a8c5-34173ddc7b9f/a8aeb00d-0b5a-48c1-b780-9278afd054ca", "https://ms.immowelt.org/3f00ed7e-8bf1-401b-8f25-642aae0303e9/8f662276-261e-4853-9a0e-c16cf1a0cf16", "https://ms.immowelt.org/33cac6b2-f066-48ee-b86f-8f34b674b64f/8da9104b-a492-47aa-af05-5e118833566f", "https://ms.immowelt.org/ac6357bc-41cd-473b-8073-52aba4823641/a4383c9d-9081-4f5f-afb3-b59a77fa5b00", "https://ms.immowelt.org/d4734ed1-2904-4290-956a-e971b09473c8/b9a53b6e-72d5-418d-a421-3175e22ad8b1", "https://ms.immowelt.org/e5fc4d4c-767b-44a4-ac3c-a5c84a34fe37/4bf5f24d-e49d-4e14-bae7-18735aba7802", "https://ms.immowelt.org/2fa16c88-73cf-4bf1-9ce3-d457a8a03c5e/caa28f6b-695e-4ee6-bc27-d83d081028ad", "https://ms.immowelt.org/600d4913-62e1-4dd5-9431-46e3dc04f5c0/31f22258-60a5-4acd-874e-d498ea457528", "https://ms.immowelt.org/c78f9909-a0a5-427d-9b1f-a8553957ae21/3eb778af-08e1-40d5-b415-3df323797a59", "https://ms.immowelt.org/de687aba-16ee-476d-a8f9-30df0fe0ec6a/a9787e5c-ea67-488e-af3c-076b4e47fea9", "https://ms.immowelt.org/8b1beea6-698d-4888-97b4-de46bd7498ed/4f90c6e0-1013-4950-9c20-5c0ff18aad7d", "https://ms.immowelt.org/da588edf-b340-4add-adc0-fb3f0c96ad72/59acdf1e-b87f-4ddb-b8d5-ab9ae3aee1eb", "https://ms.immowelt.org/9642eeca-e631-4ac4-ae64-100ae2a9f0e9/996373fc-c623-4411-afbc-f2104a65e4a7", "https://ms.immowelt.org/773ea5c5-cb8c-413d-a62d-d05b7ed9e19e/ca6e755b-48d9-4b44-9df9-56eb13fc5024", "https://ms.immowelt.org/e7f711ba-ac7b-44fc-90e8-deda2cee8b0c/bd0ca932-727d-4d26-8518-5c0e19bf2160"]</t>
+          <t>["https://ms.immowelt.org/231cfc3d-f3ec-4eea-b3d8-d3f27a286b40/3058b16a-8a05-47d3-8512-63886059b512", "https://ms.immowelt.org/2660e3fb-eb65-4bd8-8844-5b667e3b062d/adc4fedc-4170-4ee1-a6c7-2d63780cfd0e", "https://ms.immowelt.org/dcb8e961-2856-45f0-8df9-13b8f9f4cadd/19a60ab9-5a93-4d74-be47-9ec0408e6e89", "https://ms.immowelt.org/4f79f7ef-0e51-49b2-ab74-287b9836cc3d/83e20f80-c025-439d-aace-e927f852a97b", "https://ms.immowelt.org/08d42db4-e036-4159-8269-dcb7bd5631a1/9cf8e0c1-3269-44d4-986b-bd625c8101ae", "https://ms.immowelt.org/2f13d3b5-8df8-4ac9-95af-5ba7f89e3dc1/d94afc12-acd9-4275-be9b-8fae1c182d5f", "https://ms.immowelt.org/0308a23f-5076-4db4-9f3b-c6024f595313/7143a6d8-6101-40b4-a19f-aba8e2a5a145", "https://ms.immowelt.org/814288ea-742a-4172-affa-ff8454f45731/e6ca30e2-64eb-4733-9789-940742a1d5d5", "https://ms.immowelt.org/ba83b81a-c23e-4eb8-8f5f-47a680847e30/7b794550-2c44-4fa8-9bb7-a6f8c6820a8a"]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>{"companyName": "M &amp;a; M Bauprojektierung  und Vertrieb GmbH", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Franz-Brentano-Stra\u00dfe 2"}, "salutation": "Herr", "firstName": "Sascha", "lastName": "Mannel"}</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "6er-Studenten-Wohngemeinschaft - Zi.Nr. 2", "basicObjectPricEur": 320, "basicRooms": 1, "basicConstructionYear": 1972, "basicCity": "W\u00fcrzburg", "basicStreet": "Amalienstr. 6", "basicUrl": "https://www.immowelt.de/expose/2abjp5u"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 649, "basicLivingSpace": 21, "basicRooms": 1, "basicConstructionYear": 2015, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2auvq5u", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2agwq5u"</t>
+          <t>"https://www.immowelt.de/expose/2ay645v"</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1586,12 +1506,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland"</t>
+          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Ger\u00e4umige 6-Zimmer-Maisonette-Wohnung"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>649</t>
+          <t>3163.32</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1601,54 +1521,49 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>218.16</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert"]</t>
+          <t>["WANNE", "gaestewc", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "Erdgeschoss", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.298,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 649, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3163.32, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 440, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/cf8697dc-afcd-47ae-aadc-64c4cc78569c/35b4d352-660a-4816-94a6-619497123ae8", "https://ms.immowelt.org/a32b8f72-a566-4394-bea1-04e883e8fce2/7099cff9-9eea-4d1f-bad4-4033626afe54", "https://ms.immowelt.org/105a8a3c-c718-4c20-83ac-d0a5ef1a7f53/9db73218-715a-4963-942c-e41a29ef7b07", "https://ms.immowelt.org/64d9efa5-0a66-44fe-aa1e-b89f834ad546/6f687f3d-4a05-4f47-a1f8-8b78ca7e8bfe", "https://ms.immowelt.org/a3fe7335-2ba5-4c30-a137-cbfb5fd2a35c/20496698-5e1f-4243-9338-f56821682d4a", "https://ms.immowelt.org/a449833e-f4f4-43ff-8ebf-01bc5160e5c9/ccc566af-477b-4888-b03f-1cc64f4f1c45", "https://ms.immowelt.org/a6d17184-1155-46e9-af2c-d83d9e1be344/aab72d40-469f-486c-9add-806a5481ac6a", "https://ms.immowelt.org/a5271f16-acef-4db4-84ba-2b1a9ddc5892/57e11dd6-6321-45eb-85e0-aaa0f1e15bfe", "https://ms.immowelt.org/921ae069-2035-4dbb-a619-8ad9012a2442/0e6324ba-04b0-4141-bcc2-3b6cb33ac8ea", "https://ms.immowelt.org/6dc638c1-e4cd-4f0c-87b2-169cc34b0bd8/2af01fd5-93ce-4fc8-ae87-9a3817a2ef84", "https://ms.immowelt.org/a5894c49-800c-4d59-bb53-e598cf560634/0aa6a439-1071-40bd-a3ef-3bd2192fad8c", "https://ms.immowelt.org/1824d009-9f1e-4248-ac1b-d6198f9c17f3/ffd7b610-0d17-43b2-b15c-614cccf8be14", "https://ms.immowelt.org/45f31b8e-c2fc-45ff-8dac-c0bf8fea6e03/a11c6ffd-ddba-4524-9aca-520b2604d193", "https://ms.immowelt.org/5ec8ff49-d6b8-4dd0-bd1b-a04062520b58/b2e43f71-c2eb-4713-a428-6da937a58826"]</t>
+          <t>["https://ms.immowelt.org/33a10e2d-1546-47e8-8bf4-47024f96365d/8d31a374-f6c2-4671-ba5e-b06a8d7c1f18", "https://ms.immowelt.org/e715d610-ea80-4459-9e3a-1ea8a574c0d7/c594e925-e9d3-4474-88ff-ee637dc4b81a", "https://ms.immowelt.org/f3e49668-7602-45ad-979f-f68f0c60ad46/6da2c38a-e66f-4112-b3c3-70ebaa38a22f", "https://ms.immowelt.org/e4691abb-17a5-41aa-949d-88daa0ab8d3a/42a9ae4f-34fd-4230-8329-9c00ba557222", "https://ms.immowelt.org/62981e85-dc6c-481f-8d77-c7e82c11d711/a90f265f-b3b3-4b6b-a854-a05b00191bac", "https://ms.immowelt.org/c1f1f311-d95b-465f-94a6-317a246989d2/e96a7cca-1527-484c-a8e9-f79e1cf28136", "https://ms.immowelt.org/935854af-6f17-4d5d-b023-6647d4cc8d4d/87cabb52-19fe-4dca-a81d-9b0f6d4daa7c", "https://ms.immowelt.org/d22f872e-159f-4f19-bb2a-75f5b228899d/044b33f6-2258-490a-ae2a-52d9ce17b653", "https://ms.immowelt.org/58dca412-8d3b-415e-9a26-359678019657/0858d4e1-5dc0-4297-8a4f-b5db5dbeb8b8", "https://ms.immowelt.org/f9bab463-404a-46c6-990a-559df575f251/6d53c5c6-d652-4e1d-98e5-448095327b4f", "https://ms.immowelt.org/6559ac4a-0154-4e05-a366-dbf71d55ad3a/29c1a7fd-15be-4a1b-91ca-9db0f1c442f3", "https://ms.immowelt.org/85c20839-cb59-4728-be4d-78d1ffcb9274/f88983a1-2f68-4f01-af1a-cae1794eb9e4", "https://ms.immowelt.org/f0a33cc2-272c-4fe9-a229-0c65344655fb/1911e15f-4afd-4691-a583-109b097d5b1a", "https://ms.immowelt.org/26da2883-f715-4c66-a8d1-3e2b9550fcf3/90d1f6cc-c1ae-4b39-889a-79bf683b589e", "https://ms.immowelt.org/b51072d7-8214-4cb3-b4f1-4c2d9c08cc58/e2548663-d3a0-4cb8-b0f7-5aaacf362ba3", "https://ms.immowelt.org/b5dd6e96-9575-46aa-af37-c7a1914335de/e4d4ff07-527e-4aff-be0a-66c047b2b747", "https://ms.immowelt.org/4c4b10ce-78b2-449d-a1c4-38ef2035555b/8094732c-995f-4ee6-af5f-e52e6a68bac8", "https://ms.immowelt.org/36750323-149d-49f3-8859-a599078cdc7a/0c862b3d-b2f3-4b3a-b234-8e9299775647", "https://ms.immowelt.org/d1d807de-1e05-4eca-b9fd-01dd45660714/8d6cc502-9779-4a2e-bfea-d50b253ff0f3"]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 649, "basicLivingSpace": 21, "basicRooms": 1, "basicConstructionYear": 2015, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2agwq5u", "basicContactPhone": "+49 931 416616"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Ger\u00e4umige 6-Zimmer-Maisonette-Wohnung", "basicObjectPricEur": 3163.32, "basicLivingSpace": 218.16, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2ay645v", "basicContactPhone": "0931/382-7708"}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a9245v"</t>
+          <t>"https://www.immowelt.de/expose/2af545v"</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1658,12 +1573,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"Neu m\u00f6blierte Wohnung im Herzen der W\u00fcrzburger Altstadt unweit des Marktplatzes mit Wlan"</t>
+          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Exklusive Penthouse-Maisonette-Wohnung"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>815</t>
+          <t>3030.93</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1673,54 +1588,49 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>178.29</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert", "TEPPICH", "FLIESEN", "Balkon"]</t>
+          <t>["barriefrei", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.630,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 815, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3030.93, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 360, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/56dbfa19-0b11-4212-a585-a3bb9055fc6c/55af236d-1cf3-446a-a9ea-5d847c1f3c78", "https://ms.immowelt.org/2321a506-3294-4da0-8ed9-9c32a877cc19/568e9ef6-6f64-4112-9523-9eaf25a3f970", "https://ms.immowelt.org/c49d4e0e-c519-4110-bf9d-48d46975f264/51ad8f90-ae3d-4f54-9436-a3ce93d787e0", "https://ms.immowelt.org/1efec59d-a37f-4e4e-81e0-d2638e029208/c9bd61b7-4af9-4819-822e-916b4c491efd", "https://ms.immowelt.org/35f3c816-30ad-4cfa-a370-9fd3df5a890b/0f5a8622-ff9b-48a3-b656-48f75cd9c811", "https://ms.immowelt.org/1d11277d-e06d-43d1-807a-35d99c5f5cd5/51935719-85d7-4a46-a718-1c1a7bedba2c", "https://ms.immowelt.org/3f9f17e0-3b0f-42d8-9623-bd41d7d12fc4/d88f57cc-ca14-47d1-b0ac-e5d037c3114a", "https://ms.immowelt.org/4c16ccd5-7611-496f-9fc2-a5cc9e95ca96/0cc9afbf-324b-4dc0-a841-e5417e3c909f", "https://ms.immowelt.org/23f4ce8d-d0f3-42f3-b7c2-cbea89a39473/eb285820-0b71-4189-8a94-494d832c127b", "https://ms.immowelt.org/36d590ab-2de9-46f3-8cef-b4af4efd9be0/8e11440a-7fe1-49cf-a002-13e4285760be", "https://ms.immowelt.org/8099beb8-56a4-493f-b95f-2490484605d5/fbb624d4-8b55-48d5-8b8f-5535a08872c5", "https://ms.immowelt.org/1978dbc1-a0ed-458a-abcd-d22f103809ef/1a5cc04f-0b65-48af-8e69-c835714ab2e7", "https://ms.immowelt.org/6b1ab129-3f95-42da-9d53-8088db0a9349/25c6e471-016e-4261-b4ae-a73987e4f403", "https://ms.immowelt.org/9b310d23-aa9d-41f5-8f34-29a9b7aa4471/bae39b36-c4b5-4cf8-882a-aca3ba40538c", "https://ms.immowelt.org/20713457-85cd-4f26-970b-eca4af0b6b71/be6308f1-d0c9-4aa5-8a10-3a4f1f28ff33"]</t>
+          <t>["https://ms.immowelt.org/2b7c4c91-7fac-4ddb-a032-3a51184dbb59/8f34d9b5-fec8-4e21-99c7-6f7a2921d4d1", "https://ms.immowelt.org/61a862a4-1bd5-4769-abb9-5e1d7113f8bc/88d5b2b5-7ef0-4388-8eb9-b7042670aee5", "https://ms.immowelt.org/37c438a9-8ae7-4d42-8006-bc3a55265670/12a6e3ea-2554-4920-bec1-7d536539c02d", "https://ms.immowelt.org/49abcb3b-4395-4691-8e92-b525edda30d4/f7c44e0e-0db0-456e-8cb8-845d816e37ec", "https://ms.immowelt.org/ce95a7e7-0ad6-4282-8ca2-5ce205488707/dbfb5e54-2bfb-4d01-91ec-1ca118a3a922", "https://ms.immowelt.org/b3cc6d40-e3b5-407e-ae5e-be0785a5a218/686cb7a1-8858-4011-a5e0-a8fd590fe4e6", "https://ms.immowelt.org/424d3898-11a5-419c-a472-b6bb5eed3e76/e7d72403-5394-43c9-a960-10468f29d064", "https://ms.immowelt.org/19d6858d-2cb5-437d-8cdb-6fb75d54c5e4/8e3114ed-77c5-47c0-8dce-725b44e8785c", "https://ms.immowelt.org/f536fdcb-a38d-4b90-beab-277e244cf6a7/ce23ee46-5ee8-4496-b672-c3ea031e92ac", "https://ms.immowelt.org/933295a3-d9da-4860-ad95-06490c6fddf4/182424c9-5902-4b40-be26-512097b49929", "https://ms.immowelt.org/a77d50f5-f8e0-4928-bcdc-2fa7c6e36e7d/05824030-0135-4ec2-93dc-52a0bf313587", "https://ms.immowelt.org/dbfe5771-25b1-460e-a2dd-140a19fae05f/4dd99d70-1f73-40c8-aab7-49051e0e90ec", "https://ms.immowelt.org/9689e92f-fdee-4ff1-99c1-89400857e515/a07a7b18-a41e-45a3-9fe1-f64211e577cd", "https://ms.immowelt.org/c3fdabd3-6c7c-4da9-9941-17117007bd14/16545b70-e49d-4309-85c5-a84123f7c8a2", "https://ms.immowelt.org/ec2b29d2-9e49-4ccb-965f-e26d155e848a/1c4de27d-2032-41cc-a466-04b10ad4f27d", "https://ms.immowelt.org/c2913eaa-8856-44c1-901b-0ae4b9a9ffa2/387a24b5-3c67-4740-ac58-0de078b68ff8", "https://ms.immowelt.org/81e05570-c572-4168-acf8-500cd9f74a65/796a2975-473d-4971-bd18-d2765832485e", "https://ms.immowelt.org/2c90ddab-a797-471f-a2aa-53b9ac172a1c/43c8617b-2da6-4fae-99be-395aaf2774e3", "https://ms.immowelt.org/24b3e778-e131-4042-ba05-7b63afaf1ce0/b0dfb227-b3fc-4605-b1c3-58573b4f24d1", "https://ms.immowelt.org/1d31929b-a5c2-410f-9bef-afc44f5e68c1/bc515335-0e9c-453b-bfcf-ae09a83fd65d", "https://ms.immowelt.org/d6e04616-c252-4d95-8d95-9d504b0fb3f4/07aa7bfb-71ab-4b13-bba6-99ba35097b80"]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Neu m\u00f6blierte Wohnung im Herzen der W\u00fcrzburger Altstadt unweit des Marktplatzes mit Wlan", "basicObjectPricEur": 815, "basicLivingSpace": 40, "basicRooms": 1.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a9245v", "basicContactPhone": "+49 931 416616"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Exklusive Penthouse-Maisonette-Wohnung", "basicObjectPricEur": 3030.93, "basicLivingSpace": 178.29, "basicRooms": 5, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2af545v", "basicContactPhone": "0931/382-7701"}</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2acjp5u"</t>
+          <t>"https://www.immowelt.de/expose/2a9245v"</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1730,12 +1640,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"6er-Studenten-Wohngemeinschaft - Zi.Nr. 4"</t>
+          <t>"Neu m\u00f6blierte Wohnung im Herzen der W\u00fcrzburger Altstadt unweit des Marktplatzes mit Wlan"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>350</t>
+          <t>815</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1745,54 +1655,49 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>40</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1972</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>["Dach ausgebaut", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "GEPFLEGT", "Massivhaus", "GAS", "Zentralheizung", "DSL", "teilweise m\u00f6bliert", "FLIESEN", "frei", "Einbauk\u00fcche", "wg_geeignet", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
+          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert", "TEPPICH", "FLIESEN", "Balkon"]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Amalienstr. 6", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 350, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 450, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.630,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 815, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/ea4c2f0b-394f-42bd-abb7-a4b389c1d47d/ff497d04-808a-4337-a3e3-2cf5516bba7a", "https://ms.immowelt.org/366939ca-53fe-483d-98bf-f2ee6195dfc0/05b63755-5ed7-47a4-8dff-3f7fe160860a", "https://ms.immowelt.org/985ea057-3cd8-4f50-902d-75b4fdfd5d80/985af61d-8d10-46f1-8973-3ca9e3128892", "https://ms.immowelt.org/d60ab3e7-f8b1-4a56-9fe7-cb3d6b251fde/39119cc8-1171-4282-96e2-7cd5703d138e", "https://ms.immowelt.org/74ddb531-c432-441d-a6d9-f10cae01c815/df9fece6-1aa2-4522-9459-fe31c0fdf7be", "https://ms.immowelt.org/90f66d94-cf4f-4975-a300-fd5fdaa057dd/e4aca2a3-3782-48dc-8ebd-01cb1c5d26af", "https://ms.immowelt.org/ed2b2673-027a-4c7d-b469-2d88936aa895/c5525e35-fb10-4c05-a6b3-3903c73a1cd5", "https://ms.immowelt.org/f444609a-1c93-44de-bc86-3bb35bbe475e/7d9d6f63-18c3-4a57-b866-759c4f01d683", "https://ms.immowelt.org/12808aff-d0d3-4ce7-90a1-158e4dc99040/43dea702-8f33-4bc8-b0cf-8fae834b567c", "https://ms.immowelt.org/8bff2dd9-2249-43dc-900d-40ea65a23212/251524b5-e8c7-49a9-b995-00de0bb85ffe", "https://ms.immowelt.org/64561934-cc49-4074-b25f-6a6806f1cdd0/7971880f-b488-43df-a3e6-ee4aec51ae9a", "https://ms.immowelt.org/3ed2c2ec-6223-4e04-99ae-df359a6754c4/1aa90e24-28b3-4bc9-99dd-a8b18c2af3bb", "https://ms.immowelt.org/43927a50-d329-414c-b0f5-ca4f4cd70c2d/5a27d374-b073-4a66-9c71-23db210c7bc5", "https://ms.immowelt.org/49b01679-3040-4664-8c50-17d1e81e7a90/6a4baaaa-1b65-421e-8e20-4ce145d2b6c7", "https://ms.immowelt.org/5be96dee-5832-445f-8d62-264839c37343/d5b9dc02-555e-49f4-8a72-b5fdde07f935", "https://ms.immowelt.org/6bc5b40d-e97f-4fba-8c44-222645648458/42d69790-b9a5-40e9-8b43-b7529c138a8a", "https://ms.immowelt.org/60dec9ad-25a6-4596-8475-c20d723fe05a/3ddd5c6e-9448-40f9-be5d-4065443127a7", "https://ms.immowelt.org/e105af84-a45f-4370-b285-74bee821da08/e6dc5c1d-ad19-4038-ada0-3eecaf37fcc2", "https://ms.immowelt.org/927559a3-db2e-471f-8de6-33b5b3a3a96a/45e4cf6e-8048-4fa0-a7e4-5494ea0506a4", "https://ms.immowelt.org/3b19e507-1683-467a-bcb1-c424c524ca2f/dc5a81f4-1daf-4f1f-b9c9-c23df92dcb8b", "https://ms.immowelt.org/f136ae8b-8c04-4e1f-be49-5859e9cc12aa/45b449b8-53d3-4136-a7a7-bb156ed3b3c2"]</t>
+          <t>["https://ms.immowelt.org/56dbfa19-0b11-4212-a585-a3bb9055fc6c/55af236d-1cf3-446a-a9ea-5d847c1f3c78", "https://ms.immowelt.org/2321a506-3294-4da0-8ed9-9c32a877cc19/568e9ef6-6f64-4112-9523-9eaf25a3f970", "https://ms.immowelt.org/c49d4e0e-c519-4110-bf9d-48d46975f264/51ad8f90-ae3d-4f54-9436-a3ce93d787e0", "https://ms.immowelt.org/1efec59d-a37f-4e4e-81e0-d2638e029208/c9bd61b7-4af9-4819-822e-916b4c491efd", "https://ms.immowelt.org/35f3c816-30ad-4cfa-a370-9fd3df5a890b/0f5a8622-ff9b-48a3-b656-48f75cd9c811", "https://ms.immowelt.org/1d11277d-e06d-43d1-807a-35d99c5f5cd5/51935719-85d7-4a46-a718-1c1a7bedba2c", "https://ms.immowelt.org/3f9f17e0-3b0f-42d8-9623-bd41d7d12fc4/d88f57cc-ca14-47d1-b0ac-e5d037c3114a", "https://ms.immowelt.org/4c16ccd5-7611-496f-9fc2-a5cc9e95ca96/0cc9afbf-324b-4dc0-a841-e5417e3c909f", "https://ms.immowelt.org/23f4ce8d-d0f3-42f3-b7c2-cbea89a39473/eb285820-0b71-4189-8a94-494d832c127b", "https://ms.immowelt.org/36d590ab-2de9-46f3-8cef-b4af4efd9be0/8e11440a-7fe1-49cf-a002-13e4285760be", "https://ms.immowelt.org/8099beb8-56a4-493f-b95f-2490484605d5/fbb624d4-8b55-48d5-8b8f-5535a08872c5", "https://ms.immowelt.org/1978dbc1-a0ed-458a-abcd-d22f103809ef/1a5cc04f-0b65-48af-8e69-c835714ab2e7", "https://ms.immowelt.org/6b1ab129-3f95-42da-9d53-8088db0a9349/25c6e471-016e-4261-b4ae-a73987e4f403", "https://ms.immowelt.org/9b310d23-aa9d-41f5-8f34-29a9b7aa4471/bae39b36-c4b5-4cf8-882a-aca3ba40538c", "https://ms.immowelt.org/20713457-85cd-4f26-970b-eca4af0b6b71/be6308f1-d0c9-4aa5-8a10-3a4f1f28ff33"]</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>{"companyName": "M &amp;a; M Bauprojektierung  und Vertrieb GmbH", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Franz-Brentano-Stra\u00dfe 2"}, "salutation": "Herr", "firstName": "Sascha", "lastName": "Mannel"}</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "6er-Studenten-Wohngemeinschaft - Zi.Nr. 4", "basicObjectPricEur": 350, "basicRooms": 1, "basicConstructionYear": 1972, "basicCity": "W\u00fcrzburg", "basicStreet": "Amalienstr. 6", "basicUrl": "https://www.immowelt.de/expose/2acjp5u"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Neu m\u00f6blierte Wohnung im Herzen der W\u00fcrzburger Altstadt unweit des Marktplatzes mit Wlan", "basicObjectPricEur": 815, "basicLivingSpace": 40, "basicRooms": 1.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a9245v", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2af545v"</t>
+          <t>"https://www.immowelt.de/expose/2agwq5u"</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1802,12 +1707,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Exklusive Penthouse-Maisonette-Wohnung"</t>
+          <t>"M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland"</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3030.93</t>
+          <t>649</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1817,54 +1722,49 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>178.29</t>
+          <t>21</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>["barriefrei", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
+          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert"]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3030.93, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 360, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.298,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 649, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/2b7c4c91-7fac-4ddb-a032-3a51184dbb59/8f34d9b5-fec8-4e21-99c7-6f7a2921d4d1", "https://ms.immowelt.org/61a862a4-1bd5-4769-abb9-5e1d7113f8bc/88d5b2b5-7ef0-4388-8eb9-b7042670aee5", "https://ms.immowelt.org/37c438a9-8ae7-4d42-8006-bc3a55265670/12a6e3ea-2554-4920-bec1-7d536539c02d", "https://ms.immowelt.org/49abcb3b-4395-4691-8e92-b525edda30d4/f7c44e0e-0db0-456e-8cb8-845d816e37ec", "https://ms.immowelt.org/ce95a7e7-0ad6-4282-8ca2-5ce205488707/dbfb5e54-2bfb-4d01-91ec-1ca118a3a922", "https://ms.immowelt.org/b3cc6d40-e3b5-407e-ae5e-be0785a5a218/686cb7a1-8858-4011-a5e0-a8fd590fe4e6", "https://ms.immowelt.org/424d3898-11a5-419c-a472-b6bb5eed3e76/e7d72403-5394-43c9-a960-10468f29d064", "https://ms.immowelt.org/19d6858d-2cb5-437d-8cdb-6fb75d54c5e4/8e3114ed-77c5-47c0-8dce-725b44e8785c", "https://ms.immowelt.org/f536fdcb-a38d-4b90-beab-277e244cf6a7/ce23ee46-5ee8-4496-b672-c3ea031e92ac", "https://ms.immowelt.org/933295a3-d9da-4860-ad95-06490c6fddf4/182424c9-5902-4b40-be26-512097b49929", "https://ms.immowelt.org/a77d50f5-f8e0-4928-bcdc-2fa7c6e36e7d/05824030-0135-4ec2-93dc-52a0bf313587", "https://ms.immowelt.org/dbfe5771-25b1-460e-a2dd-140a19fae05f/4dd99d70-1f73-40c8-aab7-49051e0e90ec", "https://ms.immowelt.org/9689e92f-fdee-4ff1-99c1-89400857e515/a07a7b18-a41e-45a3-9fe1-f64211e577cd", "https://ms.immowelt.org/c3fdabd3-6c7c-4da9-9941-17117007bd14/16545b70-e49d-4309-85c5-a84123f7c8a2", "https://ms.immowelt.org/ec2b29d2-9e49-4ccb-965f-e26d155e848a/1c4de27d-2032-41cc-a466-04b10ad4f27d", "https://ms.immowelt.org/c2913eaa-8856-44c1-901b-0ae4b9a9ffa2/387a24b5-3c67-4740-ac58-0de078b68ff8", "https://ms.immowelt.org/81e05570-c572-4168-acf8-500cd9f74a65/796a2975-473d-4971-bd18-d2765832485e", "https://ms.immowelt.org/2c90ddab-a797-471f-a2aa-53b9ac172a1c/43c8617b-2da6-4fae-99be-395aaf2774e3", "https://ms.immowelt.org/24b3e778-e131-4042-ba05-7b63afaf1ce0/b0dfb227-b3fc-4605-b1c3-58573b4f24d1", "https://ms.immowelt.org/1d31929b-a5c2-410f-9bef-afc44f5e68c1/bc515335-0e9c-453b-bfcf-ae09a83fd65d", "https://ms.immowelt.org/d6e04616-c252-4d95-8d95-9d504b0fb3f4/07aa7bfb-71ab-4b13-bba6-99ba35097b80"]</t>
+          <t>["https://ms.immowelt.org/cf8697dc-afcd-47ae-aadc-64c4cc78569c/35b4d352-660a-4816-94a6-619497123ae8", "https://ms.immowelt.org/a32b8f72-a566-4394-bea1-04e883e8fce2/7099cff9-9eea-4d1f-bad4-4033626afe54", "https://ms.immowelt.org/105a8a3c-c718-4c20-83ac-d0a5ef1a7f53/9db73218-715a-4963-942c-e41a29ef7b07", "https://ms.immowelt.org/64d9efa5-0a66-44fe-aa1e-b89f834ad546/6f687f3d-4a05-4f47-a1f8-8b78ca7e8bfe", "https://ms.immowelt.org/a3fe7335-2ba5-4c30-a137-cbfb5fd2a35c/20496698-5e1f-4243-9338-f56821682d4a", "https://ms.immowelt.org/a449833e-f4f4-43ff-8ebf-01bc5160e5c9/ccc566af-477b-4888-b03f-1cc64f4f1c45", "https://ms.immowelt.org/a6d17184-1155-46e9-af2c-d83d9e1be344/aab72d40-469f-486c-9add-806a5481ac6a", "https://ms.immowelt.org/a5271f16-acef-4db4-84ba-2b1a9ddc5892/57e11dd6-6321-45eb-85e0-aaa0f1e15bfe", "https://ms.immowelt.org/921ae069-2035-4dbb-a619-8ad9012a2442/0e6324ba-04b0-4141-bcc2-3b6cb33ac8ea", "https://ms.immowelt.org/6dc638c1-e4cd-4f0c-87b2-169cc34b0bd8/2af01fd5-93ce-4fc8-ae87-9a3817a2ef84", "https://ms.immowelt.org/a5894c49-800c-4d59-bb53-e598cf560634/0aa6a439-1071-40bd-a3ef-3bd2192fad8c", "https://ms.immowelt.org/1824d009-9f1e-4248-ac1b-d6198f9c17f3/ffd7b610-0d17-43b2-b15c-614cccf8be14", "https://ms.immowelt.org/45f31b8e-c2fc-45ff-8dac-c0bf8fea6e03/a11c6ffd-ddba-4524-9aca-520b2604d193", "https://ms.immowelt.org/5ec8ff49-d6b8-4dd0-bd1b-a04062520b58/b2e43f71-c2eb-4713-a428-6da937a58826"]</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>{"companyName": "Sparkasse Mainfranken W\u00fcrzburg Facilitymanagement", "address": {"city": "W\u00fcrzburg", "zipCode": "97070", "street": "Hofstra\u00dfe 9"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Jendrzej", "phone": "0931/382-7701"}</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Exklusive Penthouse-Maisonette-Wohnung", "basicObjectPricEur": 3030.93, "basicLivingSpace": 178.29, "basicRooms": 5, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2af545v", "basicContactPhone": "0931/382-7701"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 649, "basicLivingSpace": 21, "basicRooms": 1, "basicConstructionYear": 2015, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2agwq5u", "basicContactPhone": "+49 931 416616"}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2auvq5u"</t>
+          <t>"https://www.immowelt.de/expose/2abjp5u"</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1874,12 +1774,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland"</t>
+          <t>"6er-Studenten-Wohngemeinschaft - Zi.Nr. 2"</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>649</t>
+          <t>320</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1889,7 +1789,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1899,37 +1799,32 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>1972</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert"]</t>
+          <t>["Dach ausgebaut", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "GEPFLEGT", "Massivhaus", "GAS", "Zentralheizung", "DSL", "teilweise m\u00f6bliert", "FLIESEN", "frei", "Einbauk\u00fcche", "wg_geeignet", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Amalienstr. 6", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.298,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 649, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "640", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/231cfc3d-f3ec-4eea-b3d8-d3f27a286b40/3058b16a-8a05-47d3-8512-63886059b512", "https://ms.immowelt.org/2660e3fb-eb65-4bd8-8844-5b667e3b062d/adc4fedc-4170-4ee1-a6c7-2d63780cfd0e", "https://ms.immowelt.org/dcb8e961-2856-45f0-8df9-13b8f9f4cadd/19a60ab9-5a93-4d74-be47-9ec0408e6e89", "https://ms.immowelt.org/4f79f7ef-0e51-49b2-ab74-287b9836cc3d/83e20f80-c025-439d-aace-e927f852a97b", "https://ms.immowelt.org/08d42db4-e036-4159-8269-dcb7bd5631a1/9cf8e0c1-3269-44d4-986b-bd625c8101ae", "https://ms.immowelt.org/2f13d3b5-8df8-4ac9-95af-5ba7f89e3dc1/d94afc12-acd9-4275-be9b-8fae1c182d5f", "https://ms.immowelt.org/0308a23f-5076-4db4-9f3b-c6024f595313/7143a6d8-6101-40b4-a19f-aba8e2a5a145", "https://ms.immowelt.org/814288ea-742a-4172-affa-ff8454f45731/e6ca30e2-64eb-4733-9789-940742a1d5d5", "https://ms.immowelt.org/ba83b81a-c23e-4eb8-8f5f-47a680847e30/7b794550-2c44-4fa8-9bb7-a6f8c6820a8a"]</t>
+          <t>["https://ms.immowelt.org/9ba52a69-6182-42ac-b135-aa03971398d6/ca08d294-c112-4542-9217-884244d0d406", "https://ms.immowelt.org/d2976824-6694-44cf-a9b6-27ee23e5ee7d/3b4552e6-7f48-4f9f-8935-65701930862a", "https://ms.immowelt.org/abd16da6-4e60-4077-9fde-df90d5c35ba9/70090f09-6bb6-46bb-8d61-ad69a6f9d337", "https://ms.immowelt.org/9241bd02-41ac-4193-ac08-cb9f982e4abd/4fa1546f-a5f4-4860-b778-44b40407edcb", "https://ms.immowelt.org/297cca9d-a7ba-4a67-92d9-93365151b7c5/d95e6e27-06ec-47b3-b787-69c008ab106a", "https://ms.immowelt.org/3b016415-9aa0-4c6f-bf4a-a08f53671a65/e9132359-9ac5-4683-82f7-c4fc218d8306", "https://ms.immowelt.org/4282be92-39da-4459-a8c5-34173ddc7b9f/a8aeb00d-0b5a-48c1-b780-9278afd054ca", "https://ms.immowelt.org/3f00ed7e-8bf1-401b-8f25-642aae0303e9/8f662276-261e-4853-9a0e-c16cf1a0cf16", "https://ms.immowelt.org/33cac6b2-f066-48ee-b86f-8f34b674b64f/8da9104b-a492-47aa-af05-5e118833566f", "https://ms.immowelt.org/ac6357bc-41cd-473b-8073-52aba4823641/a4383c9d-9081-4f5f-afb3-b59a77fa5b00", "https://ms.immowelt.org/d4734ed1-2904-4290-956a-e971b09473c8/b9a53b6e-72d5-418d-a421-3175e22ad8b1", "https://ms.immowelt.org/e5fc4d4c-767b-44a4-ac3c-a5c84a34fe37/4bf5f24d-e49d-4e14-bae7-18735aba7802", "https://ms.immowelt.org/2fa16c88-73cf-4bf1-9ce3-d457a8a03c5e/caa28f6b-695e-4ee6-bc27-d83d081028ad", "https://ms.immowelt.org/600d4913-62e1-4dd5-9431-46e3dc04f5c0/31f22258-60a5-4acd-874e-d498ea457528", "https://ms.immowelt.org/c78f9909-a0a5-427d-9b1f-a8553957ae21/3eb778af-08e1-40d5-b415-3df323797a59", "https://ms.immowelt.org/de687aba-16ee-476d-a8f9-30df0fe0ec6a/a9787e5c-ea67-488e-af3c-076b4e47fea9", "https://ms.immowelt.org/8b1beea6-698d-4888-97b4-de46bd7498ed/4f90c6e0-1013-4950-9c20-5c0ff18aad7d", "https://ms.immowelt.org/da588edf-b340-4add-adc0-fb3f0c96ad72/59acdf1e-b87f-4ddb-b8d5-ab9ae3aee1eb", "https://ms.immowelt.org/9642eeca-e631-4ac4-ae64-100ae2a9f0e9/996373fc-c623-4411-afbc-f2104a65e4a7", "https://ms.immowelt.org/773ea5c5-cb8c-413d-a62d-d05b7ed9e19e/ca6e755b-48d9-4b44-9df9-56eb13fc5024", "https://ms.immowelt.org/e7f711ba-ac7b-44fc-90e8-deda2cee8b0c/bd0ca932-727d-4d26-8518-5c0e19bf2160"]</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>{"companyName": "HC24 GmbH &amp;a; Co. KG - Niederlassung HC24 W\u00fcrzburg", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 16"}, "salutation": "Frau", "firstName": "Konstanze", "lastName": "Kress", "phone": "+49 931 416616"}</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 649, "basicLivingSpace": 21, "basicRooms": 1, "basicConstructionYear": 2015, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2auvq5u", "basicContactPhone": "+49 931 416616"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "6er-Studenten-Wohngemeinschaft - Zi.Nr. 2", "basicObjectPricEur": 320, "basicRooms": 1, "basicConstructionYear": 1972, "basicCity": "W\u00fcrzburg", "basicStreet": "Amalienstr. 6", "basicUrl": "https://www.immowelt.de/expose/2abjp5u"}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Bugfixing & Formatting
</commit_message>
<xml_diff>
--- a/immowelt_price_guide/data/retrain_train_data.xlsx
+++ b/immowelt_price_guide/data/retrain_train_data.xlsx
@@ -491,7 +491,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ac5n5w"</t>
+          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -501,12 +501,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"2 Zi. DG-Wohnung, W\u00fcrzburg unteres Frauenland"</t>
+          <t>"Bestlage mit Festungsblick"</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>690</t>
+          <t>610</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -516,49 +516,49 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1948</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung"]</t>
+          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1380,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 690, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 100, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 790, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/e560fee6-d1f5-4d88-985d-2a45b56bc9a2/99e465d7-a211-46b1-ac83-d807f3f05105", "https://ms.immowelt.org/9f3548eb-53e1-4cd6-8cb8-72ff7391acc6/ddb97f1a-0052-45f9-b9df-21dcd92def3c", "https://ms.immowelt.org/d1f1a1e6-ea57-41dd-8c06-2cfc4853af60/04a5afa5-cf13-40fa-a2cd-3199f38ef40d", "https://ms.immowelt.org/d841b2f1-d6c2-497e-91b0-23f06f9d6d27/6f421745-0421-4c7a-bdc0-0a9a0757dd75", "https://ms.immowelt.org/05eb2f1d-7605-4c8a-88be-6d8b50879f62/254e4f03-d100-4ac1-9006-92edb86499d0"]</t>
+          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "2 Zi. DG-Wohnung, W\u00fcrzburg unteres Frauenland", "basicObjectPricEur": 690, "basicLivingSpace": 53, "basicRooms": 2, "basicConstructionYear": 1948, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2ac5n5w", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2agsm5w"</t>
+          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -568,12 +568,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Citywohnung - lichtduchflutetes, top gepflegtes Penthouse! Ideal f\u00fcr Paar oder Single!"</t>
+          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1280</t>
+          <t>566.96</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -583,49 +583,49 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>59.68</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>["barriefrei", "WANNE", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GEPFLEGT", "GAS", "Ofenheizung", "Fu\u00dfbodenheizung", "Zentralheizung", "GRANIT", "STEIN", "Einbauk\u00fcche", "Pantry", "Garage", "Tiefgarage", "Haustiere erlaubt", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
+          <t>["Stellplatz"]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 1280, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 190, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"NumberValue": 60, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/087193bc-fbfe-4a52-b25b-e976836c1b5a/6a5b7c77-451a-4444-9e21-f08a30e84553", "https://ms.immowelt.org/83a83c8a-c9c6-4cf7-b43c-21eecdbba0a9/80a620ac-1526-4549-b2ca-23be56ff4f5a", "https://ms.immowelt.org/142e7bcb-13e5-4ba8-826f-0bb3477eeb84/6db81d67-746c-494c-8adf-241b0f790d25", "https://ms.immowelt.org/f1496f59-6df9-425d-80d7-a838a4c1a7dd/66c09951-f14f-40f3-992d-ff3131e560c1", "https://ms.immowelt.org/b8d31f37-b561-4a6f-8745-57f46eb10ed6/e6426a61-57e2-410d-aecc-cb8e2deef6b0", "https://ms.immowelt.org/1241e16d-eca9-4eec-be49-8aed89eb3c6d/b19ad343-bd92-4c30-8d65-53cba1a86284", "https://ms.immowelt.org/ae757e91-851b-4fd5-b3aa-99dd0708076f/71448955-dfdd-4e1f-9447-480c20308908", "https://ms.immowelt.org/be7d12b0-4181-43f8-b138-00c8310c7889/ae021a73-ada6-4d98-b0dd-f8c788c60dd0", "https://ms.immowelt.org/134da61a-9c60-489e-b415-750246407abd/75331e46-7b8a-4d66-8f57-4f231cc26b1d", "https://ms.immowelt.org/64cb559e-398e-40d2-be5b-741d2361ca27/508831f6-c1eb-4e3a-97ce-645df8543b1e", "https://ms.immowelt.org/18ebf27e-34e3-4335-8cc2-c3fdc9f7d169/13c919fb-bef2-4bbf-8082-ac2b0ac4cec0", "https://ms.immowelt.org/366f7626-f55b-4890-9261-6568e13c0baa/62107a51-7c55-4cc6-b568-20f40f73a08f", "https://ms.immowelt.org/dd1b4339-5b92-4a1c-8713-56831bf116fb/fcce419b-3d7a-4ac6-90a3-d2413b204e81", "https://ms.immowelt.org/db68b6e1-11c7-4fee-b27e-05fc368d1e21/9a1f7ab6-c52f-4c92-9a36-9f9c94b29e44", "https://ms.immowelt.org/b865ff14-0572-4d3b-9c2f-70802b0e184f/b56cc229-4d56-467c-a072-5423dcd43b7f", "https://ms.immowelt.org/892021cf-32e9-41d5-a3b8-0de681cff430/615b71ea-8b7a-4a21-a250-1ccaf78e0a78", "https://ms.immowelt.org/9cdea49c-15e1-4690-8319-b6123fa0ba6d/af8b431e-04c0-4e61-8ac3-cc5b91b65cf6", "https://ms.immowelt.org/4e649d99-0530-4699-a49c-1c2d54b75864/42ca3ca9-9bb9-463b-b699-93a83334ee83", "https://ms.immowelt.org/f687209c-d010-48d0-b7f0-d008c073c90f/f09cb602-c580-4bfa-977a-b78fc6c12a08", "https://ms.immowelt.org/10588fd4-5729-46fc-a950-a6b4f503f822/c4b5a180-0a63-4a89-801a-08495fade004", "https://ms.immowelt.org/1988d005-94ff-4366-824a-0a677ac1048b/ee762483-847a-487b-9a8b-43cb18c83601", "https://ms.immowelt.org/701b1fce-8ea9-4639-86ec-c876fb8d60c0/f85d54f8-97e3-4162-8128-9f10c36c696a", "https://ms.immowelt.org/063918a7-f509-4932-917f-6e97756cb928/5b9c3953-9989-4eb7-afec-653cbae3b849", "https://ms.immowelt.org/e89c2e3e-5bf0-406b-8e24-e497254debb9/b5b21bd8-cb20-4cda-8ab7-ce3244c40f72", "https://ms.immowelt.org/49831b1a-fce7-489e-bdf3-76f96d7abd5e/69dbfab0-97ce-4237-974d-eb8c8d54e2cd", "https://ms.immowelt.org/40098914-40dd-4139-ab0f-098a2932701f/5ae023e6-7b08-4d5d-b11c-7cbdf12d1eb2", "https://ms.immowelt.org/f5792c76-576c-4323-9097-78892bc73d7a/326861a6-cc9e-443f-b0e9-74d107bb6510", "https://ms.immowelt.org/f161e360-2dad-418f-8978-7403a69563db/2ff7a1f2-5d9e-4062-8844-5d0058909dfa", "https://ms.immowelt.org/5788e892-87e3-4272-8297-196413bdb41d/83782693-5404-4178-af87-f111ce69be6e", "https://ms.immowelt.org/8602c387-94df-4af2-a96b-96fa55ec0e6e/ee530b22-2e6d-4fb0-8050-f5a64133dff6", "https://ms.immowelt.org/486f43c7-bd90-494e-ad54-db9190a931aa/73b78181-d54b-4866-8f69-1af08d5ec696", "https://ms.immowelt.org/32fed4ea-fd60-48b1-bf9c-1ff2fad91246/8fd8016c-df0c-47fa-95f5-198192d9ce7f", "https://ms.immowelt.org/95ec384f-3bfd-488e-9f13-042aac27cda5/01ac96ae-4b3b-495f-9bd8-4ae62cabec7b", "https://ms.immowelt.org/398619b9-4081-4e83-b7d7-1c1ee8964121/64199e70-d8bc-4f27-9d36-ffc7ee133043", "https://ms.immowelt.org/9e944bc3-5e80-4825-a0a3-8d41b67b15ab/83a99408-4d6c-4aed-b27f-1127fb21ca17", "https://ms.immowelt.org/0d1ac5dd-ca4e-4c78-9fc3-1041acad6512/a946e1e1-dc5a-474f-84fe-5885560548f7", "https://ms.immowelt.org/651ae26c-78ee-4769-bad4-834192c9be7a/f7079b1a-b717-4ee7-bfc0-ab47a8128def", "https://ms.immowelt.org/03df58c9-b108-44ec-88bb-cb8c7d0ebd08/e285e4c0-d360-408b-8f11-a7f0b344f7ab", "https://ms.immowelt.org/1b5f727a-bef3-4da7-a041-e249c4bd8cb4/8489e8b8-18f8-4a8a-9944-36098d0905b3"]</t>
+          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Citywohnung - lichtduchflutetes, top gepflegtes Penthouse! Ideal f\u00fcr Paar oder Single!", "basicObjectPricEur": 1280, "basicLivingSpace": 88, "basicRooms": 3, "basicConstructionYear": 1998, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2agsm5w", "basicContactPhone": "09366/6543"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a54x5v"</t>
+          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -635,12 +635,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>554.99</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -650,49 +650,49 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>58.42</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>["FENSTER", "Kelleranteil", "Personenaufzug", "GAS", "Zentralheizung"]</t>
+          <t>["Personenaufzug", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Rottenbauer", "ZipCode": "97084", "LocationId": 496020, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1800", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Rottenbauer)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-rottenbauer/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1100, "Unit": "EUR"}, {"NumberValue": 20, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 900, "basicLivingSpace": 80, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a54x5v"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a5ll5v"</t>
+          <t>"https://www.immowelt.de/expose/2a7j75n"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -702,12 +702,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Exklusive 4-Zimmer-Neubauwohnung W\u00fcrzburg-Frauenland *Gartenstadt Keesburg*"</t>
+          <t>"Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1483.93</t>
+          <t>1181.21</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -717,49 +717,49 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>102.34</t>
+          <t>70.87</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>["Neubau", "gaestewc", "DUSCHE", "Kelleranteil", "Personenaufzug", "Erdgeschoss", "PELLET", "Zentralheizung", "DSL", "PARKETT", "FLIESEN", "frei", "abstellraum", "Tiefgarage", "REINIGUNG", "Loggia", "kable_sat_tv", "Kunststofffenster"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Hans-L\u00f6ffler-Stra\u00dfe 3", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1483.93, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 290, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3540", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1181.21, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 219, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 169, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1629.21, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/46db7f7a-e5d8-4eb4-a01b-a2d4e62ab2be/bb78636c-2f3f-4c2e-a53b-ef1fa9683a15", "https://ms.immowelt.org/b16389b6-eb92-42af-8130-0a76d6025358/fce845ed-0986-423b-8c1e-afd09a953917"]</t>
+          <t>["https://ms.immowelt.org/0d9ec1ef-21cc-484a-88ae-193c7267a3bb/1e78105c-6490-4468-a6c3-936b8b388b80", "https://ms.immowelt.org/5c55f670-770f-44e9-b26b-7c9164f4a76a/9f56e225-8915-45d3-9af7-0e36ad2d804e", "https://ms.immowelt.org/12a9fd2a-da00-49a5-9999-efb246a9d727/efc35e4b-a860-47d1-823d-1282d60e0bc6", "https://ms.immowelt.org/bb9a6b97-0d40-46d1-9b24-011a5dcc7508/40526838-218d-4a4c-9422-8bd98023d9f6", "https://ms.immowelt.org/1a701923-58c4-4074-92b3-3e6bc100d51c/2f4849ee-2b95-432d-8ed4-b41b0211a117", "https://ms.immowelt.org/4d6aee50-6e8f-423f-b67a-bd01a011592d/4d58cead-e166-4a77-8c0f-2ee869a9e824"]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Exklusive 4-Zimmer-Neubauwohnung W\u00fcrzburg-Frauenland *Gartenstadt Keesburg*", "basicObjectPricEur": 1483.93, "basicLivingSpace": 102.34, "basicRooms": 4, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Hans-L\u00f6ffler-Stra\u00dfe 3", "basicUrl": "https://www.immowelt.de/expose/2a5ll5v", "basicContactPhone": "0931/382-7701"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon", "basicObjectPricEur": 1181.21, "basicLivingSpace": 70.87, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a7j75n", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2am365w"</t>
+          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -769,12 +769,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Helle Wohnung mit Balkon in der vorderen Sanderau!"</t>
+          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>1183.37</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -784,49 +784,49 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>81.32</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1955</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>["Kelleranteil", "GEPFLEGT", "FERN", "kable_sat_tv", "Balkon"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "LocationId": 496022, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.400,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 190, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 890, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/0cd8c2fc-f0f8-4803-b570-0bc0474a7ed0/ff573215-5a42-4351-ba40-cfa78f0e290f", "https://ms.immowelt.org/9f20ac68-d479-4226-9c79-53570da7eb1d/e2de2ea2-5dcd-44f2-94d5-5e6076766679", "https://ms.immowelt.org/65a23389-315b-4e17-9a6f-c8bcf8e849a7/ef1d6fb2-36ee-4c22-9b98-1f57d5548397", "https://ms.immowelt.org/57d6c377-cfc6-48d1-a1d5-1088cf6393f3/bbd12d5a-7478-4c07-bfbf-ce2e86b907b4", "https://ms.immowelt.org/0a903ef0-4c0b-431f-af10-207debb8ec0e/ced5048e-e943-4b27-acce-5dba9b2424d9", "https://ms.immowelt.org/c5093796-6848-4a03-8695-1e10dfd39fb2/ee4c2860-ca11-43ee-b24a-c8691f01283c"]</t>
+          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Helle Wohnung mit Balkon in der vorderen Sanderau!", "basicObjectPricEur": 700, "basicLivingSpace": 58, "basicRooms": 2, "basicConstructionYear": 1955, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2am365w", "basicContactPhone": "0931 46079392"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a6kh5w"</t>
+          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -836,12 +836,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"neu renovierte 1-Zi-Wohnung in W\u00fcrzburg-Versbach ab sofort zu vermieten"</t>
+          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>950</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -851,49 +851,49 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>79</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1975</t>
+          <t>1911</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>["FENSTER", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche", "Balkon"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Versbach", "ZipCode": "97074", "Street": "Siebenb\u00fcrgenstra\u00dfe 2", "LocationId": 496021, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "900,00 &amp;a;#8364;", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Versbach)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-versbach/mietspiegel"}}, "DataTable": [{"NumberValue": 450, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 110, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 560, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/a43abc82-8ac3-4cab-a5b6-53bc82b3a86b/3a377faf-3eb8-4817-be74-cb42138a316c", "https://ms.immowelt.org/e7f30df8-dc76-47cb-9993-d30f406bd8d7/13c28acf-3d54-44f2-b940-4b8bdca4a9b6", "https://ms.immowelt.org/7093aa31-b326-4705-9fbd-9689f3f8db74/224d0bcd-b01c-4d21-bda9-75ebc02a4552", "https://ms.immowelt.org/60513d87-9ec5-4214-9438-9c82e1100233/0408ab34-5e7b-44a9-b736-d6039cff046b", "https://ms.immowelt.org/bb880bc5-4b45-4b22-9fe2-b905e66ae9d1/10cb98ca-5eaa-46e9-ba7c-515ddaf73266", "https://ms.immowelt.org/3f6c46dd-57a1-4a50-bee1-6913fdd35dc7/1a1e4495-8064-4237-9f2e-15ca8389d065", "https://ms.immowelt.org/1ad6bb21-d96d-4ba9-b01a-517a299fd375/faefc4fa-e636-4172-bd4d-3e933b48c285", "https://ms.immowelt.org/8c2bb07f-94a9-44fe-adcb-a12981d34755/81618401-0fc8-40af-9ff3-ea3b21b45879", "https://ms.immowelt.org/d14dc2a4-c385-48c9-81cc-a266c929d0f5/b3d185e0-37ac-4025-9318-bbf2dbb44558", "https://ms.immowelt.org/f689d644-a825-4147-bbe3-902acd0ca0e0/99e83e8b-81ea-4991-8d97-9873a562ab60"]</t>
+          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "neu renovierte 1-Zi-Wohnung in W\u00fcrzburg-Versbach ab sofort zu vermieten", "basicObjectPricEur": 450, "basicLivingSpace": 36, "basicRooms": 1, "basicConstructionYear": 1975, "basicCity": "W\u00fcrzburg", "basicStreet": "Siebenb\u00fcrgenstra\u00dfe 2", "basicUrl": "https://www.immowelt.de/expose/2a6kh5w", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2affg5v"</t>
+          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -903,12 +903,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"M\u00f6blierte Wohnung in W\u00fcrzburg/Mainviertel"</t>
+          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1125</t>
+          <t>532.19</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -918,7 +918,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>56.02</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -928,39 +928,39 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1957</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>["WANNE", "Etagenheizung", "moebliert", "Einbauk\u00fcche"]</t>
+          <t>["Personenaufzug"]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97082", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2.250,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1125, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/ed2e6e9a-a8cf-4e9e-89c9-92ebe0bd9ab9/3c8c330e-15e6-439e-be44-6f02de4b9dd5", "https://ms.immowelt.org/e963b58b-6a58-4830-8e37-e9e446a7ca40/edda2664-fb0a-48dc-bfe4-3b20c61c8b1d", "https://ms.immowelt.org/6945f917-297e-4dfb-b166-4245a2333e2c/5a890870-d05f-4063-b0e5-63ad31ca7572", "https://ms.immowelt.org/ffa99189-2ca2-46fb-aa14-f6fda02818ae/6a859704-19f9-4907-92f9-a5b7fcbe4248", "https://ms.immowelt.org/86e1504e-0c46-4800-a6e0-cf24601a2518/bf8eec93-53d3-4368-82bc-ca50c66a45a1", "https://ms.immowelt.org/f15519e3-ee04-4739-b40a-ce0f84fb29ff/2c2c7101-3482-420d-826e-9efd57863f1e", "https://ms.immowelt.org/54ea5d30-e104-4f39-8a41-429b5961bbd1/55bee8cc-3633-4bce-9b47-af1971f0523b", "https://ms.immowelt.org/e88c0a6a-0da8-4b88-8865-a9f37cbd0e2d/9452b370-8d6d-4324-8a35-57b8a433c48a"]</t>
+          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6blierte Wohnung in W\u00fcrzburg/Mainviertel", "basicObjectPricEur": 1125, "basicLivingSpace": 60, "basicRooms": 2, "basicConstructionYear": 1957, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2affg5v", "basicContactPhone": "+49 931 416616"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2adnh5w"</t>
+          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -970,12 +970,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg    Bezug ab 15.9. m\u00f6glich"</t>
+          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>1165</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>55.5</t>
+          <t>77</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -995,39 +995,39 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>["Neubau", "FENSTER", "Kelleranteil", "Personenaufzug", "GAS", "Fu\u00dfbodenheizung", "Einbauk\u00fcche", "Balkon"]</t>
+          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2400", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 800, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1000, "Unit": "EUR"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/ee16496e-0dcb-422b-b16e-d699f185c085/e0074c45-8e78-4192-9756-f9278eb48a3a", "https://ms.immowelt.org/34cd4c76-b8f2-4c80-aaa0-3ba60d1a14e4/c30f95d8-f7d1-41da-8ab7-64f008ba22e3", "https://ms.immowelt.org/7cdf79f6-934a-465d-ae81-272122e4ad00/69a5616c-d5ed-44db-890b-18a37c89f844", "https://ms.immowelt.org/730b7e47-988e-4c9b-b9ca-38230c929bbd/8d28dea0-8bbd-491b-8b5e-ed026c23978f", "https://ms.immowelt.org/5cf9e8f7-5445-4c99-bbfd-72ddff2dd761/b95383ac-aea0-4515-915c-88dcc18dbb15", "https://ms.immowelt.org/b67a10fc-cc10-4396-bbfa-844933e844e9/04dea6cf-8d76-4be7-8224-c27e2bf199c1", "https://ms.immowelt.org/de5686e9-6074-4e4f-9879-dae2270685a7/2bbe33f7-5d8e-4b72-8e50-965982c18903", "https://ms.immowelt.org/12bb0074-4492-41d7-aa45-4df0db4365ee/9d25213c-7c6d-4977-89f6-74f00de3ed8f", "https://ms.immowelt.org/537f0baa-9185-426f-adf2-579b2e0d97a6/da2fea6f-5ca7-490e-88ab-23aee1f38d29", "https://ms.immowelt.org/e53647b0-ae47-4085-8791-a49d5315fe02/535808f7-0bdc-48b6-8548-029216ba5437", "https://ms.immowelt.org/ea21f2d4-e176-4ff8-a99c-6939795da2d0/81b62de4-3f86-41a9-9f6c-8c455c7e4e51", "https://ms.immowelt.org/e99bbe16-63b1-4af9-af0e-9d7ef4382d36/eca8d831-a91c-45ad-b0e9-24c092aaf555", "https://ms.immowelt.org/2418511f-c9bb-4db5-88e7-cb4071afa55e/8809677e-7263-443f-a2cf-5cbf38323693"]</t>
+          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg    Bezug ab 15.9. m\u00f6glich", "basicObjectPricEur": 800, "basicLivingSpace": 55.5, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2adnh5w", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
+          <t>"https://www.immowelt.de/expose/2arkq5m"</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1037,12 +1037,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City"</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>2175</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1052,12 +1052,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1067,34 +1067,34 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>["GAS"]</t>
+          <t>["WANNE", "DUSCHE", "FENSTER", "Personenaufzug", "FERNE", "renoviert", "FERN", "Fu\u00dfbodenheizung", "Zentralheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Speisekammer", "Balkon", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "\u20ac 6.525,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 2175, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 450, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2625, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["https://ms.immowelt.org/1e8dcfd3-4788-4f09-a3c0-28d3414e57a3/5c7e81c2-8706-4ef4-8899-cfd4e8a5a029"]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City", "basicObjectPricEur": 2175, "basicLivingSpace": 150, "basicRooms": 5.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2arkq5m", "basicContactPhone": "0931/2706700"}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
+          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1104,12 +1104,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
+          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>474.53</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>49.95</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1129,39 +1129,39 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>["WANNE"]</t>
+          <t>["Personenaufzug"]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
+          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2av845v"</t>
+          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1171,12 +1171,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Helle 3-Zimmer-Wohnung mit Balkon"</t>
+          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1797.71</t>
+          <t>750</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1186,49 +1186,49 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>123.98</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1960</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "DUSCHE", "Kelleranteil", "Personenaufzug", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Balkon", "Kunststofffenster"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 1797.71, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 250, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/34aad469-3611-425d-9832-c02c7060cb23/77ba9d6f-e612-4962-9317-bd0107dc25f7", "https://ms.immowelt.org/8ea07a0f-c3a2-4e3e-a9d2-fe6544358d93/58dbc143-5e69-4062-9eae-b767cf0c69b1", "https://ms.immowelt.org/6b6cd2cc-a04d-480c-949a-1a21bbd7e1d4/51babd4b-8fbc-456a-862b-c4ebde7dc41a", "https://ms.immowelt.org/a8f09c5d-403e-4528-a15f-17ef6819f51c/15cf94e1-0865-4970-bdbc-7eeb2e4e321a", "https://ms.immowelt.org/a74342e9-df14-4a0d-b4c6-600423e5e886/caed2534-21fc-4d11-981c-a2164e56802b", "https://ms.immowelt.org/57b465e5-f400-4f58-8856-6a92ccb5dc5c/e24df36d-9d71-44a2-bd39-c0146b4df941", "https://ms.immowelt.org/4d380785-997d-4deb-b741-8c14d08622b6/d794011b-6b71-4e97-adb0-c319032680b3", "https://ms.immowelt.org/a1aeaa9b-89a7-4a5b-b3ed-598756319607/14a91c1a-5084-49dc-b75d-74d20228a8f0", "https://ms.immowelt.org/af2232f0-1ef7-4481-801f-2a5ff59e0092/96a901ff-03de-431d-886e-d860ac84fbc4", "https://ms.immowelt.org/eb83b1d9-acf0-4e74-b0b3-5fa3fcc1ca01/705ad620-364a-4237-968f-e9f4e0c3eb36", "https://ms.immowelt.org/b34e24ec-eac1-4eae-b4db-e1f386853cb1/292b937e-2528-4472-8123-fa7a878ef84b", "https://ms.immowelt.org/4111770b-ae7b-4dce-b625-f990d3c5ba1e/b7539eac-4bf3-4d62-ab60-f12720be1758", "https://ms.immowelt.org/73dc46c5-cb67-4432-b97f-e11d22268b50/6613c506-3bb4-4e53-a0ac-d3296fe50f9c", "https://ms.immowelt.org/d8083607-cc91-46ee-92df-9a6f4eed9d3b/59f57e14-612a-4c44-8a58-7436d9771597"]</t>
+          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Helle 3-Zimmer-Wohnung mit Balkon", "basicObjectPricEur": 1797.71, "basicLivingSpace": 123.98, "basicRooms": 3, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2av845v", "basicContactPhone": "0931/382-7702"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2af545v"</t>
+          <t>"https://www.immowelt.de/expose/2awv45u"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1238,12 +1238,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Exklusive Penthouse-Maisonette-Wohnung"</t>
+          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3030.93</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1253,49 +1253,49 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>178.29</t>
+          <t>123.36</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>["barriefrei", "WANNE", "gaestewc", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3030.93, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 360, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/2b7c4c91-7fac-4ddb-a032-3a51184dbb59/8f34d9b5-fec8-4e21-99c7-6f7a2921d4d1", "https://ms.immowelt.org/61a862a4-1bd5-4769-abb9-5e1d7113f8bc/88d5b2b5-7ef0-4388-8eb9-b7042670aee5", "https://ms.immowelt.org/37c438a9-8ae7-4d42-8006-bc3a55265670/12a6e3ea-2554-4920-bec1-7d536539c02d", "https://ms.immowelt.org/49abcb3b-4395-4691-8e92-b525edda30d4/f7c44e0e-0db0-456e-8cb8-845d816e37ec", "https://ms.immowelt.org/ce95a7e7-0ad6-4282-8ca2-5ce205488707/dbfb5e54-2bfb-4d01-91ec-1ca118a3a922", "https://ms.immowelt.org/b3cc6d40-e3b5-407e-ae5e-be0785a5a218/686cb7a1-8858-4011-a5e0-a8fd590fe4e6", "https://ms.immowelt.org/424d3898-11a5-419c-a472-b6bb5eed3e76/e7d72403-5394-43c9-a960-10468f29d064", "https://ms.immowelt.org/19d6858d-2cb5-437d-8cdb-6fb75d54c5e4/8e3114ed-77c5-47c0-8dce-725b44e8785c", "https://ms.immowelt.org/f536fdcb-a38d-4b90-beab-277e244cf6a7/ce23ee46-5ee8-4496-b672-c3ea031e92ac", "https://ms.immowelt.org/933295a3-d9da-4860-ad95-06490c6fddf4/182424c9-5902-4b40-be26-512097b49929", "https://ms.immowelt.org/a77d50f5-f8e0-4928-bcdc-2fa7c6e36e7d/05824030-0135-4ec2-93dc-52a0bf313587", "https://ms.immowelt.org/dbfe5771-25b1-460e-a2dd-140a19fae05f/4dd99d70-1f73-40c8-aab7-49051e0e90ec", "https://ms.immowelt.org/9689e92f-fdee-4ff1-99c1-89400857e515/a07a7b18-a41e-45a3-9fe1-f64211e577cd", "https://ms.immowelt.org/c3fdabd3-6c7c-4da9-9941-17117007bd14/16545b70-e49d-4309-85c5-a84123f7c8a2", "https://ms.immowelt.org/ec2b29d2-9e49-4ccb-965f-e26d155e848a/1c4de27d-2032-41cc-a466-04b10ad4f27d", "https://ms.immowelt.org/c2913eaa-8856-44c1-901b-0ae4b9a9ffa2/387a24b5-3c67-4740-ac58-0de078b68ff8", "https://ms.immowelt.org/81e05570-c572-4168-acf8-500cd9f74a65/796a2975-473d-4971-bd18-d2765832485e", "https://ms.immowelt.org/2c90ddab-a797-471f-a2aa-53b9ac172a1c/43c8617b-2da6-4fae-99be-395aaf2774e3", "https://ms.immowelt.org/24b3e778-e131-4042-ba05-7b63afaf1ce0/b0dfb227-b3fc-4605-b1c3-58573b4f24d1", "https://ms.immowelt.org/1d31929b-a5c2-410f-9bef-afc44f5e68c1/bc515335-0e9c-453b-bfcf-ae09a83fd65d", "https://ms.immowelt.org/d6e04616-c252-4d95-8d95-9d504b0fb3f4/07aa7bfb-71ab-4b13-bba6-99ba35097b80"]</t>
+          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Exklusive Penthouse-Maisonette-Wohnung", "basicObjectPricEur": 3030.93, "basicLivingSpace": 178.29, "basicRooms": 5, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2af545v", "basicContactPhone": "0931/382-7701"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ayb45v"</t>
+          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1305,12 +1305,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Gro\u00dfz\u00fcgige 6-Zimmer-Maisonette-Wohnung"</t>
+          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3601.44</t>
+          <t>580</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1320,49 +1320,49 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>225.09</t>
+          <t>44</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>["WANNE", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Balkon", "Kunststofffenster"]</t>
+          <t>["WANNE"]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3601.44, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 460, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/b888654a-7be0-4b1f-bb51-2d8dca6a1aa1/5dc0db39-67ad-4630-8a84-004692c1c198", "https://ms.immowelt.org/4cb98d26-30d4-40dd-9345-c05636fc3d6e/3d269755-d356-448a-a4e4-c9c9225867b0", "https://ms.immowelt.org/71ab24a9-6d26-4798-959a-526196ab2526/2338dbdc-85e0-452f-bbf4-cbd765176db2", "https://ms.immowelt.org/e212abae-27ab-4901-ad56-4abbf1ab429a/076c61fa-ae56-43bd-90cc-3d4a1f246534", "https://ms.immowelt.org/45fda28f-bd4b-477c-8e5b-025d3035fc24/25270c0c-e6f1-42be-9bc6-154afc390bde", "https://ms.immowelt.org/250e735d-28bf-4e41-a26e-10bdcc174a72/9ffa4901-709f-4a22-bcf8-4026af4845a8", "https://ms.immowelt.org/47738d72-90e1-400f-8f26-b0c89e0a04d4/b2671ee7-2150-4931-ae87-848ca314834d", "https://ms.immowelt.org/09239b5c-efed-4862-9be0-12284713015c/c50d605a-b30b-4c1e-b8c7-c377d0105c47", "https://ms.immowelt.org/32be8996-eac0-4fda-8211-2d8fadd6467a/c5cb6c3d-45d4-45e6-8603-f3cc8967b34e", "https://ms.immowelt.org/de7996d0-a07e-44a3-a014-b9f228303c3b/f4242060-e83a-4836-b64b-41645c5c5e94", "https://ms.immowelt.org/d9382006-8b3f-46eb-802b-250a8fca3f96/03f39cab-4da2-4c36-80c1-23a7fbd309fe", "https://ms.immowelt.org/36af7108-dfdd-4ff3-ab8b-6e92d3508062/2f20f749-7813-4534-bde5-1a624ad88952", "https://ms.immowelt.org/ba912dea-da2a-4abd-add2-64d03801c9f2/0f910eff-7ebe-4154-9f66-0556d0a42237", "https://ms.immowelt.org/469127b9-c85a-4e77-a7fa-af7365f65cc3/9cd962ef-da29-4690-9168-413036c7882b", "https://ms.immowelt.org/0341b685-a77c-4318-bf97-0b0facbf1946/c0c91076-cd90-41c2-8e29-c3d9b6bc4e76", "https://ms.immowelt.org/349ba8bc-380d-425c-9404-fe30348c76fb/be7df368-083b-4bf6-bb15-c9ee4809e9b4", "https://ms.immowelt.org/769d004b-9208-4258-b045-f78d35bbe304/cab7c6e2-a6fe-44e9-b980-49f912c4dc33", "https://ms.immowelt.org/32a4701e-f4a1-4e08-ac43-7f82a0871c0e/05462d50-f4b2-41fb-94fc-03251da46a31", "https://ms.immowelt.org/c3b62a14-8ad0-4bc1-ad12-407a7b7d45c1/1e082fb8-309d-48fd-9675-1e19df39056b"]</t>
+          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Gro\u00dfz\u00fcgige 6-Zimmer-Maisonette-Wohnung", "basicObjectPricEur": 3601.44, "basicLivingSpace": 225.09, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2ayb45v", "basicContactPhone": "0931/382-7708"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2akwq5u"</t>
+          <t>"https://www.immowelt.de/expose/2upu84s"</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1372,12 +1372,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"Hell m\u00f6blierte  2-Zimmerwohnung in W\u00fcrzburg/Frauenland"</t>
+          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1095</t>
+          <t>900</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1387,12 +1387,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>90</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1402,34 +1402,34 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>["DUSCHE", "moebliert", "PARKETT", "FLIESEN", "Einbauk\u00fcche"]</t>
+          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2.190,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1095, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/f58fd648-14ff-458e-b34e-ed1a79e43d74/d87e4e66-4884-409c-b2cb-2157459b3064", "https://ms.immowelt.org/0a87650a-5809-4688-8750-7ae6c25a4099/e24ce7b4-9191-4f35-a1d0-23492c9ab7b0", "https://ms.immowelt.org/791a160a-38a3-4dce-a18c-5ce7143fd3f5/bd4c9b95-f50f-4c31-a999-9365ab6d2f07", "https://ms.immowelt.org/d04e8834-3fb6-41c7-b54a-e8fbd81f4738/544118d8-4448-48cb-b903-f895e30a79c2", "https://ms.immowelt.org/0a28069f-f140-484b-8e74-4397443a7579/52a860be-e6e0-41df-ad9f-635a12c08567", "https://ms.immowelt.org/93620f2c-07ac-40ae-89e8-09de2a90ffff/0aad3bf6-a9a2-41e4-841c-299b26265c3a", "https://ms.immowelt.org/a67d6581-3a59-4dc4-a4f3-965a7168620b/da1adff0-5907-4ab5-8913-e075b2d30c48", "https://ms.immowelt.org/deeb3874-cc27-4a7f-ac51-854d6765dd3f/3218f2ca-a245-4045-af54-619a9b8882e3", "https://ms.immowelt.org/ac67f904-20c4-4c6b-90f1-3d808fa8dae1/795689c7-539e-470a-a2a4-32e423451bd3", "https://ms.immowelt.org/974474bd-d9e3-4117-a672-6922106d164c/a2bb49a6-741b-40b0-8a0b-40d9f75d0f02", "https://ms.immowelt.org/936ffd96-d118-4d3d-8f77-ff73d6726300/5bb5b59e-9b1c-44ee-816e-31d9b28dd5a2", "https://ms.immowelt.org/9e5f7e76-6418-46d5-af9c-45309a550a97/c9909e8a-e4cd-4d4e-826e-4ec43a4165d9", "https://ms.immowelt.org/fc5c4ab6-6dd7-402d-aa17-1d5f9d8e29b0/f9213bf7-281b-4c08-8f0b-e78f6fcb7c71", "https://ms.immowelt.org/efbfc541-75da-4200-8395-1db7a9483e5b/68140100-e86c-4af6-88d7-26d0e819a523", "https://ms.immowelt.org/6069128c-8b73-4678-abc6-ee0b63823860/cceb6f64-a341-4849-9927-b2c5dd025aad", "https://ms.immowelt.org/c13a4106-75b6-444b-87e0-05ccdb99308c/a077d4b3-99d4-474b-b40f-6be9110341d9"]</t>
+          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Hell m\u00f6blierte  2-Zimmerwohnung in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 1095, "basicLivingSpace": 63, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2akwq5u", "basicContactPhone": "+49 931 416616"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a9245v"</t>
+          <t>"https://www.immowelt.de/expose/2aebr5t"</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1439,12 +1439,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"Neu m\u00f6blierte Wohnung im Herzen der W\u00fcrzburger Altstadt unweit des Marktplatzes mit Wlan"</t>
+          <t>"Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!"</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>815</t>
+          <t>1290</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1454,49 +1454,49 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>93</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert", "TEPPICH", "FLIESEN", "Balkon"]</t>
+          <t>["Neubau", "barriefrei", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "PELLET", "Fu\u00dfbodenheizung", "Garten", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "Eibelstadt", "ZipCode": "97246", "Street": "W\u00fcrzburger Strasse 25", "LocationId": 11869, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.630,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 815, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2600", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Eibelstadt", "Link": "https://www.immowelt.de/immobilienpreise/eibelstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1290, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1570, "Unit": "EUR"}, {"NumberValue": 40, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/56dbfa19-0b11-4212-a585-a3bb9055fc6c/55af236d-1cf3-446a-a9ea-5d847c1f3c78", "https://ms.immowelt.org/2321a506-3294-4da0-8ed9-9c32a877cc19/568e9ef6-6f64-4112-9523-9eaf25a3f970", "https://ms.immowelt.org/c49d4e0e-c519-4110-bf9d-48d46975f264/51ad8f90-ae3d-4f54-9436-a3ce93d787e0", "https://ms.immowelt.org/1efec59d-a37f-4e4e-81e0-d2638e029208/c9bd61b7-4af9-4819-822e-916b4c491efd", "https://ms.immowelt.org/35f3c816-30ad-4cfa-a370-9fd3df5a890b/0f5a8622-ff9b-48a3-b656-48f75cd9c811", "https://ms.immowelt.org/1d11277d-e06d-43d1-807a-35d99c5f5cd5/51935719-85d7-4a46-a718-1c1a7bedba2c", "https://ms.immowelt.org/3f9f17e0-3b0f-42d8-9623-bd41d7d12fc4/d88f57cc-ca14-47d1-b0ac-e5d037c3114a", "https://ms.immowelt.org/4c16ccd5-7611-496f-9fc2-a5cc9e95ca96/0cc9afbf-324b-4dc0-a841-e5417e3c909f", "https://ms.immowelt.org/23f4ce8d-d0f3-42f3-b7c2-cbea89a39473/eb285820-0b71-4189-8a94-494d832c127b", "https://ms.immowelt.org/36d590ab-2de9-46f3-8cef-b4af4efd9be0/8e11440a-7fe1-49cf-a002-13e4285760be", "https://ms.immowelt.org/8099beb8-56a4-493f-b95f-2490484605d5/fbb624d4-8b55-48d5-8b8f-5535a08872c5", "https://ms.immowelt.org/1978dbc1-a0ed-458a-abcd-d22f103809ef/1a5cc04f-0b65-48af-8e69-c835714ab2e7", "https://ms.immowelt.org/6b1ab129-3f95-42da-9d53-8088db0a9349/25c6e471-016e-4261-b4ae-a73987e4f403", "https://ms.immowelt.org/9b310d23-aa9d-41f5-8f34-29a9b7aa4471/bae39b36-c4b5-4cf8-882a-aca3ba40538c", "https://ms.immowelt.org/20713457-85cd-4f26-970b-eca4af0b6b71/be6308f1-d0c9-4aa5-8a10-3a4f1f28ff33"]</t>
+          <t>["https://ms.immowelt.org/7c821767-b600-4ad9-8a2a-50874a2a87cf/92a3b2aa-0393-4e55-ad97-c6c3a803a0d8", "https://ms.immowelt.org/8081e4f6-2ad6-46c7-957d-07597db5c5a8/ee5c7a33-80cd-4c89-bb96-98be1b013e27", "https://ms.immowelt.org/515a3a85-6263-4990-b640-f75ec6075c4b/8456cc16-2fc0-409e-ba1f-f103285c6d18", "https://ms.immowelt.org/340c6f6f-746d-421c-aab8-4850f62a5e6b/e971e1c3-7527-4fb5-a83c-f5221d132bc5", "https://ms.immowelt.org/6205eb16-8906-4267-a472-86439d570e9c/39733ff0-9850-43ab-a6fa-f4f2291ba17d", "https://ms.immowelt.org/3b9c4f71-f8fa-46fa-a1d6-7bab696693cb/eccec98b-d098-4d62-ae2c-f62c71c18721", "https://ms.immowelt.org/ab60445b-088f-4fe5-9554-7448a4a29bb2/0eb8642f-4cb3-4252-b4b5-622b757475d6", "https://ms.immowelt.org/6b12d3cb-5e11-4c67-9c0e-a69e674fc018/3d35f5b5-f31d-4200-8572-5eb83a1079e5", "https://ms.immowelt.org/11466902-020f-43ec-9441-09395d524b18/3136e448-448b-41f8-bcec-58fea52abdd5"]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Neu m\u00f6blierte Wohnung im Herzen der W\u00fcrzburger Altstadt unweit des Marktplatzes mit Wlan", "basicObjectPricEur": 815, "basicLivingSpace": 40, "basicRooms": 1.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a9245v", "basicContactPhone": "+49 931 416616"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!", "basicObjectPricEur": 1290, "basicLivingSpace": 93, "basicRooms": 3.5, "basicConstructionYear": 2022, "basicCity": "Eibelstadt", "basicStreet": "W\u00fcrzburger Strasse 25", "basicUrl": "https://www.immowelt.de/expose/2aebr5t"}</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2agwq5u"</t>
+          <t>"https://www.immowelt.de/expose/2asr65p"</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1506,12 +1506,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland"</t>
+          <t>"Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld "</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>649</t>
+          <t>1100</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1521,49 +1521,49 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>103</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>1984</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>["DUSCHE", "Personenaufzug", "Zentralheizung", "moebliert"]</t>
+          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "renoviert", "GAS", "Etagenheizung", "gartennutzung", "Einbauk\u00fcche", "wg_geeignet", "Balkon"]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "LocationId": 496008, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "Street": "Unterer Kirchbergweg 37", "LocationId": 496013, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.298,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 649, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2200,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1400, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/cf8697dc-afcd-47ae-aadc-64c4cc78569c/35b4d352-660a-4816-94a6-619497123ae8", "https://ms.immowelt.org/a32b8f72-a566-4394-bea1-04e883e8fce2/7099cff9-9eea-4d1f-bad4-4033626afe54", "https://ms.immowelt.org/105a8a3c-c718-4c20-83ac-d0a5ef1a7f53/9db73218-715a-4963-942c-e41a29ef7b07", "https://ms.immowelt.org/64d9efa5-0a66-44fe-aa1e-b89f834ad546/6f687f3d-4a05-4f47-a1f8-8b78ca7e8bfe", "https://ms.immowelt.org/a3fe7335-2ba5-4c30-a137-cbfb5fd2a35c/20496698-5e1f-4243-9338-f56821682d4a", "https://ms.immowelt.org/a449833e-f4f4-43ff-8ebf-01bc5160e5c9/ccc566af-477b-4888-b03f-1cc64f4f1c45", "https://ms.immowelt.org/a6d17184-1155-46e9-af2c-d83d9e1be344/aab72d40-469f-486c-9add-806a5481ac6a", "https://ms.immowelt.org/a5271f16-acef-4db4-84ba-2b1a9ddc5892/57e11dd6-6321-45eb-85e0-aaa0f1e15bfe", "https://ms.immowelt.org/921ae069-2035-4dbb-a619-8ad9012a2442/0e6324ba-04b0-4141-bcc2-3b6cb33ac8ea", "https://ms.immowelt.org/6dc638c1-e4cd-4f0c-87b2-169cc34b0bd8/2af01fd5-93ce-4fc8-ae87-9a3817a2ef84", "https://ms.immowelt.org/a5894c49-800c-4d59-bb53-e598cf560634/0aa6a439-1071-40bd-a3ef-3bd2192fad8c", "https://ms.immowelt.org/1824d009-9f1e-4248-ac1b-d6198f9c17f3/ffd7b610-0d17-43b2-b15c-614cccf8be14", "https://ms.immowelt.org/45f31b8e-c2fc-45ff-8dac-c0bf8fea6e03/a11c6ffd-ddba-4524-9aca-520b2604d193", "https://ms.immowelt.org/5ec8ff49-d6b8-4dd0-bd1b-a04062520b58/b2e43f71-c2eb-4713-a428-6da937a58826"]</t>
+          <t>["https://ms.immowelt.org/bbd4dcbf-c64e-4c60-9789-afc66db53a3f/7fc04ce4-7f84-4ce5-8111-31fcc917306c", "https://ms.immowelt.org/315ff83e-d234-453a-ad52-c4b99bef7055/a979f182-320d-49d1-8002-bcde353d36ee", "https://ms.immowelt.org/6137c704-6a29-47ae-a5a3-88abd0a2fde0/d535204c-f43a-4229-8152-507fc644a211", "https://ms.immowelt.org/1981c2ad-23cb-41f4-825a-77d67f5fbbe7/e968ecc9-ea46-4188-a2c4-968720f069c0", "https://ms.immowelt.org/a4965ee1-de2b-4d90-8333-b793f90a7406/867d9997-6f27-48da-ade0-9096bf31cf3e", "https://ms.immowelt.org/aed0a388-445d-4f8f-9afd-4a146b35d962/3bc7e507-92a3-446a-a3f1-5799c1df7338", "https://ms.immowelt.org/f9d8ba2e-fb1a-4cdd-98ea-ba6ba4973c25/fde9d74e-bd14-4413-a148-81aad236c43f", "https://ms.immowelt.org/e0fbe89c-ecbb-41e9-9ecd-61c2762b9189/3784b2d8-f66d-4f7f-a893-cb9c7b3e982c", "https://ms.immowelt.org/16af38b3-f1c4-4d16-ba17-2685efc0dbe6/b5361690-0608-4e15-8167-e5ab29ac41e7", "https://ms.immowelt.org/fb842589-0c99-45bb-b567-5d04f811adf5/729e7fb7-c4eb-47db-936a-8a406b3efda8", "https://ms.immowelt.org/2f97e2d2-4fcd-40db-bee9-5d4161812bb0/a57df980-0cf8-4352-8cf0-5e867376c343", "https://ms.immowelt.org/79cf67c5-73a5-4097-8b85-e20df2ab786e/363fc58b-d0d5-4f6e-afda-b1d880cf8747", "https://ms.immowelt.org/d9ae7b88-e98c-4d7f-8096-8ede0076f326/e28b854c-9b59-46d6-84a5-28d2595f9ff2", "https://ms.immowelt.org/dffe6319-03a2-4071-98a5-e0f1e3954460/de63d734-7d33-492b-acbf-be5ca5b61e49", "https://ms.immowelt.org/8af5caf8-2627-4044-83b1-a3824003abcd/a9a95b7e-658f-4e56-989c-5a564997561b", "https://ms.immowelt.org/de373ea2-fa91-495b-aa05-ffa24233b025/ff4e0de7-6c79-411b-bec2-3f5b973c460c", "https://ms.immowelt.org/1db3601f-db1c-4e6f-8b1d-e2f17c88804b/e84274ae-8668-49f0-8327-447ff8511752", "https://ms.immowelt.org/6bc525ad-0769-42c3-aaff-a169a251a660/789b8d1b-633d-4989-a0e8-50949ea51d51"]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "M\u00f6bliertes Apartment in W\u00fcrzburg/Frauenland", "basicObjectPricEur": 649, "basicLivingSpace": 21, "basicRooms": 1, "basicConstructionYear": 2015, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2agwq5u", "basicContactPhone": "+49 931 416616"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld ", "basicObjectPricEur": 1100, "basicLivingSpace": 103, "basicRooms": 4, "basicConstructionYear": 1984, "basicCity": "W\u00fcrzburg", "basicStreet": "Unterer Kirchbergweg 37", "basicUrl": "https://www.immowelt.de/expose/2asr65p", "basicContactPhone": "0931/60565", "basicContactMobile": "017683299994"}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2abty5v"</t>
+          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1573,12 +1573,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"[TAUSCHWOHNUNG] Wundersch\u00f6ne helle Altbauwohnung"</t>
+          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>430</t>
+          <t>2880</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1588,49 +1588,49 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>195</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 430, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 115, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7a4af935-fdca-42b8-b470-a905b68d671e/717dc8fc-8461-4d19-89e3-3eaf6c5bfb76"]</t>
+          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "[TAUSCHWOHNUNG] Wundersch\u00f6ne helle Altbauwohnung", "basicObjectPricEur": 430, "basicLivingSpace": 64, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2abty5v", "basicContactPhone": "+4922892939484"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a4kg5w"</t>
+          <t>"https://www.immowelt.de/expose/2almm5r"</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1640,12 +1640,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"2-Zi. Penthouse Wohnung  mit gr. Terrasse, teilm\u00f6bliert, N\u00e4he Uniklinik"</t>
+          <t>"TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>1700</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1655,49 +1655,49 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>153.3</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>["Neubau", "Kelleranteil", "GAS", "Zentralheizung", "moebliert", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "GAS", "Zentralheizung", "teilweise m\u00f6bliert", "TEPPICH", "PARKETT", "FLIESEN", "Einbauk\u00fcche", "offene K\u00fcche", "Stellplatz", "Tiefgarage", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Lindleinsm\u00fchle", "ZipCode": "97078", "LocationId": 496017, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Gartenstra\u00dfe 9", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1500", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Lindleinsm\u00fchle)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-lindleinsmuehle/mietspiegel"}}, "DataTable": [{"NumberValue": 700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 900, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5.400,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 1700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 240, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten", "Comments": ["in Warmmiete enthalten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2340, "Unit": "EUR"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/5ffec635-8f46-4cc1-aadb-8b583ac94f49/a055949a-2702-4368-b5b3-7b0ed426b642", "https://ms.immowelt.org/8908f348-9991-4a07-ad66-d7d75614e10a/fca9e8be-88e9-418f-a5eb-9e0d5767a5f4", "https://ms.immowelt.org/cc8d5f7e-0ed9-47a3-818b-45790a8111fc/1ff9a9de-b0c2-4a71-935d-2fd2d9164ad1", "https://ms.immowelt.org/e595bf82-bf35-4dea-bb76-166a24244d92/420389cc-e1aa-4a32-94b8-9d099fca203b", "https://ms.immowelt.org/2512e689-4ae0-4ff9-9611-9f151ac18678/c4e6c45b-c697-41d7-a51f-d244d8f1a417", "https://ms.immowelt.org/e0483e5d-da13-4926-a03f-c238c4a327ae/737d7425-941f-4ec9-a90e-14f51213a74f", "https://ms.immowelt.org/23fe53b7-3d5a-4509-a222-5cb8ed3d516c/a46ccbc0-6aef-4e2f-ac21-6d245e72052d", "https://ms.immowelt.org/349313e4-73e0-40b7-b119-9fe817365e7a/7f23958c-275b-4a0e-8d30-ad6e79f317f7", "https://ms.immowelt.org/ac9b1a48-16e2-4119-98ba-9a1a890ff38b/c3716b49-d728-4b6a-900b-7d66e9cd4354", "https://ms.immowelt.org/e3084b71-0919-4d54-96d4-4d35ce184a9c/c4edd6a6-581b-4387-81e6-1df5e276dda7", "https://ms.immowelt.org/fa543343-fde7-4b91-b370-eee9cd1e0f90/62763f8c-bf88-4f8a-bbfc-b721085c2412", "https://ms.immowelt.org/2a737240-80f0-4710-a8f3-7c4f1c3f6233/08bf7007-717d-4120-b7cb-50bf91a1393b", "https://ms.immowelt.org/727ce8f8-3e8b-4da9-95ec-b855705005c5/07256d94-2372-4172-b756-d7101c994e5e"]</t>
+          <t>["https://ms.immowelt.org/338d1cbc-cb3f-423f-8523-42cc120d72f9/e4b563bc-671f-4dea-a726-71d7b9386009", "https://ms.immowelt.org/4da068e4-1a27-465c-b0e7-ffb77b79880b/908c43fa-aa39-4e85-97c8-98295a3c363c", "https://ms.immowelt.org/cab19ffc-0f4a-42a9-89e9-7189e9dafd92/2a5e6769-ad31-4185-a454-e8d753be9cdb", "https://ms.immowelt.org/f6511334-9f04-476c-9659-9f19a5df115f/ff04d8f5-f770-493d-9394-6ac1a456d4ef", "https://ms.immowelt.org/733f5f85-bc20-4e60-ba25-388eeb6563cf/4094751f-b73c-432d-b6b4-6d68ba45d6d9", "https://ms.immowelt.org/05e1b42e-75a4-4206-aaad-48ffa57f162d/a3aafbff-20b6-4c17-a8a1-b916eb14b8aa", "https://ms.immowelt.org/1233e75d-2ab4-4291-8b67-e87c5a4898f1/6153dd66-9325-4066-80d3-ed8642487cd8", "https://ms.immowelt.org/99f6825d-9789-4ae1-9a78-4e6acb5853a7/f727c1c7-69a0-420d-adf8-9119f5849a16", "https://ms.immowelt.org/19d94014-cd12-4f9a-81a5-8f9745f63b90/48988be8-85bb-4980-a25a-276af2606ac6", "https://ms.immowelt.org/f351ce35-7e50-4939-b806-4f6dc375cc86/84c997d9-1332-4173-9248-fb7b75a10943", "https://ms.immowelt.org/cdd250a7-47f6-4535-ac59-6ea51157c95e/bed7b410-ef26-42d6-a562-595eafba5999", "https://ms.immowelt.org/644f0235-e6ba-482b-bb26-2fea622cd4a1/6d2746f3-ea97-4996-8617-e82aeced34e0", "https://ms.immowelt.org/0174f587-e7b3-4c39-8603-c1d8465305ec/508d427a-f8c5-4d05-bd55-06ee858889be", "https://ms.immowelt.org/e3dbe0a9-b856-43a6-97a0-ca238574c6f8/f20530d2-b140-4eb5-b229-ad329853d7f3"]</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "2-Zi. Penthouse Wohnung  mit gr. Terrasse, teilm\u00f6bliert, N\u00e4he Uniklinik", "basicObjectPricEur": 700, "basicLivingSpace": 47, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a4kg5w", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE", "basicObjectPricEur": 1700, "basicLivingSpace": 153.3, "basicRooms": 3, "basicConstructionYear": 1998, "basicCity": "W\u00fcrzburg", "basicStreet": "Gartenstra\u00dfe 9", "basicUrl": "https://www.immowelt.de/expose/2almm5r", "basicContactPhone": "0931/45466333", "basicContactMobile": "0175-5994950"}</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ay645v"</t>
+          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1707,12 +1707,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Wohnanlage Alte M\u00e4lzerei - Haus 5 - Ger\u00e4umige 6-Zimmer-Maisonette-Wohnung"</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3163.32</t>
+          <t>420</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1722,49 +1722,49 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>218.16</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "DUSCHE", "FENSTER", "Kelleranteil", "Personenaufzug", "Erdgeschoss", "kontrollierte Be- und Entl\u00fcftungsanlage", "LUFTWP", "ELEKTRO", "ERDWAERME", "Fu\u00dfbodenheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Garage", "REINIGUNG", "kable_sat_tv", "Terrasse", "Kunststofffenster"]</t>
+          <t>["GAS"]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "Street": "Frankfurter Stra\u00dfe 81", "LocationId": 496026, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 3163.32, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 440, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/33a10e2d-1546-47e8-8bf4-47024f96365d/8d31a374-f6c2-4671-ba5e-b06a8d7c1f18", "https://ms.immowelt.org/e715d610-ea80-4459-9e3a-1ea8a574c0d7/c594e925-e9d3-4474-88ff-ee637dc4b81a", "https://ms.immowelt.org/f3e49668-7602-45ad-979f-f68f0c60ad46/6da2c38a-e66f-4112-b3c3-70ebaa38a22f", "https://ms.immowelt.org/e4691abb-17a5-41aa-949d-88daa0ab8d3a/42a9ae4f-34fd-4230-8329-9c00ba557222", "https://ms.immowelt.org/62981e85-dc6c-481f-8d77-c7e82c11d711/a90f265f-b3b3-4b6b-a854-a05b00191bac", "https://ms.immowelt.org/c1f1f311-d95b-465f-94a6-317a246989d2/e96a7cca-1527-484c-a8e9-f79e1cf28136", "https://ms.immowelt.org/935854af-6f17-4d5d-b023-6647d4cc8d4d/87cabb52-19fe-4dca-a81d-9b0f6d4daa7c", "https://ms.immowelt.org/d22f872e-159f-4f19-bb2a-75f5b228899d/044b33f6-2258-490a-ae2a-52d9ce17b653", "https://ms.immowelt.org/58dca412-8d3b-415e-9a26-359678019657/0858d4e1-5dc0-4297-8a4f-b5db5dbeb8b8", "https://ms.immowelt.org/f9bab463-404a-46c6-990a-559df575f251/6d53c5c6-d652-4e1d-98e5-448095327b4f", "https://ms.immowelt.org/6559ac4a-0154-4e05-a366-dbf71d55ad3a/29c1a7fd-15be-4a1b-91ca-9db0f1c442f3", "https://ms.immowelt.org/85c20839-cb59-4728-be4d-78d1ffcb9274/f88983a1-2f68-4f01-af1a-cae1794eb9e4", "https://ms.immowelt.org/f0a33cc2-272c-4fe9-a229-0c65344655fb/1911e15f-4afd-4691-a583-109b097d5b1a", "https://ms.immowelt.org/26da2883-f715-4c66-a8d1-3e2b9550fcf3/90d1f6cc-c1ae-4b39-889a-79bf683b589e", "https://ms.immowelt.org/b51072d7-8214-4cb3-b4f1-4c2d9c08cc58/e2548663-d3a0-4cb8-b0f7-5aaacf362ba3", "https://ms.immowelt.org/b5dd6e96-9575-46aa-af37-c7a1914335de/e4d4ff07-527e-4aff-be0a-66c047b2b747", "https://ms.immowelt.org/4c4b10ce-78b2-449d-a1c4-38ef2035555b/8094732c-995f-4ee6-af5f-e52e6a68bac8", "https://ms.immowelt.org/36750323-149d-49f3-8859-a599078cdc7a/0c862b3d-b2f3-4b3a-b234-8e9299775647", "https://ms.immowelt.org/d1d807de-1e05-4eca-b9fd-01dd45660714/8d6cc502-9779-4a2e-bfea-d50b253ff0f3"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnanlage Alte M\u00e4lzerei - Haus 5 - Ger\u00e4umige 6-Zimmer-Maisonette-Wohnung", "basicObjectPricEur": 3163.32, "basicLivingSpace": 218.16, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "W\u00fcrzburg", "basicStreet": "Frankfurter Stra\u00dfe 81", "basicUrl": "https://www.immowelt.de/expose/2ay645v", "basicContactPhone": "0931/382-7708"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aeal5v"</t>
+          <t>"https://www.immowelt.de/expose/2uewf4g"</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1774,12 +1774,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"**Erstbezug** Renoviertes Studenten-Apartment nahe Uni Hubland und Wittelsbacherplatz"</t>
+          <t>"Boutique Wohnung m\u00f6bliert mieten"</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>415</t>
+          <t>1100</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1789,42 +1789,42 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>55</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>["DUSCHE", "FENSTER", "Souterrain", "GAS", "Zentralheizung", "LAMINAT", "FLIESEN", "frei", "Einbauk\u00fcche", "Kunststofffenster"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Rottendorferstra\u00dfe 55", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "830", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 415, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 145, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/a3c1d1a9-92f0-4260-b2b3-41eb1b7cb966/c490aefe-bdcb-4b73-9783-a0bcc158c257", "https://ms.immowelt.org/b05abc2c-f624-4093-86a5-80f153fa6197/05af8f24-b7e4-4ba5-872c-39eed41b4cb5", "https://ms.immowelt.org/5be4bd8f-231a-44d8-8f0b-608a4f6581bd/0af81664-7d97-498f-8adf-3b5b5fe348ae", "https://ms.immowelt.org/725fb4fb-900c-4cd8-9554-dd83fc7bd725/99474ade-0e13-4d47-bf95-373cf4af43ec", "https://ms.immowelt.org/a0bb9c06-d60a-40e4-9521-94d9c183a14d/93799d3a-657d-4385-b487-2691349273e9", "https://ms.immowelt.org/3b4d1b7b-a5fe-4a37-b98d-6fc308d03c5b/c80e2b27-9270-47ef-b292-eb1efd72ee07"]</t>
+          <t>["https://ms.immowelt.org/a13c7ad0-2b70-4b4d-a3ea-a34885d87b08/ec7d0988-cc69-4927-b78a-e0331046ca91", "https://ms.immowelt.org/fde8fa3b-e4a0-4ded-a7b8-8420d1a01a9f/d1572cf7-7d4c-4a02-98e6-2d6e2eaf2b62", "https://ms.immowelt.org/44adf4be-fce6-455d-9181-c27144d0b47e/2f83da82-fc2a-4b88-be4c-03e254e651ef", "https://ms.immowelt.org/ecad88ed-f5a2-43ee-9dac-2470c0ec1f30/b45f2c26-817a-4b2e-8c51-b6b4e1ffdb1d", "https://ms.immowelt.org/38e4f785-7a20-46ce-bc01-3909054d335a/ad336fba-e265-4254-b66b-537222384071", "https://ms.immowelt.org/1e7916ab-6c4d-4283-a5fa-b6ccb79f8f6e/58a84848-235f-402d-a541-f5f6b47652ab", "https://ms.immowelt.org/1160b145-63b1-49fd-9bc5-54104f7bf183/20f3af07-2776-4471-981e-ff09df9d66a7", "https://ms.immowelt.org/1498b260-43eb-4602-8d7d-ad06837fbc82/adf6d355-f74c-45b5-bfa8-b60c2f35c3b9", "https://ms.immowelt.org/3606502e-37fa-4430-9bd8-fe84c0031264/e4a61da6-7999-4ec3-b472-e1f89796a906", "https://ms.immowelt.org/d2aadef4-121e-4c0a-8d0a-767393cc0b74/6210ad93-fbc0-4207-8cf8-9c21f2312742", "https://ms.immowelt.org/477b2242-e6a2-4599-8d7d-52d225d39692/c3547552-3022-4c61-8d1c-52b44db4589a", "https://ms.immowelt.org/b6435004-0e35-4fc6-b7d5-548a1c6bd865/18ecd94d-aeb5-4db7-9ece-c9056b7c18f5", "https://ms.immowelt.org/fffca264-e9b1-4647-8e64-c60be93744f8/191162cc-7517-4fc6-be4a-5a945715134c", "https://ms.immowelt.org/93d1fc99-9be1-4826-a8df-e3a22d03c005/b7d69f86-c033-49d5-941d-d0decd68be56", "https://ms.immowelt.org/3593ecfa-644d-4979-ae0d-0fc4d4e9ae7a/1ec892e1-00ff-49d2-b6db-03c288ea7d6d", "https://ms.immowelt.org/19ab9c79-4170-4a92-b48b-ed773d6437fd/7b0670d3-4d77-4ec4-919e-937dab966ff8", "https://ms.immowelt.org/b4d5be21-2515-403f-8215-e2eb79cc92db/3cf8ef03-8de3-42ff-929d-ff3a020a5b25", "https://ms.immowelt.org/b2b6d755-c0f3-4890-a478-6ac51ea07508/68baa9ce-b806-47ca-8c89-b3ed586305cf", "https://ms.immowelt.org/cc54eb68-d41d-4945-85c5-cc8e8c9b5e81/e3d73054-2d37-4c41-8117-5dad34c03029", "https://ms.immowelt.org/8f0aea64-d4d8-47a0-a269-0ddfd36d2981/93df92fb-6eae-41b6-8679-00bb4a30474f", "https://ms.immowelt.org/824566f0-3a4c-4806-a951-d3eecde604c1/9e360642-24e2-44c2-94e2-d1336be6f715", "https://ms.immowelt.org/edc590e2-19f1-4a3d-8938-add9dfc4b56f/db68466a-1681-4bf8-85cb-489b4ffa5436"]</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "**Erstbezug** Renoviertes Studenten-Apartment nahe Uni Hubland und Wittelsbacherplatz", "basicObjectPricEur": 415, "basicLivingSpace": 26, "basicRooms": 1, "basicConstructionYear": 1950, "basicCity": "W\u00fcrzburg", "basicStreet": "Rottendorferstra\u00dfe 55", "basicUrl": "https://www.immowelt.de/expose/2aeal5v", "basicContactMobile": "+49 176 21469496"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Boutique Wohnung m\u00f6bliert mieten", "basicObjectPricEur": 1100, "basicLivingSpace": 55, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2uewf4g", "basicContactMobile": "0171-9546505"}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
MLFlow run triggered automatically
</commit_message>
<xml_diff>
--- a/immowelt_price_guide/data/retrain_train_data.xlsx
+++ b/immowelt_price_guide/data/retrain_train_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>ContactData</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>BasicInfo</t>
         </is>
       </c>
@@ -491,7 +496,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
+          <t>"https://www.immowelt.de/expose/2arkq5m"</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -501,12 +506,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"Bestlage mit Festungsblick"</t>
+          <t>"Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City"</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>610</t>
+          <t>2175</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -516,12 +521,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -531,34 +536,39 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
+          <t>["WANNE", "DUSCHE", "FENSTER", "Personenaufzug", "FERNE", "renoviert", "FERN", "Fu\u00dfbodenheizung", "Zentralheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Speisekammer", "Balkon", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "\u20ac 6.525,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 2175, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 450, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2625, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
+          <t>["https://ms.immowelt.org/1e8dcfd3-4788-4f09-a3c0-28d3414e57a3/5c7e81c2-8706-4ef4-8899-cfd4e8a5a029"]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"companyName": "Werner Fleischhacker Immobilien GmbH &amp;a; Co. KG", "address": {"city": "W\u00fcrzburg", "zipCode": "97072", "street": "Valentin-Becker-Stra\u00dfe 8"}, "salutation": "Herr", "firstName": "Werner", "lastName": "Fleischhacker", "phone": "0931/2706700"}</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City", "basicObjectPricEur": 2175, "basicLivingSpace": 150, "basicRooms": 5.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2arkq5m", "basicContactPhone": "0931/2706700"}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
+          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -568,12 +578,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
+          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>566.96</t>
+          <t>474.53</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -583,7 +593,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>59.68</t>
+          <t>49.95</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -598,7 +608,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>["Stellplatz"]</t>
+          <t>["Personenaufzug"]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -608,24 +618,29 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
+          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
+          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -635,12 +650,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
+          <t>"Bestlage mit Festungsblick"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>554.99</t>
+          <t>610</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -650,49 +665,54 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>58.42</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Stellplatz"]</t>
+          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
+          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
+          <t>""</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a7j75n"</t>
+          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -702,12 +722,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon"</t>
+          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1181.21</t>
+          <t>532.19</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -717,7 +737,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>70.87</t>
+          <t>56.02</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -732,34 +752,39 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["Personenaufzug"]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3540", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1181.21, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 219, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 169, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1629.21, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/0d9ec1ef-21cc-484a-88ae-193c7267a3bb/1e78105c-6490-4468-a6c3-936b8b388b80", "https://ms.immowelt.org/5c55f670-770f-44e9-b26b-7c9164f4a76a/9f56e225-8915-45d3-9af7-0e36ad2d804e", "https://ms.immowelt.org/12a9fd2a-da00-49a5-9999-efb246a9d727/efc35e4b-a860-47d1-823d-1282d60e0bc6", "https://ms.immowelt.org/bb9a6b97-0d40-46d1-9b24-011a5dcc7508/40526838-218d-4a4c-9422-8bd98023d9f6", "https://ms.immowelt.org/1a701923-58c4-4074-92b3-3e6bc100d51c/2f4849ee-2b95-432d-8ed4-b41b0211a117", "https://ms.immowelt.org/4d6aee50-6e8f-423f-b67a-bd01a011592d/4d58cead-e166-4a77-8c0f-2ee869a9e824"]</t>
+          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon", "basicObjectPricEur": 1181.21, "basicLivingSpace": 70.87, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a7j75n", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
+          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -769,12 +794,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
+          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1183.37</t>
+          <t>566.96</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -784,12 +809,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>81.32</t>
+          <t>59.68</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -799,34 +824,39 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["Stellplatz"]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
+          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
+          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -836,12 +866,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
+          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>950</t>
+          <t>554.99</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -851,49 +881,54 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>58.42</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1911</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
+          <t>["Personenaufzug", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
+          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
+          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -903,12 +938,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
+          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>532.19</t>
+          <t>950</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -918,49 +953,54 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>56.02</t>
+          <t>79</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1911</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>["Personenaufzug"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
+          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
+          <t>""</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
+          <t>"https://www.immowelt.de/expose/2a7j75n"</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -970,12 +1010,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
+          <t>"Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1165</t>
+          <t>1181.21</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -985,7 +1025,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>70.87</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -995,39 +1035,44 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3540", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1181.21, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 219, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 169, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1629.21, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
+          <t>["https://ms.immowelt.org/0d9ec1ef-21cc-484a-88ae-193c7267a3bb/1e78105c-6490-4468-a6c3-936b8b388b80", "https://ms.immowelt.org/5c55f670-770f-44e9-b26b-7c9164f4a76a/9f56e225-8915-45d3-9af7-0e36ad2d804e", "https://ms.immowelt.org/12a9fd2a-da00-49a5-9999-efb246a9d727/efc35e4b-a860-47d1-823d-1282d60e0bc6", "https://ms.immowelt.org/bb9a6b97-0d40-46d1-9b24-011a5dcc7508/40526838-218d-4a4c-9422-8bd98023d9f6", "https://ms.immowelt.org/1a701923-58c4-4074-92b3-3e6bc100d51c/2f4849ee-2b95-432d-8ed4-b41b0211a117", "https://ms.immowelt.org/4d6aee50-6e8f-423f-b67a-bd01a011592d/4d58cead-e166-4a77-8c0f-2ee869a9e824"]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon", "basicObjectPricEur": 1181.21, "basicLivingSpace": 70.87, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a7j75n", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2arkq5m"</t>
+          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1037,12 +1082,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City"</t>
+          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2175</t>
+          <t>1183.37</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1052,49 +1097,54 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>81.32</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>["WANNE", "DUSCHE", "FENSTER", "Personenaufzug", "FERNE", "renoviert", "FERN", "Fu\u00dfbodenheizung", "Zentralheizung", "PARKETT", "FLIESEN", "frei", "abstellraum", "Speisekammer", "Balkon", "Kunststofffenster"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97070", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "\u20ac 6.525,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 2175, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 450, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2625, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/1e8dcfd3-4788-4f09-a3c0-28d3414e57a3/5c7e81c2-8706-4ef4-8899-cfd4e8a5a029"]</t>
+          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Erstbezug nach Kernsanierung! Ca. 150 m\u00b2 Wohnfl\u00e4che auf einer Ebene in der City", "basicObjectPricEur": 2175, "basicLivingSpace": 150, "basicRooms": 5.5, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2arkq5m", "basicContactPhone": "0931/2706700"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
+          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1104,12 +1154,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
+          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>474.53</t>
+          <t>750</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1119,49 +1169,54 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>49.95</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1960</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>["Personenaufzug"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
+          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
+          <t>""</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
+          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1171,12 +1226,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
+          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>1165</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1186,49 +1241,54 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>77</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
+          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
+          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>""</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2awv45u"</t>
+          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1238,12 +1298,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1720</t>
+          <t>420</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1253,49 +1313,54 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>123.36</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
+          <t>["GAS"]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
+          <t>""</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
+          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1305,12 +1370,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
+          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>2880</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1320,49 +1385,54 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>195</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>["WANNE"]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
+          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
+          <t>""</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2upu84s"</t>
+          <t>"https://www.immowelt.de/expose/2asr65p"</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1372,12 +1442,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
+          <t>"Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld "</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>1100</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1387,49 +1457,54 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>103</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1984</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
+          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "renoviert", "GAS", "Etagenheizung", "gartennutzung", "Einbauk\u00fcche", "wg_geeignet", "Balkon"]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "Street": "Unterer Kirchbergweg 37", "LocationId": 496013, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2200,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1400, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
+          <t>["https://ms.immowelt.org/bbd4dcbf-c64e-4c60-9789-afc66db53a3f/7fc04ce4-7f84-4ce5-8111-31fcc917306c", "https://ms.immowelt.org/315ff83e-d234-453a-ad52-c4b99bef7055/a979f182-320d-49d1-8002-bcde353d36ee", "https://ms.immowelt.org/6137c704-6a29-47ae-a5a3-88abd0a2fde0/d535204c-f43a-4229-8152-507fc644a211", "https://ms.immowelt.org/1981c2ad-23cb-41f4-825a-77d67f5fbbe7/e968ecc9-ea46-4188-a2c4-968720f069c0", "https://ms.immowelt.org/a4965ee1-de2b-4d90-8333-b793f90a7406/867d9997-6f27-48da-ade0-9096bf31cf3e", "https://ms.immowelt.org/aed0a388-445d-4f8f-9afd-4a146b35d962/3bc7e507-92a3-446a-a3f1-5799c1df7338", "https://ms.immowelt.org/f9d8ba2e-fb1a-4cdd-98ea-ba6ba4973c25/fde9d74e-bd14-4413-a148-81aad236c43f", "https://ms.immowelt.org/e0fbe89c-ecbb-41e9-9ecd-61c2762b9189/3784b2d8-f66d-4f7f-a893-cb9c7b3e982c", "https://ms.immowelt.org/16af38b3-f1c4-4d16-ba17-2685efc0dbe6/b5361690-0608-4e15-8167-e5ab29ac41e7", "https://ms.immowelt.org/fb842589-0c99-45bb-b567-5d04f811adf5/729e7fb7-c4eb-47db-936a-8a406b3efda8", "https://ms.immowelt.org/2f97e2d2-4fcd-40db-bee9-5d4161812bb0/a57df980-0cf8-4352-8cf0-5e867376c343", "https://ms.immowelt.org/79cf67c5-73a5-4097-8b85-e20df2ab786e/363fc58b-d0d5-4f6e-afda-b1d880cf8747", "https://ms.immowelt.org/d9ae7b88-e98c-4d7f-8096-8ede0076f326/e28b854c-9b59-46d6-84a5-28d2595f9ff2", "https://ms.immowelt.org/dffe6319-03a2-4071-98a5-e0f1e3954460/de63d734-7d33-492b-acbf-be5ca5b61e49", "https://ms.immowelt.org/8af5caf8-2627-4044-83b1-a3824003abcd/a9a95b7e-658f-4e56-989c-5a564997561b", "https://ms.immowelt.org/de373ea2-fa91-495b-aa05-ffa24233b025/ff4e0de7-6c79-411b-bec2-3f5b973c460c", "https://ms.immowelt.org/1db3601f-db1c-4e6f-8b1d-e2f17c88804b/e84274ae-8668-49f0-8327-447ff8511752", "https://ms.immowelt.org/6bc525ad-0769-42c3-aaff-a169a251a660/789b8d1b-633d-4989-a0e8-50949ea51d51"]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"salutation": "Herr", "firstName": "Arnold", "lastName": "Hammer", "mobile": "017683299994", "phone": "0931/60565"}</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld ", "basicObjectPricEur": 1100, "basicLivingSpace": 103, "basicRooms": 4, "basicConstructionYear": 1984, "basicCity": "W\u00fcrzburg", "basicStreet": "Unterer Kirchbergweg 37", "basicUrl": "https://www.immowelt.de/expose/2asr65p", "basicContactPhone": "0931/60565", "basicContactMobile": "017683299994"}</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aebr5t"</t>
+          <t>"https://www.immowelt.de/expose/2awv45u"</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1439,12 +1514,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!"</t>
+          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1290</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1454,12 +1529,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>123.36</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1469,34 +1544,39 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "PELLET", "Fu\u00dfbodenheizung", "Garten", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Eibelstadt", "ZipCode": "97246", "Street": "W\u00fcrzburger Strasse 25", "LocationId": 11869, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2600", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Eibelstadt", "Link": "https://www.immowelt.de/immobilienpreise/eibelstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1290, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1570, "Unit": "EUR"}, {"NumberValue": 40, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7c821767-b600-4ad9-8a2a-50874a2a87cf/92a3b2aa-0393-4e55-ad97-c6c3a803a0d8", "https://ms.immowelt.org/8081e4f6-2ad6-46c7-957d-07597db5c5a8/ee5c7a33-80cd-4c89-bb96-98be1b013e27", "https://ms.immowelt.org/515a3a85-6263-4990-b640-f75ec6075c4b/8456cc16-2fc0-409e-ba1f-f103285c6d18", "https://ms.immowelt.org/340c6f6f-746d-421c-aab8-4850f62a5e6b/e971e1c3-7527-4fb5-a83c-f5221d132bc5", "https://ms.immowelt.org/6205eb16-8906-4267-a472-86439d570e9c/39733ff0-9850-43ab-a6fa-f4f2291ba17d", "https://ms.immowelt.org/3b9c4f71-f8fa-46fa-a1d6-7bab696693cb/eccec98b-d098-4d62-ae2c-f62c71c18721", "https://ms.immowelt.org/ab60445b-088f-4fe5-9554-7448a4a29bb2/0eb8642f-4cb3-4252-b4b5-622b757475d6", "https://ms.immowelt.org/6b12d3cb-5e11-4c67-9c0e-a69e674fc018/3d35f5b5-f31d-4200-8572-5eb83a1079e5", "https://ms.immowelt.org/11466902-020f-43ec-9441-09395d524b18/3136e448-448b-41f8-bcec-58fea52abdd5"]</t>
+          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!", "basicObjectPricEur": 1290, "basicLivingSpace": 93, "basicRooms": 3.5, "basicConstructionYear": 2022, "basicCity": "Eibelstadt", "basicStreet": "W\u00fcrzburger Strasse 25", "basicUrl": "https://www.immowelt.de/expose/2aebr5t"}</t>
+          <t>{"companyName": "Gute Bude Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 3c"}, "salutation": "Frau", "firstName": "Nelly", "lastName": "Gronau"}</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2asr65p"</t>
+          <t>"https://www.immowelt.de/expose/2uewf4g"</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1506,7 +1586,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld "</t>
+          <t>"Boutique Wohnung m\u00f6bliert mieten"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1521,49 +1601,54 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>55</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "renoviert", "GAS", "Etagenheizung", "gartennutzung", "Einbauk\u00fcche", "wg_geeignet", "Balkon"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "Street": "Unterer Kirchbergweg 37", "LocationId": 496013, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2200,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1400, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/bbd4dcbf-c64e-4c60-9789-afc66db53a3f/7fc04ce4-7f84-4ce5-8111-31fcc917306c", "https://ms.immowelt.org/315ff83e-d234-453a-ad52-c4b99bef7055/a979f182-320d-49d1-8002-bcde353d36ee", "https://ms.immowelt.org/6137c704-6a29-47ae-a5a3-88abd0a2fde0/d535204c-f43a-4229-8152-507fc644a211", "https://ms.immowelt.org/1981c2ad-23cb-41f4-825a-77d67f5fbbe7/e968ecc9-ea46-4188-a2c4-968720f069c0", "https://ms.immowelt.org/a4965ee1-de2b-4d90-8333-b793f90a7406/867d9997-6f27-48da-ade0-9096bf31cf3e", "https://ms.immowelt.org/aed0a388-445d-4f8f-9afd-4a146b35d962/3bc7e507-92a3-446a-a3f1-5799c1df7338", "https://ms.immowelt.org/f9d8ba2e-fb1a-4cdd-98ea-ba6ba4973c25/fde9d74e-bd14-4413-a148-81aad236c43f", "https://ms.immowelt.org/e0fbe89c-ecbb-41e9-9ecd-61c2762b9189/3784b2d8-f66d-4f7f-a893-cb9c7b3e982c", "https://ms.immowelt.org/16af38b3-f1c4-4d16-ba17-2685efc0dbe6/b5361690-0608-4e15-8167-e5ab29ac41e7", "https://ms.immowelt.org/fb842589-0c99-45bb-b567-5d04f811adf5/729e7fb7-c4eb-47db-936a-8a406b3efda8", "https://ms.immowelt.org/2f97e2d2-4fcd-40db-bee9-5d4161812bb0/a57df980-0cf8-4352-8cf0-5e867376c343", "https://ms.immowelt.org/79cf67c5-73a5-4097-8b85-e20df2ab786e/363fc58b-d0d5-4f6e-afda-b1d880cf8747", "https://ms.immowelt.org/d9ae7b88-e98c-4d7f-8096-8ede0076f326/e28b854c-9b59-46d6-84a5-28d2595f9ff2", "https://ms.immowelt.org/dffe6319-03a2-4071-98a5-e0f1e3954460/de63d734-7d33-492b-acbf-be5ca5b61e49", "https://ms.immowelt.org/8af5caf8-2627-4044-83b1-a3824003abcd/a9a95b7e-658f-4e56-989c-5a564997561b", "https://ms.immowelt.org/de373ea2-fa91-495b-aa05-ffa24233b025/ff4e0de7-6c79-411b-bec2-3f5b973c460c", "https://ms.immowelt.org/1db3601f-db1c-4e6f-8b1d-e2f17c88804b/e84274ae-8668-49f0-8327-447ff8511752", "https://ms.immowelt.org/6bc525ad-0769-42c3-aaff-a169a251a660/789b8d1b-633d-4989-a0e8-50949ea51d51"]</t>
+          <t>["https://ms.immowelt.org/a13c7ad0-2b70-4b4d-a3ea-a34885d87b08/ec7d0988-cc69-4927-b78a-e0331046ca91", "https://ms.immowelt.org/fde8fa3b-e4a0-4ded-a7b8-8420d1a01a9f/d1572cf7-7d4c-4a02-98e6-2d6e2eaf2b62", "https://ms.immowelt.org/44adf4be-fce6-455d-9181-c27144d0b47e/2f83da82-fc2a-4b88-be4c-03e254e651ef", "https://ms.immowelt.org/ecad88ed-f5a2-43ee-9dac-2470c0ec1f30/b45f2c26-817a-4b2e-8c51-b6b4e1ffdb1d", "https://ms.immowelt.org/38e4f785-7a20-46ce-bc01-3909054d335a/ad336fba-e265-4254-b66b-537222384071", "https://ms.immowelt.org/1e7916ab-6c4d-4283-a5fa-b6ccb79f8f6e/58a84848-235f-402d-a541-f5f6b47652ab", "https://ms.immowelt.org/1160b145-63b1-49fd-9bc5-54104f7bf183/20f3af07-2776-4471-981e-ff09df9d66a7", "https://ms.immowelt.org/1498b260-43eb-4602-8d7d-ad06837fbc82/adf6d355-f74c-45b5-bfa8-b60c2f35c3b9", "https://ms.immowelt.org/3606502e-37fa-4430-9bd8-fe84c0031264/e4a61da6-7999-4ec3-b472-e1f89796a906", "https://ms.immowelt.org/d2aadef4-121e-4c0a-8d0a-767393cc0b74/6210ad93-fbc0-4207-8cf8-9c21f2312742", "https://ms.immowelt.org/477b2242-e6a2-4599-8d7d-52d225d39692/c3547552-3022-4c61-8d1c-52b44db4589a", "https://ms.immowelt.org/b6435004-0e35-4fc6-b7d5-548a1c6bd865/18ecd94d-aeb5-4db7-9ece-c9056b7c18f5", "https://ms.immowelt.org/fffca264-e9b1-4647-8e64-c60be93744f8/191162cc-7517-4fc6-be4a-5a945715134c", "https://ms.immowelt.org/93d1fc99-9be1-4826-a8df-e3a22d03c005/b7d69f86-c033-49d5-941d-d0decd68be56", "https://ms.immowelt.org/3593ecfa-644d-4979-ae0d-0fc4d4e9ae7a/1ec892e1-00ff-49d2-b6db-03c288ea7d6d", "https://ms.immowelt.org/19ab9c79-4170-4a92-b48b-ed773d6437fd/7b0670d3-4d77-4ec4-919e-937dab966ff8", "https://ms.immowelt.org/b4d5be21-2515-403f-8215-e2eb79cc92db/3cf8ef03-8de3-42ff-929d-ff3a020a5b25", "https://ms.immowelt.org/b2b6d755-c0f3-4890-a478-6ac51ea07508/68baa9ce-b806-47ca-8c89-b3ed586305cf", "https://ms.immowelt.org/cc54eb68-d41d-4945-85c5-cc8e8c9b5e81/e3d73054-2d37-4c41-8117-5dad34c03029", "https://ms.immowelt.org/8f0aea64-d4d8-47a0-a269-0ddfd36d2981/93df92fb-6eae-41b6-8679-00bb4a30474f", "https://ms.immowelt.org/824566f0-3a4c-4806-a951-d3eecde604c1/9e360642-24e2-44c2-94e2-d1336be6f715", "https://ms.immowelt.org/edc590e2-19f1-4a3d-8938-add9dfc4b56f/db68466a-1681-4bf8-85cb-489b4ffa5436"]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld ", "basicObjectPricEur": 1100, "basicLivingSpace": 103, "basicRooms": 4, "basicConstructionYear": 1984, "basicCity": "W\u00fcrzburg", "basicStreet": "Unterer Kirchbergweg 37", "basicUrl": "https://www.immowelt.de/expose/2asr65p", "basicContactPhone": "0931/60565", "basicContactMobile": "017683299994"}</t>
+          <t>{"companyName": "Michael Engelbrecht", "address": {"city": "W\u00fcrzburg", "zipCode": "97072", "street": "Sartoriusstra\u00dfe 7"}, "salutation": "Herr/Frau", "firstName": "Michael", "lastName": "Engelbrecht", "mobile": "0171-9546505"}</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Boutique Wohnung m\u00f6bliert mieten", "basicObjectPricEur": 1100, "basicLivingSpace": 55, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2uewf4g", "basicContactMobile": "0171-9546505"}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
+          <t>"https://www.immowelt.de/expose/2almm5r"</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1573,12 +1658,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
+          <t>"TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2880</t>
+          <t>1700</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1588,49 +1673,54 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>153.3</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
+          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "GAS", "Zentralheizung", "teilweise m\u00f6bliert", "TEPPICH", "PARKETT", "FLIESEN", "Einbauk\u00fcche", "offene K\u00fcche", "Stellplatz", "Tiefgarage", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Gartenstra\u00dfe 9", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5.400,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 1700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 240, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten", "Comments": ["in Warmmiete enthalten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2340, "Unit": "EUR"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
+          <t>["https://ms.immowelt.org/338d1cbc-cb3f-423f-8523-42cc120d72f9/e4b563bc-671f-4dea-a726-71d7b9386009", "https://ms.immowelt.org/4da068e4-1a27-465c-b0e7-ffb77b79880b/908c43fa-aa39-4e85-97c8-98295a3c363c", "https://ms.immowelt.org/cab19ffc-0f4a-42a9-89e9-7189e9dafd92/2a5e6769-ad31-4185-a454-e8d753be9cdb", "https://ms.immowelt.org/f6511334-9f04-476c-9659-9f19a5df115f/ff04d8f5-f770-493d-9394-6ac1a456d4ef", "https://ms.immowelt.org/733f5f85-bc20-4e60-ba25-388eeb6563cf/4094751f-b73c-432d-b6b4-6d68ba45d6d9", "https://ms.immowelt.org/05e1b42e-75a4-4206-aaad-48ffa57f162d/a3aafbff-20b6-4c17-a8a1-b916eb14b8aa", "https://ms.immowelt.org/1233e75d-2ab4-4291-8b67-e87c5a4898f1/6153dd66-9325-4066-80d3-ed8642487cd8", "https://ms.immowelt.org/99f6825d-9789-4ae1-9a78-4e6acb5853a7/f727c1c7-69a0-420d-adf8-9119f5849a16", "https://ms.immowelt.org/19d94014-cd12-4f9a-81a5-8f9745f63b90/48988be8-85bb-4980-a25a-276af2606ac6", "https://ms.immowelt.org/f351ce35-7e50-4939-b806-4f6dc375cc86/84c997d9-1332-4173-9248-fb7b75a10943", "https://ms.immowelt.org/cdd250a7-47f6-4535-ac59-6ea51157c95e/bed7b410-ef26-42d6-a562-595eafba5999", "https://ms.immowelt.org/644f0235-e6ba-482b-bb26-2fea622cd4a1/6d2746f3-ea97-4996-8617-e82aeced34e0", "https://ms.immowelt.org/0174f587-e7b3-4c39-8603-c1d8465305ec/508d427a-f8c5-4d05-bd55-06ee858889be", "https://ms.immowelt.org/e3dbe0a9-b856-43a6-97a0-ca238574c6f8/f20530d2-b140-4eb5-b229-ad329853d7f3"]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"companyName": "hv Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Wilhelm-Dahl-Str. 9"}, "profilePicture": "https://filestore.immowelt.de/ProfilBilder/150_98e1685eae1346a2a90a2847489951ff.jpg", "salutation": "Herr", "firstName": "Hartwig", "lastName": "Vogel", "mobile": "0175-5994950", "phone": "0931/45466333"}</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE", "basicObjectPricEur": 1700, "basicLivingSpace": 153.3, "basicRooms": 3, "basicConstructionYear": 1998, "basicCity": "W\u00fcrzburg", "basicStreet": "Gartenstra\u00dfe 9", "basicUrl": "https://www.immowelt.de/expose/2almm5r", "basicContactPhone": "0931/45466333", "basicContactMobile": "0175-5994950"}</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2almm5r"</t>
+          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1640,12 +1730,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE"</t>
+          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1700</t>
+          <t>580</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1655,49 +1745,54 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>153.3</t>
+          <t>44</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "GAS", "Zentralheizung", "teilweise m\u00f6bliert", "TEPPICH", "PARKETT", "FLIESEN", "Einbauk\u00fcche", "offene K\u00fcche", "Stellplatz", "Tiefgarage", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
+          <t>["WANNE"]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Gartenstra\u00dfe 9", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5.400,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 1700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 240, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten", "Comments": ["in Warmmiete enthalten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2340, "Unit": "EUR"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/338d1cbc-cb3f-423f-8523-42cc120d72f9/e4b563bc-671f-4dea-a726-71d7b9386009", "https://ms.immowelt.org/4da068e4-1a27-465c-b0e7-ffb77b79880b/908c43fa-aa39-4e85-97c8-98295a3c363c", "https://ms.immowelt.org/cab19ffc-0f4a-42a9-89e9-7189e9dafd92/2a5e6769-ad31-4185-a454-e8d753be9cdb", "https://ms.immowelt.org/f6511334-9f04-476c-9659-9f19a5df115f/ff04d8f5-f770-493d-9394-6ac1a456d4ef", "https://ms.immowelt.org/733f5f85-bc20-4e60-ba25-388eeb6563cf/4094751f-b73c-432d-b6b4-6d68ba45d6d9", "https://ms.immowelt.org/05e1b42e-75a4-4206-aaad-48ffa57f162d/a3aafbff-20b6-4c17-a8a1-b916eb14b8aa", "https://ms.immowelt.org/1233e75d-2ab4-4291-8b67-e87c5a4898f1/6153dd66-9325-4066-80d3-ed8642487cd8", "https://ms.immowelt.org/99f6825d-9789-4ae1-9a78-4e6acb5853a7/f727c1c7-69a0-420d-adf8-9119f5849a16", "https://ms.immowelt.org/19d94014-cd12-4f9a-81a5-8f9745f63b90/48988be8-85bb-4980-a25a-276af2606ac6", "https://ms.immowelt.org/f351ce35-7e50-4939-b806-4f6dc375cc86/84c997d9-1332-4173-9248-fb7b75a10943", "https://ms.immowelt.org/cdd250a7-47f6-4535-ac59-6ea51157c95e/bed7b410-ef26-42d6-a562-595eafba5999", "https://ms.immowelt.org/644f0235-e6ba-482b-bb26-2fea622cd4a1/6d2746f3-ea97-4996-8617-e82aeced34e0", "https://ms.immowelt.org/0174f587-e7b3-4c39-8603-c1d8465305ec/508d427a-f8c5-4d05-bd55-06ee858889be", "https://ms.immowelt.org/e3dbe0a9-b856-43a6-97a0-ca238574c6f8/f20530d2-b140-4eb5-b229-ad329853d7f3"]</t>
+          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE", "basicObjectPricEur": 1700, "basicLivingSpace": 153.3, "basicRooms": 3, "basicConstructionYear": 1998, "basicCity": "W\u00fcrzburg", "basicStreet": "Gartenstra\u00dfe 9", "basicUrl": "https://www.immowelt.de/expose/2almm5r", "basicContactPhone": "0931/45466333", "basicContactMobile": "0175-5994950"}</t>
+          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
+          <t>"https://www.immowelt.de/expose/2upu84s"</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1707,12 +1802,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>900</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1722,49 +1817,54 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
           <t>""</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>["GAS"]</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2uewf4g"</t>
+          <t>"https://www.immowelt.de/expose/2aebr5t"</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1774,12 +1874,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"Boutique Wohnung m\u00f6bliert mieten"</t>
+          <t>"Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!"</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1290</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1789,42 +1889,47 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>93</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["Neubau", "barriefrei", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "PELLET", "Fu\u00dfbodenheizung", "Garten", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "Eibelstadt", "ZipCode": "97246", "Street": "W\u00fcrzburger Strasse 25", "LocationId": 11869, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2600", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Eibelstadt", "Link": "https://www.immowelt.de/immobilienpreise/eibelstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1290, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1570, "Unit": "EUR"}, {"NumberValue": 40, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/a13c7ad0-2b70-4b4d-a3ea-a34885d87b08/ec7d0988-cc69-4927-b78a-e0331046ca91", "https://ms.immowelt.org/fde8fa3b-e4a0-4ded-a7b8-8420d1a01a9f/d1572cf7-7d4c-4a02-98e6-2d6e2eaf2b62", "https://ms.immowelt.org/44adf4be-fce6-455d-9181-c27144d0b47e/2f83da82-fc2a-4b88-be4c-03e254e651ef", "https://ms.immowelt.org/ecad88ed-f5a2-43ee-9dac-2470c0ec1f30/b45f2c26-817a-4b2e-8c51-b6b4e1ffdb1d", "https://ms.immowelt.org/38e4f785-7a20-46ce-bc01-3909054d335a/ad336fba-e265-4254-b66b-537222384071", "https://ms.immowelt.org/1e7916ab-6c4d-4283-a5fa-b6ccb79f8f6e/58a84848-235f-402d-a541-f5f6b47652ab", "https://ms.immowelt.org/1160b145-63b1-49fd-9bc5-54104f7bf183/20f3af07-2776-4471-981e-ff09df9d66a7", "https://ms.immowelt.org/1498b260-43eb-4602-8d7d-ad06837fbc82/adf6d355-f74c-45b5-bfa8-b60c2f35c3b9", "https://ms.immowelt.org/3606502e-37fa-4430-9bd8-fe84c0031264/e4a61da6-7999-4ec3-b472-e1f89796a906", "https://ms.immowelt.org/d2aadef4-121e-4c0a-8d0a-767393cc0b74/6210ad93-fbc0-4207-8cf8-9c21f2312742", "https://ms.immowelt.org/477b2242-e6a2-4599-8d7d-52d225d39692/c3547552-3022-4c61-8d1c-52b44db4589a", "https://ms.immowelt.org/b6435004-0e35-4fc6-b7d5-548a1c6bd865/18ecd94d-aeb5-4db7-9ece-c9056b7c18f5", "https://ms.immowelt.org/fffca264-e9b1-4647-8e64-c60be93744f8/191162cc-7517-4fc6-be4a-5a945715134c", "https://ms.immowelt.org/93d1fc99-9be1-4826-a8df-e3a22d03c005/b7d69f86-c033-49d5-941d-d0decd68be56", "https://ms.immowelt.org/3593ecfa-644d-4979-ae0d-0fc4d4e9ae7a/1ec892e1-00ff-49d2-b6db-03c288ea7d6d", "https://ms.immowelt.org/19ab9c79-4170-4a92-b48b-ed773d6437fd/7b0670d3-4d77-4ec4-919e-937dab966ff8", "https://ms.immowelt.org/b4d5be21-2515-403f-8215-e2eb79cc92db/3cf8ef03-8de3-42ff-929d-ff3a020a5b25", "https://ms.immowelt.org/b2b6d755-c0f3-4890-a478-6ac51ea07508/68baa9ce-b806-47ca-8c89-b3ed586305cf", "https://ms.immowelt.org/cc54eb68-d41d-4945-85c5-cc8e8c9b5e81/e3d73054-2d37-4c41-8117-5dad34c03029", "https://ms.immowelt.org/8f0aea64-d4d8-47a0-a269-0ddfd36d2981/93df92fb-6eae-41b6-8679-00bb4a30474f", "https://ms.immowelt.org/824566f0-3a4c-4806-a951-d3eecde604c1/9e360642-24e2-44c2-94e2-d1336be6f715", "https://ms.immowelt.org/edc590e2-19f1-4a3d-8938-add9dfc4b56f/db68466a-1681-4bf8-85cb-489b4ffa5436"]</t>
+          <t>["https://ms.immowelt.org/7c821767-b600-4ad9-8a2a-50874a2a87cf/92a3b2aa-0393-4e55-ad97-c6c3a803a0d8", "https://ms.immowelt.org/8081e4f6-2ad6-46c7-957d-07597db5c5a8/ee5c7a33-80cd-4c89-bb96-98be1b013e27", "https://ms.immowelt.org/515a3a85-6263-4990-b640-f75ec6075c4b/8456cc16-2fc0-409e-ba1f-f103285c6d18", "https://ms.immowelt.org/340c6f6f-746d-421c-aab8-4850f62a5e6b/e971e1c3-7527-4fb5-a83c-f5221d132bc5", "https://ms.immowelt.org/6205eb16-8906-4267-a472-86439d570e9c/39733ff0-9850-43ab-a6fa-f4f2291ba17d", "https://ms.immowelt.org/3b9c4f71-f8fa-46fa-a1d6-7bab696693cb/eccec98b-d098-4d62-ae2c-f62c71c18721", "https://ms.immowelt.org/ab60445b-088f-4fe5-9554-7448a4a29bb2/0eb8642f-4cb3-4252-b4b5-622b757475d6", "https://ms.immowelt.org/6b12d3cb-5e11-4c67-9c0e-a69e674fc018/3d35f5b5-f31d-4200-8572-5eb83a1079e5", "https://ms.immowelt.org/11466902-020f-43ec-9441-09395d524b18/3136e448-448b-41f8-bcec-58fea52abdd5"]</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Boutique Wohnung m\u00f6bliert mieten", "basicObjectPricEur": 1100, "basicLivingSpace": 55, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2uewf4g", "basicContactMobile": "0171-9546505"}</t>
+          <t>{"salutation": "Herr", "firstName": "Maximilian", "lastName": "Kauschke"}</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!", "basicObjectPricEur": 1290, "basicLivingSpace": 93, "basicRooms": 3.5, "basicConstructionYear": 2022, "basicCity": "Eibelstadt", "basicStreet": "W\u00fcrzburger Strasse 25", "basicUrl": "https://www.immowelt.de/expose/2aebr5t"}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Bug & MLFlow Runs adjusted
</commit_message>
<xml_diff>
--- a/immowelt_price_guide/data/retrain_train_data.xlsx
+++ b/immowelt_price_guide/data/retrain_train_data.xlsx
@@ -568,7 +568,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
+          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -578,12 +578,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
+          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>474.53</t>
+          <t>566.96</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>49.95</t>
+          <t>59.68</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>["Personenaufzug"]</t>
+          <t>["Stellplatz"]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -618,12 +618,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
+          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -633,14 +633,14 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
+          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -650,12 +650,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"Bestlage mit Festungsblick"</t>
+          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>610</t>
+          <t>950</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -665,37 +665,37 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>79</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1911</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
+          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -705,14 +705,14 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
+          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -722,12 +722,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
+          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>532.19</t>
+          <t>1183.37</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -737,12 +737,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>56.02</t>
+          <t>81.32</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -752,39 +752,39 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>["Personenaufzug"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
+          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
+          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -794,12 +794,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
+          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>566.96</t>
+          <t>474.53</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>59.68</t>
+          <t>49.95</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>["Stellplatz"]</t>
+          <t>["Personenaufzug"]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -834,12 +834,12 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
+          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -849,14 +849,14 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
+          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -866,12 +866,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
+          <t>"Bestlage mit Festungsblick"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>554.99</t>
+          <t>610</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -881,54 +881,54 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>58.42</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Stellplatz"]</t>
+          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
+          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
+          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -938,12 +938,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
+          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>950</t>
+          <t>1165</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -953,37 +953,37 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>77</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1911</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
+          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
+          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -993,14 +993,14 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a7j75n"</t>
+          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1010,12 +1010,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon"</t>
+          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1181.21</t>
+          <t>532.19</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>70.87</t>
+          <t>56.02</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1040,39 +1040,39 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["Personenaufzug"]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3540", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1181.21, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 219, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 169, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1629.21, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/0d9ec1ef-21cc-484a-88ae-193c7267a3bb/1e78105c-6490-4468-a6c3-936b8b388b80", "https://ms.immowelt.org/5c55f670-770f-44e9-b26b-7c9164f4a76a/9f56e225-8915-45d3-9af7-0e36ad2d804e", "https://ms.immowelt.org/12a9fd2a-da00-49a5-9999-efb246a9d727/efc35e4b-a860-47d1-823d-1282d60e0bc6", "https://ms.immowelt.org/bb9a6b97-0d40-46d1-9b24-011a5dcc7508/40526838-218d-4a4c-9422-8bd98023d9f6", "https://ms.immowelt.org/1a701923-58c4-4074-92b3-3e6bc100d51c/2f4849ee-2b95-432d-8ed4-b41b0211a117", "https://ms.immowelt.org/4d6aee50-6e8f-423f-b67a-bd01a011592d/4d58cead-e166-4a77-8c0f-2ee869a9e824"]</t>
+          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon", "basicObjectPricEur": 1181.21, "basicLivingSpace": 70.87, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a7j75n", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
+          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1082,12 +1082,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
+          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1183.37</t>
+          <t>750</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1097,54 +1097,54 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>81.32</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1960</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
+          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
+          <t>"https://www.immowelt.de/expose/2a7j75n"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1154,12 +1154,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
+          <t>"Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>1181.21</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1169,54 +1169,54 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>70.87</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3540", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1181.21, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 219, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 169, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1629.21, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
+          <t>["https://ms.immowelt.org/0d9ec1ef-21cc-484a-88ae-193c7267a3bb/1e78105c-6490-4468-a6c3-936b8b388b80", "https://ms.immowelt.org/5c55f670-770f-44e9-b26b-7c9164f4a76a/9f56e225-8915-45d3-9af7-0e36ad2d804e", "https://ms.immowelt.org/12a9fd2a-da00-49a5-9999-efb246a9d727/efc35e4b-a860-47d1-823d-1282d60e0bc6", "https://ms.immowelt.org/bb9a6b97-0d40-46d1-9b24-011a5dcc7508/40526838-218d-4a4c-9422-8bd98023d9f6", "https://ms.immowelt.org/1a701923-58c4-4074-92b3-3e6bc100d51c/2f4849ee-2b95-432d-8ed4-b41b0211a117", "https://ms.immowelt.org/4d6aee50-6e8f-423f-b67a-bd01a011592d/4d58cead-e166-4a77-8c0f-2ee869a9e824"]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon", "basicObjectPricEur": 1181.21, "basicLivingSpace": 70.87, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a7j75n", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
+          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1226,12 +1226,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1165</t>
+          <t>420</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1241,12 +1241,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1256,22 +1256,22 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["GAS"]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1281,14 +1281,14 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
+          <t>"https://www.immowelt.de/expose/2asr65p"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld "</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>1100</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1313,54 +1313,54 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>103</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1984</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>["GAS"]</t>
+          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "renoviert", "GAS", "Etagenheizung", "gartennutzung", "Einbauk\u00fcche", "wg_geeignet", "Balkon"]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "Street": "Unterer Kirchbergweg 37", "LocationId": 496013, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2200,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1400, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["https://ms.immowelt.org/bbd4dcbf-c64e-4c60-9789-afc66db53a3f/7fc04ce4-7f84-4ce5-8111-31fcc917306c", "https://ms.immowelt.org/315ff83e-d234-453a-ad52-c4b99bef7055/a979f182-320d-49d1-8002-bcde353d36ee", "https://ms.immowelt.org/6137c704-6a29-47ae-a5a3-88abd0a2fde0/d535204c-f43a-4229-8152-507fc644a211", "https://ms.immowelt.org/1981c2ad-23cb-41f4-825a-77d67f5fbbe7/e968ecc9-ea46-4188-a2c4-968720f069c0", "https://ms.immowelt.org/a4965ee1-de2b-4d90-8333-b793f90a7406/867d9997-6f27-48da-ade0-9096bf31cf3e", "https://ms.immowelt.org/aed0a388-445d-4f8f-9afd-4a146b35d962/3bc7e507-92a3-446a-a3f1-5799c1df7338", "https://ms.immowelt.org/f9d8ba2e-fb1a-4cdd-98ea-ba6ba4973c25/fde9d74e-bd14-4413-a148-81aad236c43f", "https://ms.immowelt.org/e0fbe89c-ecbb-41e9-9ecd-61c2762b9189/3784b2d8-f66d-4f7f-a893-cb9c7b3e982c", "https://ms.immowelt.org/16af38b3-f1c4-4d16-ba17-2685efc0dbe6/b5361690-0608-4e15-8167-e5ab29ac41e7", "https://ms.immowelt.org/fb842589-0c99-45bb-b567-5d04f811adf5/729e7fb7-c4eb-47db-936a-8a406b3efda8", "https://ms.immowelt.org/2f97e2d2-4fcd-40db-bee9-5d4161812bb0/a57df980-0cf8-4352-8cf0-5e867376c343", "https://ms.immowelt.org/79cf67c5-73a5-4097-8b85-e20df2ab786e/363fc58b-d0d5-4f6e-afda-b1d880cf8747", "https://ms.immowelt.org/d9ae7b88-e98c-4d7f-8096-8ede0076f326/e28b854c-9b59-46d6-84a5-28d2595f9ff2", "https://ms.immowelt.org/dffe6319-03a2-4071-98a5-e0f1e3954460/de63d734-7d33-492b-acbf-be5ca5b61e49", "https://ms.immowelt.org/8af5caf8-2627-4044-83b1-a3824003abcd/a9a95b7e-658f-4e56-989c-5a564997561b", "https://ms.immowelt.org/de373ea2-fa91-495b-aa05-ffa24233b025/ff4e0de7-6c79-411b-bec2-3f5b973c460c", "https://ms.immowelt.org/1db3601f-db1c-4e6f-8b1d-e2f17c88804b/e84274ae-8668-49f0-8327-447ff8511752", "https://ms.immowelt.org/6bc525ad-0769-42c3-aaff-a169a251a660/789b8d1b-633d-4989-a0e8-50949ea51d51"]</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"salutation": "Herr", "firstName": "Arnold", "lastName": "Hammer", "mobile": "017683299994", "phone": "0931/60565"}</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld ", "basicObjectPricEur": 1100, "basicLivingSpace": 103, "basicRooms": 4, "basicConstructionYear": 1984, "basicCity": "W\u00fcrzburg", "basicStreet": "Unterer Kirchbergweg 37", "basicUrl": "https://www.immowelt.de/expose/2asr65p", "basicContactPhone": "0931/60565", "basicContactMobile": "017683299994"}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
+          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
+          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2880</t>
+          <t>554.99</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1385,54 +1385,54 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>58.42</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
+          <t>["Personenaufzug", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
+          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2asr65p"</t>
+          <t>"https://www.immowelt.de/expose/2awv45u"</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1442,12 +1442,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld "</t>
+          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1457,54 +1457,54 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>123.36</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "renoviert", "GAS", "Etagenheizung", "gartennutzung", "Einbauk\u00fcche", "wg_geeignet", "Balkon"]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "Street": "Unterer Kirchbergweg 37", "LocationId": 496013, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2200,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1400, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/bbd4dcbf-c64e-4c60-9789-afc66db53a3f/7fc04ce4-7f84-4ce5-8111-31fcc917306c", "https://ms.immowelt.org/315ff83e-d234-453a-ad52-c4b99bef7055/a979f182-320d-49d1-8002-bcde353d36ee", "https://ms.immowelt.org/6137c704-6a29-47ae-a5a3-88abd0a2fde0/d535204c-f43a-4229-8152-507fc644a211", "https://ms.immowelt.org/1981c2ad-23cb-41f4-825a-77d67f5fbbe7/e968ecc9-ea46-4188-a2c4-968720f069c0", "https://ms.immowelt.org/a4965ee1-de2b-4d90-8333-b793f90a7406/867d9997-6f27-48da-ade0-9096bf31cf3e", "https://ms.immowelt.org/aed0a388-445d-4f8f-9afd-4a146b35d962/3bc7e507-92a3-446a-a3f1-5799c1df7338", "https://ms.immowelt.org/f9d8ba2e-fb1a-4cdd-98ea-ba6ba4973c25/fde9d74e-bd14-4413-a148-81aad236c43f", "https://ms.immowelt.org/e0fbe89c-ecbb-41e9-9ecd-61c2762b9189/3784b2d8-f66d-4f7f-a893-cb9c7b3e982c", "https://ms.immowelt.org/16af38b3-f1c4-4d16-ba17-2685efc0dbe6/b5361690-0608-4e15-8167-e5ab29ac41e7", "https://ms.immowelt.org/fb842589-0c99-45bb-b567-5d04f811adf5/729e7fb7-c4eb-47db-936a-8a406b3efda8", "https://ms.immowelt.org/2f97e2d2-4fcd-40db-bee9-5d4161812bb0/a57df980-0cf8-4352-8cf0-5e867376c343", "https://ms.immowelt.org/79cf67c5-73a5-4097-8b85-e20df2ab786e/363fc58b-d0d5-4f6e-afda-b1d880cf8747", "https://ms.immowelt.org/d9ae7b88-e98c-4d7f-8096-8ede0076f326/e28b854c-9b59-46d6-84a5-28d2595f9ff2", "https://ms.immowelt.org/dffe6319-03a2-4071-98a5-e0f1e3954460/de63d734-7d33-492b-acbf-be5ca5b61e49", "https://ms.immowelt.org/8af5caf8-2627-4044-83b1-a3824003abcd/a9a95b7e-658f-4e56-989c-5a564997561b", "https://ms.immowelt.org/de373ea2-fa91-495b-aa05-ffa24233b025/ff4e0de7-6c79-411b-bec2-3f5b973c460c", "https://ms.immowelt.org/1db3601f-db1c-4e6f-8b1d-e2f17c88804b/e84274ae-8668-49f0-8327-447ff8511752", "https://ms.immowelt.org/6bc525ad-0769-42c3-aaff-a169a251a660/789b8d1b-633d-4989-a0e8-50949ea51d51"]</t>
+          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>{"salutation": "Herr", "firstName": "Arnold", "lastName": "Hammer", "mobile": "017683299994", "phone": "0931/60565"}</t>
+          <t>{"companyName": "Gute Bude Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 3c"}, "salutation": "Frau", "firstName": "Nelly", "lastName": "Gronau"}</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Familienfreundliche 4 - Zimmer Wohnung in W\u00fcrzburg - Heidingsfeld ", "basicObjectPricEur": 1100, "basicLivingSpace": 103, "basicRooms": 4, "basicConstructionYear": 1984, "basicCity": "W\u00fcrzburg", "basicStreet": "Unterer Kirchbergweg 37", "basicUrl": "https://www.immowelt.de/expose/2asr65p", "basicContactPhone": "0931/60565", "basicContactMobile": "017683299994"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2awv45u"</t>
+          <t>"https://www.immowelt.de/expose/2upu84s"</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1514,12 +1514,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
+          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1720</t>
+          <t>900</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>123.36</t>
+          <t>90</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1539,44 +1539,44 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
+          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
+          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>{"companyName": "Gute Bude Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 3c"}, "salutation": "Frau", "firstName": "Nelly", "lastName": "Gronau"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2uewf4g"</t>
+          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"Boutique Wohnung m\u00f6bliert mieten"</t>
+          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>2880</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1601,54 +1601,54 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>195</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
           <t>""</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>null</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>["https://ms.immowelt.org/a13c7ad0-2b70-4b4d-a3ea-a34885d87b08/ec7d0988-cc69-4927-b78a-e0331046ca91", "https://ms.immowelt.org/fde8fa3b-e4a0-4ded-a7b8-8420d1a01a9f/d1572cf7-7d4c-4a02-98e6-2d6e2eaf2b62", "https://ms.immowelt.org/44adf4be-fce6-455d-9181-c27144d0b47e/2f83da82-fc2a-4b88-be4c-03e254e651ef", "https://ms.immowelt.org/ecad88ed-f5a2-43ee-9dac-2470c0ec1f30/b45f2c26-817a-4b2e-8c51-b6b4e1ffdb1d", "https://ms.immowelt.org/38e4f785-7a20-46ce-bc01-3909054d335a/ad336fba-e265-4254-b66b-537222384071", "https://ms.immowelt.org/1e7916ab-6c4d-4283-a5fa-b6ccb79f8f6e/58a84848-235f-402d-a541-f5f6b47652ab", "https://ms.immowelt.org/1160b145-63b1-49fd-9bc5-54104f7bf183/20f3af07-2776-4471-981e-ff09df9d66a7", "https://ms.immowelt.org/1498b260-43eb-4602-8d7d-ad06837fbc82/adf6d355-f74c-45b5-bfa8-b60c2f35c3b9", "https://ms.immowelt.org/3606502e-37fa-4430-9bd8-fe84c0031264/e4a61da6-7999-4ec3-b472-e1f89796a906", "https://ms.immowelt.org/d2aadef4-121e-4c0a-8d0a-767393cc0b74/6210ad93-fbc0-4207-8cf8-9c21f2312742", "https://ms.immowelt.org/477b2242-e6a2-4599-8d7d-52d225d39692/c3547552-3022-4c61-8d1c-52b44db4589a", "https://ms.immowelt.org/b6435004-0e35-4fc6-b7d5-548a1c6bd865/18ecd94d-aeb5-4db7-9ece-c9056b7c18f5", "https://ms.immowelt.org/fffca264-e9b1-4647-8e64-c60be93744f8/191162cc-7517-4fc6-be4a-5a945715134c", "https://ms.immowelt.org/93d1fc99-9be1-4826-a8df-e3a22d03c005/b7d69f86-c033-49d5-941d-d0decd68be56", "https://ms.immowelt.org/3593ecfa-644d-4979-ae0d-0fc4d4e9ae7a/1ec892e1-00ff-49d2-b6db-03c288ea7d6d", "https://ms.immowelt.org/19ab9c79-4170-4a92-b48b-ed773d6437fd/7b0670d3-4d77-4ec4-919e-937dab966ff8", "https://ms.immowelt.org/b4d5be21-2515-403f-8215-e2eb79cc92db/3cf8ef03-8de3-42ff-929d-ff3a020a5b25", "https://ms.immowelt.org/b2b6d755-c0f3-4890-a478-6ac51ea07508/68baa9ce-b806-47ca-8c89-b3ed586305cf", "https://ms.immowelt.org/cc54eb68-d41d-4945-85c5-cc8e8c9b5e81/e3d73054-2d37-4c41-8117-5dad34c03029", "https://ms.immowelt.org/8f0aea64-d4d8-47a0-a269-0ddfd36d2981/93df92fb-6eae-41b6-8679-00bb4a30474f", "https://ms.immowelt.org/824566f0-3a4c-4806-a951-d3eecde604c1/9e360642-24e2-44c2-94e2-d1336be6f715", "https://ms.immowelt.org/edc590e2-19f1-4a3d-8938-add9dfc4b56f/db68466a-1681-4bf8-85cb-489b4ffa5436"]</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>{"companyName": "Michael Engelbrecht", "address": {"city": "W\u00fcrzburg", "zipCode": "97072", "street": "Sartoriusstra\u00dfe 7"}, "salutation": "Herr/Frau", "firstName": "Michael", "lastName": "Engelbrecht", "mobile": "0171-9546505"}</t>
-        </is>
-      </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Boutique Wohnung m\u00f6bliert mieten", "basicObjectPricEur": 1100, "basicLivingSpace": 55, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2uewf4g", "basicContactMobile": "0171-9546505"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2almm5r"</t>
+          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1658,12 +1658,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE"</t>
+          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1700</t>
+          <t>580</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1673,54 +1673,54 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>153.3</t>
+          <t>44</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "GAS", "Zentralheizung", "teilweise m\u00f6bliert", "TEPPICH", "PARKETT", "FLIESEN", "Einbauk\u00fcche", "offene K\u00fcche", "Stellplatz", "Tiefgarage", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
+          <t>["WANNE"]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Gartenstra\u00dfe 9", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5.400,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 1700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 240, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten", "Comments": ["in Warmmiete enthalten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2340, "Unit": "EUR"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/338d1cbc-cb3f-423f-8523-42cc120d72f9/e4b563bc-671f-4dea-a726-71d7b9386009", "https://ms.immowelt.org/4da068e4-1a27-465c-b0e7-ffb77b79880b/908c43fa-aa39-4e85-97c8-98295a3c363c", "https://ms.immowelt.org/cab19ffc-0f4a-42a9-89e9-7189e9dafd92/2a5e6769-ad31-4185-a454-e8d753be9cdb", "https://ms.immowelt.org/f6511334-9f04-476c-9659-9f19a5df115f/ff04d8f5-f770-493d-9394-6ac1a456d4ef", "https://ms.immowelt.org/733f5f85-bc20-4e60-ba25-388eeb6563cf/4094751f-b73c-432d-b6b4-6d68ba45d6d9", "https://ms.immowelt.org/05e1b42e-75a4-4206-aaad-48ffa57f162d/a3aafbff-20b6-4c17-a8a1-b916eb14b8aa", "https://ms.immowelt.org/1233e75d-2ab4-4291-8b67-e87c5a4898f1/6153dd66-9325-4066-80d3-ed8642487cd8", "https://ms.immowelt.org/99f6825d-9789-4ae1-9a78-4e6acb5853a7/f727c1c7-69a0-420d-adf8-9119f5849a16", "https://ms.immowelt.org/19d94014-cd12-4f9a-81a5-8f9745f63b90/48988be8-85bb-4980-a25a-276af2606ac6", "https://ms.immowelt.org/f351ce35-7e50-4939-b806-4f6dc375cc86/84c997d9-1332-4173-9248-fb7b75a10943", "https://ms.immowelt.org/cdd250a7-47f6-4535-ac59-6ea51157c95e/bed7b410-ef26-42d6-a562-595eafba5999", "https://ms.immowelt.org/644f0235-e6ba-482b-bb26-2fea622cd4a1/6d2746f3-ea97-4996-8617-e82aeced34e0", "https://ms.immowelt.org/0174f587-e7b3-4c39-8603-c1d8465305ec/508d427a-f8c5-4d05-bd55-06ee858889be", "https://ms.immowelt.org/e3dbe0a9-b856-43a6-97a0-ca238574c6f8/f20530d2-b140-4eb5-b229-ad329853d7f3"]</t>
+          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>{"companyName": "hv Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Wilhelm-Dahl-Str. 9"}, "profilePicture": "https://filestore.immowelt.de/ProfilBilder/150_98e1685eae1346a2a90a2847489951ff.jpg", "salutation": "Herr", "firstName": "Hartwig", "lastName": "Vogel", "mobile": "0175-5994950", "phone": "0931/45466333"}</t>
+          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE", "basicObjectPricEur": 1700, "basicLivingSpace": 153.3, "basicRooms": 3, "basicConstructionYear": 1998, "basicCity": "W\u00fcrzburg", "basicStreet": "Gartenstra\u00dfe 9", "basicUrl": "https://www.immowelt.de/expose/2almm5r", "basicContactPhone": "0931/45466333", "basicContactMobile": "0175-5994950"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
+          <t>"https://www.immowelt.de/expose/2uewf4g"</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1730,12 +1730,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
+          <t>"Boutique Wohnung m\u00f6bliert mieten"</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>1100</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1745,12 +1745,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>55</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>["WANNE"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1770,29 +1770,29 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1100, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
+          <t>["https://ms.immowelt.org/a13c7ad0-2b70-4b4d-a3ea-a34885d87b08/ec7d0988-cc69-4927-b78a-e0331046ca91", "https://ms.immowelt.org/fde8fa3b-e4a0-4ded-a7b8-8420d1a01a9f/d1572cf7-7d4c-4a02-98e6-2d6e2eaf2b62", "https://ms.immowelt.org/44adf4be-fce6-455d-9181-c27144d0b47e/2f83da82-fc2a-4b88-be4c-03e254e651ef", "https://ms.immowelt.org/ecad88ed-f5a2-43ee-9dac-2470c0ec1f30/b45f2c26-817a-4b2e-8c51-b6b4e1ffdb1d", "https://ms.immowelt.org/38e4f785-7a20-46ce-bc01-3909054d335a/ad336fba-e265-4254-b66b-537222384071", "https://ms.immowelt.org/1e7916ab-6c4d-4283-a5fa-b6ccb79f8f6e/58a84848-235f-402d-a541-f5f6b47652ab", "https://ms.immowelt.org/1160b145-63b1-49fd-9bc5-54104f7bf183/20f3af07-2776-4471-981e-ff09df9d66a7", "https://ms.immowelt.org/1498b260-43eb-4602-8d7d-ad06837fbc82/adf6d355-f74c-45b5-bfa8-b60c2f35c3b9", "https://ms.immowelt.org/3606502e-37fa-4430-9bd8-fe84c0031264/e4a61da6-7999-4ec3-b472-e1f89796a906", "https://ms.immowelt.org/d2aadef4-121e-4c0a-8d0a-767393cc0b74/6210ad93-fbc0-4207-8cf8-9c21f2312742", "https://ms.immowelt.org/477b2242-e6a2-4599-8d7d-52d225d39692/c3547552-3022-4c61-8d1c-52b44db4589a", "https://ms.immowelt.org/b6435004-0e35-4fc6-b7d5-548a1c6bd865/18ecd94d-aeb5-4db7-9ece-c9056b7c18f5", "https://ms.immowelt.org/fffca264-e9b1-4647-8e64-c60be93744f8/191162cc-7517-4fc6-be4a-5a945715134c", "https://ms.immowelt.org/93d1fc99-9be1-4826-a8df-e3a22d03c005/b7d69f86-c033-49d5-941d-d0decd68be56", "https://ms.immowelt.org/3593ecfa-644d-4979-ae0d-0fc4d4e9ae7a/1ec892e1-00ff-49d2-b6db-03c288ea7d6d", "https://ms.immowelt.org/19ab9c79-4170-4a92-b48b-ed773d6437fd/7b0670d3-4d77-4ec4-919e-937dab966ff8", "https://ms.immowelt.org/b4d5be21-2515-403f-8215-e2eb79cc92db/3cf8ef03-8de3-42ff-929d-ff3a020a5b25", "https://ms.immowelt.org/b2b6d755-c0f3-4890-a478-6ac51ea07508/68baa9ce-b806-47ca-8c89-b3ed586305cf", "https://ms.immowelt.org/cc54eb68-d41d-4945-85c5-cc8e8c9b5e81/e3d73054-2d37-4c41-8117-5dad34c03029", "https://ms.immowelt.org/8f0aea64-d4d8-47a0-a269-0ddfd36d2981/93df92fb-6eae-41b6-8679-00bb4a30474f", "https://ms.immowelt.org/824566f0-3a4c-4806-a951-d3eecde604c1/9e360642-24e2-44c2-94e2-d1336be6f715", "https://ms.immowelt.org/edc590e2-19f1-4a3d-8938-add9dfc4b56f/db68466a-1681-4bf8-85cb-489b4ffa5436"]</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
+          <t>{"companyName": "Michael Engelbrecht", "address": {"city": "W\u00fcrzburg", "zipCode": "97072", "street": "Sartoriusstra\u00dfe 7"}, "salutation": "Herr/Frau", "firstName": "Michael", "lastName": "Engelbrecht", "mobile": "0171-9546505"}</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Boutique Wohnung m\u00f6bliert mieten", "basicObjectPricEur": 1100, "basicLivingSpace": 55, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2uewf4g", "basicContactMobile": "0171-9546505"}</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2upu84s"</t>
+          <t>"https://www.immowelt.de/expose/2aebr5t"</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1802,12 +1802,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
+          <t>"Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!"</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>1290</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1817,54 +1817,54 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>93</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
+          <t>["Neubau", "barriefrei", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "PELLET", "Fu\u00dfbodenheizung", "Garten", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "Eibelstadt", "ZipCode": "97246", "Street": "W\u00fcrzburger Strasse 25", "LocationId": 11869, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2600", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Eibelstadt", "Link": "https://www.immowelt.de/immobilienpreise/eibelstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1290, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1570, "Unit": "EUR"}, {"NumberValue": 40, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
+          <t>["https://ms.immowelt.org/7c821767-b600-4ad9-8a2a-50874a2a87cf/92a3b2aa-0393-4e55-ad97-c6c3a803a0d8", "https://ms.immowelt.org/8081e4f6-2ad6-46c7-957d-07597db5c5a8/ee5c7a33-80cd-4c89-bb96-98be1b013e27", "https://ms.immowelt.org/515a3a85-6263-4990-b640-f75ec6075c4b/8456cc16-2fc0-409e-ba1f-f103285c6d18", "https://ms.immowelt.org/340c6f6f-746d-421c-aab8-4850f62a5e6b/e971e1c3-7527-4fb5-a83c-f5221d132bc5", "https://ms.immowelt.org/6205eb16-8906-4267-a472-86439d570e9c/39733ff0-9850-43ab-a6fa-f4f2291ba17d", "https://ms.immowelt.org/3b9c4f71-f8fa-46fa-a1d6-7bab696693cb/eccec98b-d098-4d62-ae2c-f62c71c18721", "https://ms.immowelt.org/ab60445b-088f-4fe5-9554-7448a4a29bb2/0eb8642f-4cb3-4252-b4b5-622b757475d6", "https://ms.immowelt.org/6b12d3cb-5e11-4c67-9c0e-a69e674fc018/3d35f5b5-f31d-4200-8572-5eb83a1079e5", "https://ms.immowelt.org/11466902-020f-43ec-9441-09395d524b18/3136e448-448b-41f8-bcec-58fea52abdd5"]</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"salutation": "Herr", "firstName": "Maximilian", "lastName": "Kauschke"}</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!", "basicObjectPricEur": 1290, "basicLivingSpace": 93, "basicRooms": 3.5, "basicConstructionYear": 2022, "basicCity": "Eibelstadt", "basicStreet": "W\u00fcrzburger Strasse 25", "basicUrl": "https://www.immowelt.de/expose/2aebr5t"}</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aebr5t"</t>
+          <t>"https://www.immowelt.de/expose/2almm5r"</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1874,12 +1874,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!"</t>
+          <t>"TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE"</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1290</t>
+          <t>1700</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1889,47 +1889,47 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>153.3</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "PELLET", "Fu\u00dfbodenheizung", "Garten", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "Dachgeschoss", "FERNE", "GEPFLEGT", "GAS", "Zentralheizung", "teilweise m\u00f6bliert", "TEPPICH", "PARKETT", "FLIESEN", "Einbauk\u00fcche", "offene K\u00fcche", "Stellplatz", "Tiefgarage", "REINIGUNG", "Terrasse", "Kunststofffenster"]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Eibelstadt", "ZipCode": "97246", "Street": "W\u00fcrzburger Strasse 25", "LocationId": 11869, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Gartenstra\u00dfe 9", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2600", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Eibelstadt", "Link": "https://www.immowelt.de/immobilienpreise/eibelstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 1290, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1570, "Unit": "EUR"}, {"NumberValue": 40, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5.400,00", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 1700, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 240, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 300, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten", "Comments": ["in Warmmiete enthalten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2340, "Unit": "EUR"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7c821767-b600-4ad9-8a2a-50874a2a87cf/92a3b2aa-0393-4e55-ad97-c6c3a803a0d8", "https://ms.immowelt.org/8081e4f6-2ad6-46c7-957d-07597db5c5a8/ee5c7a33-80cd-4c89-bb96-98be1b013e27", "https://ms.immowelt.org/515a3a85-6263-4990-b640-f75ec6075c4b/8456cc16-2fc0-409e-ba1f-f103285c6d18", "https://ms.immowelt.org/340c6f6f-746d-421c-aab8-4850f62a5e6b/e971e1c3-7527-4fb5-a83c-f5221d132bc5", "https://ms.immowelt.org/6205eb16-8906-4267-a472-86439d570e9c/39733ff0-9850-43ab-a6fa-f4f2291ba17d", "https://ms.immowelt.org/3b9c4f71-f8fa-46fa-a1d6-7bab696693cb/eccec98b-d098-4d62-ae2c-f62c71c18721", "https://ms.immowelt.org/ab60445b-088f-4fe5-9554-7448a4a29bb2/0eb8642f-4cb3-4252-b4b5-622b757475d6", "https://ms.immowelt.org/6b12d3cb-5e11-4c67-9c0e-a69e674fc018/3d35f5b5-f31d-4200-8572-5eb83a1079e5", "https://ms.immowelt.org/11466902-020f-43ec-9441-09395d524b18/3136e448-448b-41f8-bcec-58fea52abdd5"]</t>
+          <t>["https://ms.immowelt.org/338d1cbc-cb3f-423f-8523-42cc120d72f9/e4b563bc-671f-4dea-a726-71d7b9386009", "https://ms.immowelt.org/4da068e4-1a27-465c-b0e7-ffb77b79880b/908c43fa-aa39-4e85-97c8-98295a3c363c", "https://ms.immowelt.org/cab19ffc-0f4a-42a9-89e9-7189e9dafd92/2a5e6769-ad31-4185-a454-e8d753be9cdb", "https://ms.immowelt.org/f6511334-9f04-476c-9659-9f19a5df115f/ff04d8f5-f770-493d-9394-6ac1a456d4ef", "https://ms.immowelt.org/733f5f85-bc20-4e60-ba25-388eeb6563cf/4094751f-b73c-432d-b6b4-6d68ba45d6d9", "https://ms.immowelt.org/05e1b42e-75a4-4206-aaad-48ffa57f162d/a3aafbff-20b6-4c17-a8a1-b916eb14b8aa", "https://ms.immowelt.org/1233e75d-2ab4-4291-8b67-e87c5a4898f1/6153dd66-9325-4066-80d3-ed8642487cd8", "https://ms.immowelt.org/99f6825d-9789-4ae1-9a78-4e6acb5853a7/f727c1c7-69a0-420d-adf8-9119f5849a16", "https://ms.immowelt.org/19d94014-cd12-4f9a-81a5-8f9745f63b90/48988be8-85bb-4980-a25a-276af2606ac6", "https://ms.immowelt.org/f351ce35-7e50-4939-b806-4f6dc375cc86/84c997d9-1332-4173-9248-fb7b75a10943", "https://ms.immowelt.org/cdd250a7-47f6-4535-ac59-6ea51157c95e/bed7b410-ef26-42d6-a562-595eafba5999", "https://ms.immowelt.org/644f0235-e6ba-482b-bb26-2fea622cd4a1/6d2746f3-ea97-4996-8617-e82aeced34e0", "https://ms.immowelt.org/0174f587-e7b3-4c39-8603-c1d8465305ec/508d427a-f8c5-4d05-bd55-06ee858889be", "https://ms.immowelt.org/e3dbe0a9-b856-43a6-97a0-ca238574c6f8/f20530d2-b140-4eb5-b229-ad329853d7f3"]</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>{"salutation": "Herr", "firstName": "Maximilian", "lastName": "Kauschke"}</t>
+          <t>{"companyName": "hv Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Wilhelm-Dahl-Str. 9"}, "profilePicture": "https://filestore.immowelt.de/ProfilBilder/150_98e1685eae1346a2a90a2847489951ff.jpg", "salutation": "Herr", "firstName": "Hartwig", "lastName": "Vogel", "mobile": "0175-5994950", "phone": "0931/45466333"}</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Tolle, neuwertige 3,5Zi Erdgeschosswohnung mit Terrasse zwischen Main und Wein in Eibelstadt!", "basicObjectPricEur": 1290, "basicLivingSpace": 93, "basicRooms": 3.5, "basicConstructionYear": 2022, "basicCity": "Eibelstadt", "basicStreet": "W\u00fcrzburger Strasse 25", "basicUrl": "https://www.immowelt.de/expose/2aebr5t"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "TOP-LAGE SANDERAU MIT GROSSER DACHTERRASSE", "basicObjectPricEur": 1700, "basicLivingSpace": 153.3, "basicRooms": 3, "basicConstructionYear": 1998, "basicCity": "W\u00fcrzburg", "basicStreet": "Gartenstra\u00dfe 9", "basicUrl": "https://www.immowelt.de/expose/2almm5r", "basicContactPhone": "0931/45466333", "basicContactMobile": "0175-5994950"}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean up and commenting
</commit_message>
<xml_diff>
--- a/immowelt_price_guide/data/retrain_train_data.xlsx
+++ b/immowelt_price_guide/data/retrain_train_data.xlsx
@@ -568,7 +568,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
+          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -578,12 +578,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
+          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>566.96</t>
+          <t>1165</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>59.68</t>
+          <t>77</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -603,44 +603,44 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>["Stellplatz"]</t>
+          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
+          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
+          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -650,12 +650,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
+          <t>"Bestlage mit Festungsblick"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>950</t>
+          <t>610</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -665,37 +665,37 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1911</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
+          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
+          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -705,14 +705,14 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
+          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -722,12 +722,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
+          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1183.37</t>
+          <t>554.99</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -737,12 +737,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>81.32</t>
+          <t>58.42</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -752,39 +752,39 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["Personenaufzug", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
+          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
+          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -794,12 +794,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
+          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>474.53</t>
+          <t>532.19</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>49.95</t>
+          <t>56.02</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -829,17 +829,17 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
+          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -849,14 +849,14 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2tfuz4l"</t>
+          <t>"https://www.immowelt.de/expose/2a97e5s"</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -866,12 +866,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"Bestlage mit Festungsblick"</t>
+          <t>"Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>610</t>
+          <t>1183.37</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -881,54 +881,54 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>81.32</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>["DUSCHE", "FENSTER", "Dachgeschoss", "frei", "offene K\u00fcche", "Stellplatz"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Breslauer Stra\u00dfe", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "Abl\u00f6se der K\u00fcche", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 610, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3550", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1183.37, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 252, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 171, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1666.37, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/b4607fa6-96c6-40a3-8049-ed2221dafd3c/bb9b114c-9b74-4749-b16f-f5402ce89d13", "https://ms.immowelt.org/0678cd9c-641a-4bcc-a0ac-02f46fc8e1ea/b0aa6847-a6e4-474c-b300-23bb59c7628b", "https://ms.immowelt.org/d524e2d3-1330-4559-987d-6495b2a4c71d/3adebae2-58ee-44b1-a898-86e63f8eff12", "https://ms.immowelt.org/61eb287f-36c7-4a51-a4db-f88e4049ad30/29721137-7a70-4a6d-9abc-340c019663bf"]</t>
+          <t>["https://ms.immowelt.org/4e4fecdb-3fe4-4b73-be6f-d02dcff6e907/a23bae17-4a7c-4155-88b0-8014e5e3021a", "https://ms.immowelt.org/324f63aa-2fff-4fc8-8ba1-ac69ea7a7e23/ed4f84b2-861b-4e99-b1c6-4e3963ae1f35", "https://ms.immowelt.org/be4e9cc8-6ad5-4ae2-a739-1b8b7178ee12/ba6c9877-b521-46d0-a222-9e1e70f8ffd4"]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Bestlage mit Festungsblick", "basicObjectPricEur": 610, "basicLivingSpace": 65, "basicRooms": 1, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicStreet": "Breslauer Stra\u00dfe", "basicUrl": "https://www.immowelt.de/expose/2tfuz4l", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gut gemacht !! 3 Zi, 81 qm, Balkon und Einbauk\u00fcche", "basicObjectPricEur": 1183.37, "basicLivingSpace": 81.32, "basicRooms": 3, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a97e5s", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aqpt5d"</t>
+          <t>"https://www.immowelt.de/expose/25dtq5g"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -938,12 +938,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal "</t>
+          <t>"3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu."</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1165</t>
+          <t>950</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -953,37 +953,37 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>79</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>1911</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>["renoviert", "GAS", "Zentralheizung", "gartennutzung", "Einbauk\u00fcche", "Terrasse"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "FENSTER", "Kelleranteil", "GAS", "Etagenheizung", "Einbauk\u00fcche", "Balkon"]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Steinbachtal", "ZipCode": "97082", "LocationId": 496023, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Sanderau", "ZipCode": "97072", "Street": "Eichendorffstrasse 4", "LocationId": 496022, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3495", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Steinbachtal)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-steinbachtal/mietspiegel"}}, "DataTable": [{"NumberValue": 1165, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 280, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1445, "Unit": "EUR"}, {"NumberValue": 75, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1900", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Sanderau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg/mietspiegel"}}, "DataTable": [{"NumberValue": 950, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}]}</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/d789ca7c-5451-48cf-a649-7af7d4c9078a/0af4290a-753d-4df9-bd0e-3989d2db4215", "https://ms.immowelt.org/2908c42c-0f96-410b-b619-dba38e6a42a1/75b141df-d3a1-4754-b265-67306b3a36e1", "https://ms.immowelt.org/fbb8e8e1-0cc5-4a95-8902-c6f6af96acc8/548e065f-569a-4838-9887-a19794c56f49", "https://ms.immowelt.org/4365c939-93fc-4ec1-b3e8-77d586d0e200/5112a29b-5171-4dc0-b36a-b9b4c4ac411f", "https://ms.immowelt.org/db7ac2e7-2969-42be-920b-36be7e6aab0d/0cf7253b-4260-4efa-af51-0074b8782be6", "https://ms.immowelt.org/d1a4bcbb-b277-4731-8486-0a09fb1b8996/475444d0-b794-44bc-ba59-ce3f2f51b9f8", "https://ms.immowelt.org/748a1662-4a4a-4f6d-bb72-baf731de8adc/700fbb9a-6ef9-48a1-8e73-4c46cba5c258", "https://ms.immowelt.org/ed9af812-426e-4e49-8e89-2ede0c407269/5a107fdf-e72a-4f22-9de2-52351751a755", "https://ms.immowelt.org/643489b1-7bf2-46a3-882c-7d8b8b0957ca/bce02d3c-331a-4110-8e99-d872140474b1", "https://ms.immowelt.org/d8490c94-8bc2-4f38-affe-7986af339d1c/5d00296c-3134-4d05-a29a-760985379123", "https://ms.immowelt.org/862887dd-fca5-4504-a254-d22277945d21/1fdaef5f-474b-4b44-84df-c23fb4960205", "https://ms.immowelt.org/235cb2e7-3834-406d-a4ac-0a1db7702757/b3d2810f-2282-453d-99bf-f70073155c71", "https://ms.immowelt.org/3ae43d7c-7b0d-435e-84bb-7a6ea4aafc03/ae2064f4-8fe0-463b-958f-a7c34e88466a"]</t>
+          <t>["https://ms.immowelt.org/53a40e8a-24fb-45ae-a531-fff2a2f4ef38/73c3faa7-d432-44a3-995c-dd6a57b55ff8", "https://ms.immowelt.org/5fd3d699-98a8-4599-a121-418d851bdca3/552eef5e-2a9f-4c01-b006-8b517f701ec2", "https://ms.immowelt.org/e1c22ef7-fa4f-4bbe-b945-4a0c9417515d/e28a4ad5-ff43-4cdd-a230-41a8a963e3de", "https://ms.immowelt.org/1fe9ddd3-4952-4f94-9aba-7b98e8a565e2/4cc8d480-3a53-414c-ada9-ef0da80900ed", "https://ms.immowelt.org/2e8ae348-cab2-4e79-8266-ee52099c1e73/524bcb38-9f3e-44ef-afa6-8810bc8ec8bf", "https://ms.immowelt.org/b0e64c11-6bbf-4ed6-9eb5-3767349429ee/e3628c5a-5b53-4019-a135-ff500cf7a0ac", "https://ms.immowelt.org/4a8c3d49-12ed-417a-b206-b38a38d9e894/7e1402ca-1074-4126-8ddc-ba9dbe8eac83", "https://ms.immowelt.org/82deeace-1bd0-4723-8a33-2c2ad6084c4a/cabe6e07-e983-4c08-826a-e189aa3d4288", "https://ms.immowelt.org/4e16951a-d91d-485c-a019-726374d3e5d3/97f13c47-29c0-4a36-8ee3-73268762ea32", "https://ms.immowelt.org/f8cc63cd-6dc9-4cc3-8aba-e6dbc1f8c911/bebff58a-a1df-4e6a-868b-ba584b296f85"]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -993,14 +993,14 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Die Einbauk\u00fcche ist schon drin - Sie m\u00fcssen nur noch einziehen! Gehobene 2-Z. Wohnung im Steinbachtal ", "basicObjectPricEur": 1165, "basicLivingSpace": 77, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2aqpt5d", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "3-ZW W\u00fcrzburg  Sanderau,  3. OG.  Bad neu.", "basicObjectPricEur": 950, "basicLivingSpace": 79, "basicRooms": 3, "basicConstructionYear": 1911, "basicCity": "W\u00fcrzburg", "basicStreet": "Eichendorffstrasse 4", "basicUrl": "https://www.immowelt.de/expose/25dtq5g", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2aaj75n"</t>
+          <t>"https://www.immowelt.de/expose/2ajt75p"</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1010,12 +1010,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2"</t>
+          <t>"Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!"</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>532.19</t>
+          <t>474.53</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>56.02</t>
+          <t>49.95</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1045,17 +1045,17 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 17", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1590", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 532.19, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 179, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 110.92, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 882.11, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1420", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 474.53, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 167, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 98.9, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 740.43, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/814cec20-d48a-4483-ae7f-5b779e29c323/404d9d3f-baa2-473d-af13-096d09772807", "https://ms.immowelt.org/60ba3310-b6df-446e-b860-6deb11ef0a09/2558c572-051e-464d-9aad-205683e0f215", "https://ms.immowelt.org/e10fa924-843a-4cd9-897d-8a60a9cd8473/3fd9082b-7a00-4210-99b9-f828a6a2e085", "https://ms.immowelt.org/20e41405-47ae-47ac-97d8-0e7340de1982/b112096a-8211-4248-a5e6-0904121ddac0", "https://ms.immowelt.org/2300c3d0-702d-4867-94fc-810ec8ca8971/f6adb669-5e8c-4182-ad4f-a5b6f477b025", "https://ms.immowelt.org/bdd38a88-61e2-4f96-bac0-895a2e862eed/9b1e1d00-b895-496c-bf47-2912364590ab", "https://ms.immowelt.org/a047e5df-c99a-4420-a028-e84ef22f3786/0dd57565-cb4f-4092-ab20-2a61b660568a"]</t>
+          <t>["https://ms.immowelt.org/059062b5-c451-4105-bfa0-dfb0db8ca29f/0f1cbcbd-e9ed-45e6-96e8-910e278b3044", "https://ms.immowelt.org/ca46e538-90d4-4fa2-8f22-2b6881ac1800/9a457fdc-44b3-4336-b20e-89b86824b294", "https://ms.immowelt.org/a1a88b02-0504-429f-b458-7c1a33126061/b8bc3487-e427-4a1b-b30b-2df51d481f90", "https://ms.immowelt.org/d507b7b4-5e3c-452e-957a-b5636948e585/d2a53e80-0b41-44e4-a681-ce8531a32c32", "https://ms.immowelt.org/ff43f21c-a328-4711-9ce2-41a9bff1bf59/83bd2e55-f9e8-44b1-bf30-e874b0a81423"]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1065,14 +1065,14 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung kann nur mit Wohnberechtigungsschein angemietet werden! 2 Zimmer auf 56 m\u00b2", "basicObjectPricEur": 532.19, "basicLivingSpace": 56.02, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 17", "basicUrl": "https://www.immowelt.de/expose/2aaj75n"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (EOF3) erforderlich!! 2-Zimmer Wohnung mit Dachterrasse!!", "basicObjectPricEur": 474.53, "basicLivingSpace": 49.95, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2ajt75p"}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
+          <t>"https://www.immowelt.de/expose/2a7j75n"</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1082,12 +1082,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
+          <t>"Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon"</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>1181.21</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1097,54 +1097,54 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>70.87</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
+          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3540", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1181.21, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 219, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 169, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1629.21, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
+          <t>["https://ms.immowelt.org/0d9ec1ef-21cc-484a-88ae-193c7267a3bb/1e78105c-6490-4468-a6c3-936b8b388b80", "https://ms.immowelt.org/5c55f670-770f-44e9-b26b-7c9164f4a76a/9f56e225-8915-45d3-9af7-0e36ad2d804e", "https://ms.immowelt.org/12a9fd2a-da00-49a5-9999-efb246a9d727/efc35e4b-a860-47d1-823d-1282d60e0bc6", "https://ms.immowelt.org/bb9a6b97-0d40-46d1-9b24-011a5dcc7508/40526838-218d-4a4c-9422-8bd98023d9f6", "https://ms.immowelt.org/1a701923-58c4-4074-92b3-3e6bc100d51c/2f4849ee-2b95-432d-8ed4-b41b0211a117", "https://ms.immowelt.org/4d6aee50-6e8f-423f-b67a-bd01a011592d/4d58cead-e166-4a77-8c0f-2ee869a9e824"]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon", "basicObjectPricEur": 1181.21, "basicLivingSpace": 70.87, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a7j75n", "basicContactPhone": "+49 931 306 990 20"}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a7j75n"</t>
+          <t>"https://www.immowelt.de/expose/2an6q5g"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1154,12 +1154,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon"</t>
+          <t>"Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1181.21</t>
+          <t>566.96</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>70.87</t>
+          <t>59.68</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1184,39 +1184,39 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Einbauk\u00fcche", "Stellplatz"]</t>
+          <t>["Stellplatz"]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 13", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3540", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 1181.21, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 219, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 169, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1629.21, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1700", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 566.96, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 199, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 124, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 949.96, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/0d9ec1ef-21cc-484a-88ae-193c7267a3bb/1e78105c-6490-4468-a6c3-936b8b388b80", "https://ms.immowelt.org/5c55f670-770f-44e9-b26b-7c9164f4a76a/9f56e225-8915-45d3-9af7-0e36ad2d804e", "https://ms.immowelt.org/12a9fd2a-da00-49a5-9999-efb246a9d727/efc35e4b-a860-47d1-823d-1282d60e0bc6", "https://ms.immowelt.org/bb9a6b97-0d40-46d1-9b24-011a5dcc7508/40526838-218d-4a4c-9422-8bd98023d9f6", "https://ms.immowelt.org/1a701923-58c4-4074-92b3-3e6bc100d51c/2f4849ee-2b95-432d-8ed4-b41b0211a117", "https://ms.immowelt.org/4d6aee50-6e8f-423f-b67a-bd01a011592d/4d58cead-e166-4a77-8c0f-2ee869a9e824"]</t>
+          <t>["https://ms.immowelt.org/04bb8e8f-62a6-4aa1-be23-fcac75a2ca80/64e8eae5-448b-4e0a-aef6-3ee4487d6cad", "https://ms.immowelt.org/07409987-f4b5-4a2f-9ed5-55d000afa646/e6d2fc11-39c9-44c4-9ab7-6b79a5e4667d", "https://ms.immowelt.org/d8d286af-d70c-4388-a156-0e4525e576c2/3f08e4d7-3ff5-4332-b507-dfc163a7d33f", "https://ms.immowelt.org/0eb043d6-e29a-4797-8d47-b95fdf183238/bda6c2c7-7309-497f-836d-6483f70abd43", "https://ms.immowelt.org/4aed45df-9c7d-4a2b-b188-b8968b22727d/50fd789e-2343-4b28-867b-f726db140de4"]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "herr", "firstName": "Stefan", "lastName": "Brogl", "phone": "+49 931 306 990 20"}</t>
+          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnen im herrlichen HUBland: 2Zi, 70m\u00b2, EBK und Balkon", "basicObjectPricEur": 1181.21, "basicLivingSpace": 70.87, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 13", "basicUrl": "https://www.immowelt.de/expose/2a7j75n", "basicContactPhone": "+49 931 306 990 20"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein (WBS3) erforderlich!! Gem\u00fctliche Zweiraumwohnung auf 59m\u00b2", "basicObjectPricEur": 566.96, "basicLivingSpace": 59.68, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2an6q5g"}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
+          <t>"https://www.immowelt.de/expose/2awv45u"</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1226,12 +1226,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
+          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>1720</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1241,47 +1241,47 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>123.36</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>["GAS"]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "Gute Bude Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 3c"}, "salutation": "Frau", "firstName": "Nelly", "lastName": "Gronau"}</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1360,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a8j75n"</t>
+          <t>"https://www.immowelt.de/expose/2at6f5v"</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon"</t>
+          <t>"Wohnung vermieten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>554.99</t>
+          <t>420</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1385,54 +1385,54 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>58.42</t>
+          <t>""</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>""</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>["Personenaufzug", "Stellplatz"]</t>
+          <t>["GAS"]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Frauenland", "ZipCode": "97074", "Street": "Athanasius-Kircher-Stra\u00dfe 15", "LocationId": 496008, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Gromb\u00fchl", "ZipCode": "97080", "LocationId": 496011, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1660", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Frauenland)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-frauenland/mietspiegel"}}, "DataTable": [{"NumberValue": 554.99, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 210, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 208, "Unit": "EUR", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 1032.99, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Gromb\u00fchl)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-grombuehl/mietspiegel"}}, "DataTable": [{"NumberValue": 420, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete", "Comments": ["zzgl. Nebenkosten"]}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 420, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/2c287869-b002-4a19-baea-0433bdc7a327/e15bc071-fe33-4461-8b34-9efe6f7f6e23", "https://ms.immowelt.org/5b165c7f-f365-48c1-841e-a8b1fd2bb6a1/23a21cb8-5f33-4e46-b102-f4960458c3e9", "https://ms.immowelt.org/4b517be9-8d93-492f-ac56-516e6bad3d95/1238a7b6-1272-4e53-9ead-1eafab0548c7", "https://ms.immowelt.org/acdfaf67-7ef9-4ee5-a2e3-416020180ea6/b120a8ca-7b3e-47f0-99b1-006c6eb00277", "https://ms.immowelt.org/540c5813-745e-419c-9217-36ba5261e842/259d75f3-7aca-466d-b4ed-f4b5a08ff770", "https://ms.immowelt.org/9ac46b17-c8c4-446e-8e96-de026ce267b4/f6098bb6-68df-4742-8eda-56e4660c3221", "https://ms.immowelt.org/09537047-f692-4086-b911-c08acb726d74/595eae7d-cd2e-4c30-b4d5-6bf58c421952"]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>{"companyName": "BUWOG Immobilien Treuhand GmbH\u00ad", "address": {"city": "Kiel", "zipCode": "24103", "street": "Fabrikstra\u00dfe 7"}, "salutation": "Herr", "firstName": "Stefan", "lastName": "Brogl"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnberechtigungsschein erforderlich - 2 Zi, 58m\u00b2, Balkon", "basicObjectPricEur": 554.99, "basicLivingSpace": 58.42, "basicRooms": 2, "basicConstructionYear": 2019, "basicCity": "W\u00fcrzburg", "basicStreet": "Athanasius-Kircher-Stra\u00dfe 15", "basicUrl": "https://www.immowelt.de/expose/2a8j75n"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Wohnung vermieten in W\u00fcrzburg", "basicObjectPricEur": 420, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2at6f5v", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2awv45u"</t>
+          <t>"https://www.immowelt.de/expose/2afyn5t"</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1442,12 +1442,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld"</t>
+          <t>"2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg"</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1720</t>
+          <t>750</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1457,54 +1457,54 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>123.36</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>1960</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "Personenaufzug", "FERNE", "GAS", "Fu\u00dfbodenheizung", "Zentralheizung", "rollstuhlgerecht", "PARKETT", "frei", "Einbauk\u00fcche", "offene K\u00fcche", "Speisekammer", "Stellplatz", "Tiefgarage", "REINIGUNG", "Balkon", "Terrasse"]</t>
+          <t>["Altbau (bis 1945)", "WANNE", "Kelleranteil", "renoviert", "GAS", "Zentralheizung", "Einbauk\u00fcche"]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Heidingsfeld", "ZipCode": "97084", "LocationId": 496013, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Zellerau", "ZipCode": "97082", "LocationId": 496026, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "5160", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Heidingsfeld)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-heidingsfeld/mietspiegel"}}, "DataTable": [{"NumberValue": 1720, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 320, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 2040, "Unit": "EUR"}, {"NumberValue": 70, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "2 Stellpl\u00e4tze, je"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2000", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Zellerau)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-zellerau/mietspiegel"}}, "DataTable": [{"NumberValue": 750, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 200, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 950, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/70edfd50-f060-4619-8d8e-0a42b4111160/271e31b7-8484-45a8-8ac9-904dabf13c7b", "https://ms.immowelt.org/efa2a84b-bb24-4421-ae15-0649647fc5f0/8490cb37-3682-446f-8b11-e9e1da37cba9", "https://ms.immowelt.org/1683eefc-9ca0-4cbc-992f-8e3a9b044b29/7df67d66-b166-4c09-b89c-52d2409839a6", "https://ms.immowelt.org/80c22a83-a553-4a11-b6d3-845ab5aee5fa/a5ed848d-87ec-43a7-91b1-3a82889e2f11", "https://ms.immowelt.org/912ad1a7-5c04-49c1-bfdb-52dfd32f4078/087254f6-99be-4f33-ad19-a0d31350b6df", "https://ms.immowelt.org/c04aac07-656d-484f-97c8-f9183167c740/27c413f7-27b3-4874-9d22-7b3ce7fb1772", "https://ms.immowelt.org/6355ac0c-0919-41d1-9939-c7327ad98472/b5a33c7f-e707-4bd6-839a-ea939f810d7c", "https://ms.immowelt.org/e86eec55-1463-4303-8c06-6e1cd90ac14e/01d5e414-8279-49e7-ac42-160f28ed6a9b", "https://ms.immowelt.org/f6c4b53e-148d-44ad-b8fb-50e2e7c095c6/9403fef4-e110-4d99-88ec-08c732282eda", "https://ms.immowelt.org/bb63f6b4-e5b8-4f84-b1e9-c19308a3d41f/20e645fd-f306-449c-82ae-d3591730cca2", "https://ms.immowelt.org/6eff25e1-ca40-4fdc-b6f2-adcf3b4d0a45/63b7a19b-f618-4933-adb0-f0cd5e1263a5", "https://ms.immowelt.org/2811d6e1-5985-40bf-a07a-594fdaf52254/4a7a045f-966f-4645-86ce-900f6e22d446", "https://ms.immowelt.org/aefa4aed-f85d-4406-ae1b-9c233616a69e/fd830bae-b6de-4525-8e19-1c72c8249092", "https://ms.immowelt.org/c0855678-63ef-4feb-a503-a8d0adf77171/3851bcbc-db22-481c-b205-d0b9fb09017f", "https://ms.immowelt.org/df7e819e-aa27-4bbf-b743-a9e2712de66b/0737cd62-424e-4825-afba-0a294eb938ec", "https://ms.immowelt.org/f47e219f-f548-45dd-a07d-bb94c2b60e97/cfc0cf18-e610-4657-b7ed-3ca18984267a"]</t>
+          <t>["https://ms.immowelt.org/7392265b-7589-4e96-8719-b289bb8ace01/19ed71d6-701a-4bbe-929c-a35f0d2ec94b", "https://ms.immowelt.org/15baddee-aaf7-4f0a-b016-7f47a07c4e37/48316143-5143-447a-8c57-f0b7e929d6fe", "https://ms.immowelt.org/027c0258-c7df-4398-b7bc-fce818803786/c5879894-c70e-4d36-87c5-2f3d1391a860", "https://ms.immowelt.org/512f5ff2-4810-463d-be09-2b1645c65d7d/c20634e3-424e-4fa7-adc1-7bb96e05a731", "https://ms.immowelt.org/0bc625b6-c3c3-4417-81a8-a0c000046701/97c3d523-e7c6-4b79-af4f-d9928909527c", "https://ms.immowelt.org/76a5fc74-de02-4ae9-aec8-48e4168cea64/423affd6-d43f-46c2-9187-ca30a02614d6", "https://ms.immowelt.org/39f67b57-3390-44ea-ab71-3cbb1b166a73/03cd65f9-4b01-46f7-832d-c4ec60e69999", "https://ms.immowelt.org/4aa9aeb4-7027-43a0-85f3-887e51080c31/b7c1b3ae-576c-44d3-a98d-260591a7c97b"]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>{"companyName": "Gute Bude Immobilien", "address": {"city": "W\u00fcrzburg", "zipCode": "97082", "street": "Zeller Str. 3c"}, "salutation": "Frau", "firstName": "Nelly", "lastName": "Gronau"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Luxuri\u00f6se Penthouse-Wohnung Erstbezug! 3-Zimmer-Neubau in W\u00fcrzburg-Heidingfeld", "basicObjectPricEur": 1720, "basicLivingSpace": 123.36, "basicRooms": 3, "basicConstructionYear": 2022, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2awv45u"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "2,5 Zimmer Wohnung beim Japanischen Garten in W\u00fcrzburg", "basicObjectPricEur": 750, "basicLivingSpace": 65, "basicRooms": 2.5, "basicConstructionYear": 1960, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2afyn5t", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2upu84s"</t>
+          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1514,12 +1514,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
+          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>2880</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1529,37 +1529,37 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>195</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
+          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
+          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1569,14 +1569,14 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2agbf5s"</t>
+          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>"Traumwohnung in Top Lage mit toller Weitsicht!"</t>
+          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2880</t>
+          <t>580</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1601,54 +1601,54 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>195</t>
+          <t>44</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>null</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>["Neubau", "barriefrei", "WANNE", "gaestewc", "FENSTER", "Kelleranteil", "LUFTWP", "Garten", "gartennutzung", "rollstuhlgerecht", "Balkon", "Terrasse"]</t>
+          <t>["WANNE"]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "Gerbrunn", "ZipCode": "97218", "Street": "Helene Wessel Weg 5", "LocationId": 12047, "PublishStreet": true, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "3 Kaltmieten", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in Gerbrunn", "Link": "https://www.immowelt.de/immobilienpreise/gerbrunn/mietspiegel"}}, "DataTable": [{"NumberValue": 2880, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 400, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Nebenkosten enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}, {"Key": "PRICE_RENT_WARM", "Label": "Warmmiete", "NumberValue": 3280, "Unit": "EUR"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/17e5aca9-793d-40b3-aab5-a5dcea349a87/0d9236ef-f790-4bac-82dc-9a229cfe4527", "https://ms.immowelt.org/cf96b674-5a06-4156-b363-d3e23b5dfe92/c12ffbff-3538-4b01-a604-ee0869a952b6", "https://ms.immowelt.org/2755511b-7b13-42f8-bad0-3d769da9305b/b3d17421-aa79-4be1-83cb-ae6fe7955297", "https://ms.immowelt.org/17109eb9-b8cf-435e-b0b9-8377b8a7c9f4/986295b9-a109-4924-b6b8-fc375860cd30", "https://ms.immowelt.org/d4384af4-fbdc-4807-9ab2-e4c02ad5e5b9/61dd1708-3529-4a40-9890-401b9917edfc", "https://ms.immowelt.org/efa4e805-be82-4e38-998b-46485660f4e5/fbb8ea8f-2b17-45b1-8691-eb2fe09dd0a7"]</t>
+          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>""</t>
+          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Traumwohnung in Top Lage mit toller Weitsicht!", "basicObjectPricEur": 2880, "basicLivingSpace": 195, "basicRooms": 6, "basicConstructionYear": 2023, "basicCity": "Gerbrunn", "basicStreet": "Helene Wessel Weg 5", "basicUrl": "https://www.immowelt.de/expose/2agbf5s", "basicContactPhone": "", "basicContactMobile": ""}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>"https://www.immowelt.de/expose/2a2yn5v"</t>
+          <t>"https://www.immowelt.de/expose/2upu84s"</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1658,12 +1658,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland"</t>
+          <t>"Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>900</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1673,12 +1673,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>90</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1688,32 +1688,32 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>["WANNE"]</t>
+          <t>["WANNE", "FENSTER", "Kelleranteil", "ELEKTRO", "Garten", "gartennutzung", "Balkon", "Terrasse"]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>{"Country": "Deutschland", "City": "W\u00fcrzburg", "District": "Altstadt", "ZipCode": "97072", "LocationId": 496004, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
+          <t>{"Country": "Deutschland", "City": "K\u00fcrnach", "ZipCode": "97273", "LocationId": 12666, "PublishStreet": false, "FederalState": "Bayern", "FederalStateId": 2}</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "1.080,00 ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in W\u00fcrzburg (Altstadt)", "Link": "https://www.immowelt.de/immobilienpreise/wuerzburg-altstadt/mietspiegel"}}, "DataTable": [{"NumberValue": 580, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 120, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"StringValue": "in Warmmiete enthalten", "Key": "PRICE_HEATINGCOSTS", "Label": "Heizkosten"}]}</t>
+          <t>{"AdditionalInformation": {"Deposit": {"StringValue": "2 Kaltmieten ", "Key": "PRICE_DEPOSIT", "Label": "Kaution"}, "MarketPricing": {"Heading": "Mietspiegel in K\u00fcrnach", "Link": "https://www.immowelt.de/immobilienpreise/kuernach/mietspiegel"}}, "DataTable": [{"NumberValue": 900, "Unit": "EUR", "Key": "PRICE_RENT_COLD", "Label": "Kaltmiete"}, {"NumberValue": 80, "Unit": "EUR", "Key": "PRICE_ADDITIONALCOSTS", "Label": "Nebenkosten"}, {"NumberValue": 50, "Unit": "EUR", "Key": "PRICE_PARKINGPRICE", "Label": "1 Stellplatz"}]}</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>["https://ms.immowelt.org/67968400-d13b-449c-8f0f-1f8dc3645f4c/4d6bfee6-a4bb-438e-a524-96840bd51ae1", "https://ms.immowelt.org/c3319402-5904-4d76-95d2-db5b70bee409/4e68c2f5-c18e-4b63-bc8f-0ee1c1309ebf", "https://ms.immowelt.org/2dd83638-fb99-4566-ba6f-cf7b62d7c4bb/6ceb0ef0-07a4-468f-8f2a-f2e6741a577f", "https://ms.immowelt.org/1609ec66-fe8f-4f74-b4d5-02421f7513b0/a1757c96-7393-44bc-bf2e-6c9466ce4f45", "https://ms.immowelt.org/35e2e29e-1627-4973-99d4-4c3b1facdc4e/b477018c-9c03-4c1b-861c-11a14bcff4e8", "https://ms.immowelt.org/48e33aa4-fbdd-48d1-ac41-d25502baa7d5/14df5c1a-b256-4cd0-a73b-72d4dd9a2961"]</t>
+          <t>["https://ms.immowelt.org/11008e51-5945-4ab3-a0eb-f2a703785b20/53fa6be7-ade6-4395-81ca-d66b9bbb1ba9", "https://ms.immowelt.org/64bc93db-da55-44ca-a2c8-c14f8ce86353/14ba8183-9d5b-4c81-a957-284d595a032f", "https://ms.immowelt.org/87e6208f-ee9e-4d96-a62a-6561d184b0e3/572c15dc-ed2e-4296-bc44-96a28e7cf135", "https://ms.immowelt.org/ba824adc-5910-4328-b432-ac6c69a928b3/dc0e3963-adad-4942-ad9a-dc0fc1b71796", "https://ms.immowelt.org/cee10f88-e7a3-499e-be76-626c1d42e77d/c1805001-8c80-4257-977c-80d06c2cbbc7", "https://ms.immowelt.org/aba27baa-44fb-49d2-833b-ffe9285cf719/2f9875be-ad3f-435e-bf3a-d7d63a5e8a17", "https://ms.immowelt.org/b63c1740-9745-464b-8364-2df590a1d676/f71392e8-2cac-4fad-aeaf-0379e7187348", "https://ms.immowelt.org/0b219ac9-8c45-4c18-9228-d206e9ff703e/4bce456f-aecf-48fa-a4a2-b0b332e7badc", "https://ms.immowelt.org/711ca5fb-12d7-42dc-a1f6-32893287c0eb/4002136b-ce99-43ba-8406-dee393492ff0", "https://ms.immowelt.org/17453203-a015-4bcc-816b-12fe9fe761ee/3c33ba0b-8a93-4d03-b3c7-0267e690bc76", "https://ms.immowelt.org/f09d3348-84eb-4a67-941e-68eee061b36d/75a81b43-153a-44e2-8336-9f323ccdad5a", "https://ms.immowelt.org/79e28d05-fb4a-4b73-ad94-cd78318ef65b/0441105e-ad78-4d19-86b1-dab1c3c87ee1", "https://ms.immowelt.org/07c2164c-067e-490d-b769-760ef64271e2/2e82cebf-00da-4337-83e8-6186da964d0d", "https://ms.immowelt.org/de5a7379-e440-43c4-8670-4bdd1e8bdca0/e80fa6cc-bbb1-48ab-b091-2b052e63948b", "https://ms.immowelt.org/9cc41d7e-f16c-4d38-ae23-e1f15da29cfc/e1740437-8eb5-4984-bba2-1c1036d06b98"]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>{"companyName": "Viefhaus Immobilien Inh. Sebastian Viefhaus", "address": {"city": "W\u00fcrzburg", "zipCode": "97074", "street": "Fichtestra\u00dfe 10"}, "salutation": "Herr", "firstName": "Thomas", "lastName": "Meister", "phone": "0931-88065061"}</t>
+          <t>""</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>{"basicTranactionType": "RENT", "basicTitle": "Optimal f\u00fcr Studenten-WG : 2-Zimmerwohnung in zentraler Lage im Frauenland", "basicObjectPricEur": 580, "basicLivingSpace": 44, "basicRooms": 2, "basicConstructionYear": null, "basicCity": "W\u00fcrzburg", "basicUrl": "https://www.immowelt.de/expose/2a2yn5v", "basicContactPhone": "0931-88065061"}</t>
+          <t>{"basicTranactionType": "RENT", "basicTitle": "Gro\u00dfe 3-Zimmer-Wohnung mit eigenem Garten und Balkon in K\u00fcrnach", "basicObjectPricEur": 900, "basicLivingSpace": 90, "basicRooms": 3, "basicConstructionYear": null, "basicCity": "K\u00fcrnach", "basicUrl": "https://www.immowelt.de/expose/2upu84s", "basicContactPhone": "", "basicContactMobile": ""}</t>
         </is>
       </c>
     </row>

</xml_diff>